<commit_message>
Edit Menu & Form
</commit_message>
<xml_diff>
--- a/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
+++ b/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project_PBMT\PBMT_TAAWUN_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\PBMT_TAAWUN\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
-    <sheet name="DATABASE" sheetId="5" r:id="rId1"/>
-    <sheet name="Menu Transaksi" sheetId="8" r:id="rId2"/>
-    <sheet name="Menu Informasi" sheetId="9" r:id="rId3"/>
-    <sheet name="Menu Properti" sheetId="11" r:id="rId4"/>
-    <sheet name="Menu Cetak" sheetId="10" r:id="rId5"/>
-    <sheet name="Menu Administrasi" sheetId="12" r:id="rId6"/>
+    <sheet name="COA" sheetId="13" r:id="rId1"/>
+    <sheet name="DATABASE" sheetId="5" r:id="rId2"/>
+    <sheet name="Menu Transaksi" sheetId="8" r:id="rId3"/>
+    <sheet name="Menu Informasi" sheetId="9" r:id="rId4"/>
+    <sheet name="Menu Properti" sheetId="11" r:id="rId5"/>
+    <sheet name="Menu Cetak" sheetId="10" r:id="rId6"/>
+    <sheet name="Menu Administrasi" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="189">
   <si>
     <t>REKENING</t>
   </si>
@@ -372,6 +373,225 @@
   </si>
   <si>
     <t>Tabel Rekening</t>
+  </si>
+  <si>
+    <t>CHART OF ACCOUNT</t>
+  </si>
+  <si>
+    <t>DAFTAR AKUN BUKU BESAR</t>
+  </si>
+  <si>
+    <t>Kas Besar</t>
+  </si>
+  <si>
+    <t>Pendapatan Taawun Jiwa</t>
+  </si>
+  <si>
+    <t>Kas Kecil Cashier</t>
+  </si>
+  <si>
+    <t>Pendapatan Taawun Kebakaran</t>
+  </si>
+  <si>
+    <t>Bank BNIS 01</t>
+  </si>
+  <si>
+    <t>Pendapatan Bagihasil Bank</t>
+  </si>
+  <si>
+    <t>Bank BNIS 02</t>
+  </si>
+  <si>
+    <t>Pendapatan Hasil Investasi</t>
+  </si>
+  <si>
+    <t>Bank BSM</t>
+  </si>
+  <si>
+    <t>Pendapatan Lain</t>
+  </si>
+  <si>
+    <t>Bank Cek &amp; BG</t>
+  </si>
+  <si>
+    <t>PPAP - Kopersai / Bank</t>
+  </si>
+  <si>
+    <t>Penempatan Deposito 01</t>
+  </si>
+  <si>
+    <t>Penempatan Deposito 02</t>
+  </si>
+  <si>
+    <t>PPAP - Penempatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDSB - Saham </t>
+  </si>
+  <si>
+    <t xml:space="preserve">IDSB - Obligasi </t>
+  </si>
+  <si>
+    <t>Biaya Adm Bank</t>
+  </si>
+  <si>
+    <t>PPAP - IDSB</t>
+  </si>
+  <si>
+    <t>Biaya Prosesi Santunan</t>
+  </si>
+  <si>
+    <t>Piutang IURAN</t>
+  </si>
+  <si>
+    <t>Biaya Adm Kantor</t>
+  </si>
+  <si>
+    <t>Piutang SANTUNAN</t>
+  </si>
+  <si>
+    <t>Biaya Listrik Air Telpon</t>
+  </si>
+  <si>
+    <t>PPAP-Piutang</t>
+  </si>
+  <si>
+    <t>Biaya Transportasi</t>
+  </si>
+  <si>
+    <t>Pembiayaan</t>
+  </si>
+  <si>
+    <t>Biaya Perjalanan Dinas</t>
+  </si>
+  <si>
+    <t>Persediaan Untuk dijual</t>
+  </si>
+  <si>
+    <t>Biaya Rapat</t>
+  </si>
+  <si>
+    <t>Persd Barang Cetakan</t>
+  </si>
+  <si>
+    <t>Biaya Sewa</t>
+  </si>
+  <si>
+    <t>Persd Alat Tulis Kantor</t>
+  </si>
+  <si>
+    <t>Biaya Perawatan dan Perbaikan</t>
+  </si>
+  <si>
+    <t>Persd Barang Promosi</t>
+  </si>
+  <si>
+    <t>Biaya Sosial</t>
+  </si>
+  <si>
+    <t>Persd Peralatan/Suplies</t>
+  </si>
+  <si>
+    <t>Biaya Personalia Gaji Pokok</t>
+  </si>
+  <si>
+    <t>Persd Lain</t>
+  </si>
+  <si>
+    <t>Biaya Personalia Tunjangan</t>
+  </si>
+  <si>
+    <t>Penyertaan Saham Ventura</t>
+  </si>
+  <si>
+    <t>Biaya Marketing</t>
+  </si>
+  <si>
+    <t>Penyertaan pada Koperasi</t>
+  </si>
+  <si>
+    <t>Biaya Pendidikan</t>
+  </si>
+  <si>
+    <t>PPAP-Penyertaan</t>
+  </si>
+  <si>
+    <t>Biaya PPAP, Penghapusan</t>
+  </si>
+  <si>
+    <t>BDD Kewajiban</t>
+  </si>
+  <si>
+    <t>Biaya Amortisasi</t>
+  </si>
+  <si>
+    <t>BDD Sewa</t>
+  </si>
+  <si>
+    <t>Biaya Penyusutan A.T.</t>
+  </si>
+  <si>
+    <t>Amortisasi BDD</t>
+  </si>
+  <si>
+    <t>Biaya Operasional Lain</t>
+  </si>
+  <si>
+    <t>At Aktiva Tetap</t>
+  </si>
+  <si>
+    <t>Biaya Non Operasional</t>
+  </si>
+  <si>
+    <t>At Penyusutan Ak.Tetap</t>
+  </si>
+  <si>
+    <t>Zakat</t>
+  </si>
+  <si>
+    <t>Rupa-rupa Aktiva</t>
+  </si>
+  <si>
+    <t>Infaq, Shodaqoh, Wakaf</t>
+  </si>
+  <si>
+    <t>Sosial dan Lingkungan</t>
+  </si>
+  <si>
+    <t>Biaya Pajak</t>
+  </si>
+  <si>
+    <t>Kewajiban segera Biaya</t>
+  </si>
+  <si>
+    <t>Kewajiban segera Titipan</t>
+  </si>
+  <si>
+    <t>Hutang Santunan</t>
+  </si>
+  <si>
+    <t>Hutang Iuran</t>
+  </si>
+  <si>
+    <t>Hutang Lain</t>
+  </si>
+  <si>
+    <t>Pembiayaan yang Diterima</t>
+  </si>
+  <si>
+    <t>Rupa Rupa Pasiva</t>
+  </si>
+  <si>
+    <t>Dana Taawun Jiwa</t>
+  </si>
+  <si>
+    <t>Dana Taawun Kebakaran</t>
+  </si>
+  <si>
+    <t>Modal</t>
+  </si>
+  <si>
+    <t>Cadangan</t>
   </si>
 </sst>
 </file>
@@ -381,7 +601,7 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -463,6 +683,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -531,7 +759,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -788,6 +1016,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -796,7 +1048,7 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -957,21 +1209,68 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -984,39 +1283,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1026,17 +1292,27 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -2041,6 +2317,1011 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:I79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="35.28515625" customWidth="1"/>
+    <col min="4" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="30.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="103" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B4" s="104" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="74"/>
+      <c r="F6" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="78" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="79"/>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="105">
+        <v>110001</v>
+      </c>
+      <c r="C8" s="106" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="107"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="105">
+        <v>650001</v>
+      </c>
+      <c r="G8" s="106" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="107"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="105">
+        <v>110002</v>
+      </c>
+      <c r="C9" s="106" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="107"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="105">
+        <v>650002</v>
+      </c>
+      <c r="G9" s="106" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="107"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="105">
+        <v>111001</v>
+      </c>
+      <c r="C10" s="106" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="107"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="105">
+        <v>651001</v>
+      </c>
+      <c r="G10" s="106" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="107"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="105">
+        <v>111002</v>
+      </c>
+      <c r="C11" s="106" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="107"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="105">
+        <v>651002</v>
+      </c>
+      <c r="G11" s="106" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="107"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="105">
+        <v>111003</v>
+      </c>
+      <c r="C12" s="106" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="107"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="105">
+        <v>652001</v>
+      </c>
+      <c r="G12" s="106" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12" s="30"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="105">
+        <v>111888</v>
+      </c>
+      <c r="C13" s="106" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="107"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="107"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="105">
+        <v>111999</v>
+      </c>
+      <c r="C14" s="106" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" s="107"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="105">
+        <v>112001</v>
+      </c>
+      <c r="C15" s="106" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" s="107"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="105">
+        <v>112002</v>
+      </c>
+      <c r="C16" s="106" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="107"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="108"/>
+      <c r="G16" s="109"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="105">
+        <v>112999</v>
+      </c>
+      <c r="C17" s="106" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="107"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="110" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="110" t="s">
+        <v>38</v>
+      </c>
+      <c r="H17" s="110" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="105">
+        <v>113001</v>
+      </c>
+      <c r="C18" s="106" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="107"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="105">
+        <v>113002</v>
+      </c>
+      <c r="C19" s="106" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="107"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="105">
+        <v>770001</v>
+      </c>
+      <c r="G19" s="106" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="105">
+        <v>113999</v>
+      </c>
+      <c r="C20" s="106" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="30"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="105">
+        <v>771001</v>
+      </c>
+      <c r="G20" s="106" t="s">
+        <v>137</v>
+      </c>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="105">
+        <v>114001</v>
+      </c>
+      <c r="C21" s="106" t="s">
+        <v>138</v>
+      </c>
+      <c r="D21" s="30"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="105">
+        <v>772001</v>
+      </c>
+      <c r="G21" s="106" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21" s="107"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="105">
+        <v>114002</v>
+      </c>
+      <c r="C22" s="106" t="s">
+        <v>140</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="105">
+        <v>772002</v>
+      </c>
+      <c r="G22" s="106" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="107"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="105">
+        <v>114999</v>
+      </c>
+      <c r="C23" s="106" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="30"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="105">
+        <v>772003</v>
+      </c>
+      <c r="G23" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" s="107"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="105">
+        <v>115001</v>
+      </c>
+      <c r="C24" s="106" t="s">
+        <v>144</v>
+      </c>
+      <c r="D24" s="30"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="105">
+        <v>772004</v>
+      </c>
+      <c r="G24" s="106" t="s">
+        <v>145</v>
+      </c>
+      <c r="H24" s="107"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="105">
+        <v>116001</v>
+      </c>
+      <c r="C25" s="106" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="105">
+        <v>772005</v>
+      </c>
+      <c r="G25" s="106" t="s">
+        <v>147</v>
+      </c>
+      <c r="H25" s="107"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="105">
+        <v>117001</v>
+      </c>
+      <c r="C26" s="106" t="s">
+        <v>148</v>
+      </c>
+      <c r="D26" s="30"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="105">
+        <v>773001</v>
+      </c>
+      <c r="G26" s="106" t="s">
+        <v>149</v>
+      </c>
+      <c r="H26" s="107"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="105">
+        <v>117002</v>
+      </c>
+      <c r="C27" s="106" t="s">
+        <v>150</v>
+      </c>
+      <c r="D27" s="30"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="105">
+        <v>773001</v>
+      </c>
+      <c r="G27" s="106" t="s">
+        <v>151</v>
+      </c>
+      <c r="H27" s="107"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="105">
+        <v>117003</v>
+      </c>
+      <c r="C28" s="106" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" s="30"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="105">
+        <v>774008</v>
+      </c>
+      <c r="G28" s="106" t="s">
+        <v>153</v>
+      </c>
+      <c r="H28" s="107"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="105">
+        <v>117004</v>
+      </c>
+      <c r="C29" s="106" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="30"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="105">
+        <v>775001</v>
+      </c>
+      <c r="G29" s="106" t="s">
+        <v>155</v>
+      </c>
+      <c r="H29" s="107"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="105">
+        <v>117888</v>
+      </c>
+      <c r="C30" s="106" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="30"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="105">
+        <v>775002</v>
+      </c>
+      <c r="G30" s="106" t="s">
+        <v>157</v>
+      </c>
+      <c r="H30" s="107"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="105">
+        <v>118001</v>
+      </c>
+      <c r="C31" s="106" t="s">
+        <v>158</v>
+      </c>
+      <c r="D31" s="30"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="105">
+        <v>776001</v>
+      </c>
+      <c r="G31" s="106" t="s">
+        <v>159</v>
+      </c>
+      <c r="H31" s="107"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="105">
+        <v>118002</v>
+      </c>
+      <c r="C32" s="106" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="30"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="105">
+        <v>777001</v>
+      </c>
+      <c r="G32" s="106" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="107"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="105">
+        <v>118999</v>
+      </c>
+      <c r="C33" s="106" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="30"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="105">
+        <v>778001</v>
+      </c>
+      <c r="G33" s="106" t="s">
+        <v>163</v>
+      </c>
+      <c r="H33" s="107"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B34" s="105">
+        <v>119001</v>
+      </c>
+      <c r="C34" s="106" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="30"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="105">
+        <v>778002</v>
+      </c>
+      <c r="G34" s="106" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="107"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B35" s="105">
+        <v>119002</v>
+      </c>
+      <c r="C35" s="106" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="30"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="105">
+        <v>778003</v>
+      </c>
+      <c r="G35" s="106" t="s">
+        <v>167</v>
+      </c>
+      <c r="H35" s="107"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="105">
+        <v>119999</v>
+      </c>
+      <c r="C36" s="106" t="s">
+        <v>168</v>
+      </c>
+      <c r="D36" s="30"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="105">
+        <v>779888</v>
+      </c>
+      <c r="G36" s="106" t="s">
+        <v>169</v>
+      </c>
+      <c r="H36" s="107"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="105">
+        <v>120001</v>
+      </c>
+      <c r="C37" s="106" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="30"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="105">
+        <v>780001</v>
+      </c>
+      <c r="G37" s="106" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="107"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="105">
+        <v>120999</v>
+      </c>
+      <c r="C38" s="106" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" s="30"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="105">
+        <v>781001</v>
+      </c>
+      <c r="G38" s="106" t="s">
+        <v>173</v>
+      </c>
+      <c r="H38" s="107"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="105">
+        <v>122001</v>
+      </c>
+      <c r="C39" s="106" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" s="30"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="105">
+        <v>781002</v>
+      </c>
+      <c r="G39" s="106" t="s">
+        <v>175</v>
+      </c>
+      <c r="H39" s="107"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="105">
+        <v>781003</v>
+      </c>
+      <c r="G40" s="106" t="s">
+        <v>176</v>
+      </c>
+      <c r="H40" s="107"/>
+    </row>
+    <row r="41" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="105">
+        <v>783001</v>
+      </c>
+      <c r="G41" s="106" t="s">
+        <v>177</v>
+      </c>
+      <c r="H41" s="30"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="78" t="s">
+        <v>37</v>
+      </c>
+      <c r="C42" s="78" t="s">
+        <v>38</v>
+      </c>
+      <c r="D42" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="E42" s="111"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="109"/>
+      <c r="H42" s="4"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="95"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
+      <c r="E43" s="111"/>
+      <c r="F43" s="108"/>
+      <c r="G43" s="109"/>
+      <c r="H43" s="4"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="105">
+        <v>210001</v>
+      </c>
+      <c r="C44" s="106" t="s">
+        <v>178</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="108"/>
+      <c r="G44" s="109"/>
+      <c r="H44" s="4"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="105">
+        <v>210002</v>
+      </c>
+      <c r="C45" s="106" t="s">
+        <v>179</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="109"/>
+      <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="105">
+        <v>211001</v>
+      </c>
+      <c r="C46" s="106" t="s">
+        <v>180</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="109"/>
+      <c r="H46" s="4"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="105">
+        <v>211002</v>
+      </c>
+      <c r="C47" s="106" t="s">
+        <v>181</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="108"/>
+      <c r="G47" s="109"/>
+      <c r="H47" s="4"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="105">
+        <v>211003</v>
+      </c>
+      <c r="C48" s="106" t="s">
+        <v>182</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="108"/>
+      <c r="G48" s="109"/>
+      <c r="H48" s="4"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="105">
+        <v>212001</v>
+      </c>
+      <c r="C49" s="106" t="s">
+        <v>183</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="108"/>
+      <c r="G49" s="109"/>
+      <c r="H49" s="4"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="105">
+        <v>219001</v>
+      </c>
+      <c r="C50" s="106" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="108"/>
+      <c r="G50" s="109"/>
+      <c r="H50" s="4"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" s="105">
+        <v>220001</v>
+      </c>
+      <c r="C51" s="106" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="108"/>
+      <c r="G51" s="109"/>
+      <c r="H51" s="4"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="105">
+        <v>220002</v>
+      </c>
+      <c r="C52" s="106" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="109"/>
+      <c r="H52" s="4"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B53" s="105">
+        <v>230001</v>
+      </c>
+      <c r="C53" s="106" t="s">
+        <v>187</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="108"/>
+      <c r="G53" s="109"/>
+      <c r="H53" s="4"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="105">
+        <v>230001</v>
+      </c>
+      <c r="C54" s="106" t="s">
+        <v>188</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="108"/>
+      <c r="G54" s="109"/>
+      <c r="H54" s="4"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" s="108"/>
+      <c r="C55" s="109"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="108"/>
+      <c r="G55" s="109"/>
+      <c r="H55" s="4"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="108"/>
+      <c r="C56" s="109"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="108"/>
+      <c r="G56" s="109"/>
+      <c r="H56" s="4"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="108"/>
+      <c r="C57" s="109"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="108"/>
+      <c r="G57" s="109"/>
+      <c r="H57" s="4"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="108"/>
+      <c r="C58" s="109"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="108"/>
+      <c r="C59" s="109"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="108"/>
+      <c r="C60" s="109"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="108"/>
+      <c r="C61" s="109"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="108"/>
+      <c r="C62" s="109"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="108"/>
+      <c r="C63" s="109"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+    </row>
+    <row r="65" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B65" s="4"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+    </row>
+    <row r="69" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+    </row>
+    <row r="70" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+    </row>
+    <row r="71" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B71" s="4"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
+    </row>
+    <row r="72" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B72" s="108"/>
+      <c r="C72" s="109"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
+    </row>
+    <row r="73" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B73" s="108"/>
+      <c r="C73" s="109"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
+    </row>
+    <row r="74" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B74" s="108"/>
+      <c r="C74" s="109"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+    </row>
+    <row r="75" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B75" s="108"/>
+      <c r="C75" s="109"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+    </row>
+    <row r="76" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B76" s="108"/>
+      <c r="C76" s="109"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+    </row>
+    <row r="77" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
+    </row>
+    <row r="78" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B78" s="4"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B79" s="4"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:S66"/>
   <sheetViews>
     <sheetView topLeftCell="F13" zoomScaleNormal="100" workbookViewId="0">
@@ -2103,48 +3384,48 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="84" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="97" t="s">
+      <c r="F8" s="89" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="75" t="s">
+      <c r="G8" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="75" t="s">
+      <c r="I8" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="75" t="s">
+      <c r="J8" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="75" t="s">
+      <c r="K8" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="89"/>
+      <c r="L8" s="88"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="88"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="89"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="90"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="88"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
@@ -2158,7 +3439,7 @@
       <c r="E10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F10" s="99" t="s">
+      <c r="F10" s="75" t="s">
         <v>96</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -2184,7 +3465,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="100"/>
+      <c r="F11" s="76"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="10"/>
@@ -2198,7 +3479,7 @@
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="101"/>
+      <c r="F12" s="77"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="67"/>
@@ -2219,50 +3500,50 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="75" t="s">
+      <c r="E15" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="75" t="s">
+      <c r="F15" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="75" t="s">
+      <c r="G15" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="75" t="s">
+      <c r="H15" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="77" t="s">
+      <c r="I15" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="90" t="s">
+      <c r="J15" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="89"/>
-      <c r="N15" s="89"/>
-      <c r="O15" s="89"/>
+      <c r="K15" s="88"/>
+      <c r="L15" s="88"/>
+      <c r="M15" s="88"/>
+      <c r="N15" s="88"/>
+      <c r="O15" s="88"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="88"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="89"/>
-      <c r="N16" s="89"/>
-      <c r="O16" s="89"/>
+      <c r="C16" s="85"/>
+      <c r="D16" s="79"/>
+      <c r="E16" s="79"/>
+      <c r="F16" s="79"/>
+      <c r="G16" s="79"/>
+      <c r="H16" s="79"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="87"/>
+      <c r="K16" s="88"/>
+      <c r="L16" s="88"/>
+      <c r="M16" s="88"/>
+      <c r="N16" s="88"/>
+      <c r="O16" s="88"/>
     </row>
     <row r="17" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="50" t="s">
@@ -2346,76 +3627,76 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="87" t="s">
+      <c r="D22" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="75" t="s">
+      <c r="E22" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="75" t="s">
+      <c r="F22" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="75" t="s">
+      <c r="G22" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="75" t="s">
+      <c r="H22" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="75" t="s">
+      <c r="I22" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="77" t="s">
+      <c r="J22" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="90" t="s">
+      <c r="K22" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="75" t="s">
+      <c r="L22" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="75" t="s">
+      <c r="M22" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="77" t="s">
+      <c r="N22" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="77" t="s">
+      <c r="O22" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="75" t="s">
+      <c r="P22" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="77" t="s">
+      <c r="Q22" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="R22" s="77" t="s">
+      <c r="R22" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="75" t="s">
+      <c r="S22" s="78" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="86"/>
-      <c r="D23" s="88"/>
-      <c r="E23" s="86"/>
-      <c r="F23" s="86"/>
-      <c r="G23" s="86"/>
-      <c r="H23" s="86"/>
-      <c r="I23" s="86"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="91"/>
-      <c r="L23" s="86"/>
-      <c r="M23" s="86"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="86"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="86"/>
+      <c r="C23" s="79"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="81"/>
+      <c r="K23" s="87"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="81"/>
+      <c r="O23" s="81"/>
+      <c r="P23" s="79"/>
+      <c r="Q23" s="81"/>
+      <c r="R23" s="81"/>
+      <c r="S23" s="79"/>
     </row>
     <row r="24" spans="3:19" s="53" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C24" s="50" t="s">
@@ -2525,72 +3806,72 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="87" t="s">
+      <c r="D29" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="75" t="s">
+      <c r="E29" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="75" t="s">
+      <c r="F29" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="90" t="s">
+      <c r="G29" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="75" t="s">
+      <c r="H29" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="75" t="s">
+      <c r="I29" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="77" t="s">
+      <c r="J29" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="77" t="s">
+      <c r="K29" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="75" t="s">
+      <c r="L29" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="M29" s="77" t="s">
+      <c r="M29" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="77" t="s">
+      <c r="N29" s="80" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="75" t="s">
+      <c r="O29" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="P29" s="75" t="s">
+      <c r="P29" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="75" t="s">
+      <c r="Q29" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="75" t="s">
+      <c r="R29" s="78" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="86"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="86"/>
-      <c r="F30" s="86"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="86"/>
-      <c r="I30" s="86"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="86"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="86"/>
-      <c r="P30" s="86"/>
-      <c r="Q30" s="86"/>
-      <c r="R30" s="86"/>
+      <c r="C30" s="79"/>
+      <c r="D30" s="85"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="87"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="81"/>
+      <c r="K30" s="81"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="81"/>
+      <c r="N30" s="81"/>
+      <c r="O30" s="79"/>
+      <c r="P30" s="79"/>
+      <c r="Q30" s="79"/>
+      <c r="R30" s="79"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="50" t="s">
@@ -2693,13 +3974,13 @@
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="75" t="s">
+      <c r="D36" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="75" t="s">
+      <c r="E36" s="78" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="12"/>
@@ -2710,9 +3991,9 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="86"/>
-      <c r="D37" s="86"/>
-      <c r="E37" s="86"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="79"/>
+      <c r="E37" s="79"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -2790,19 +4071,19 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="75" t="s">
+      <c r="C44" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="75" t="s">
+      <c r="D44" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="75" t="s">
+      <c r="E44" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="77" t="s">
+      <c r="F44" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="92" t="s">
+      <c r="G44" s="82" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="4"/>
@@ -2812,11 +4093,11 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="86"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="93"/>
+      <c r="C45" s="79"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="79"/>
+      <c r="F45" s="81"/>
+      <c r="G45" s="83"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -2861,28 +4142,28 @@
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="75" t="s">
+      <c r="C52" s="78" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="75" t="s">
+      <c r="D52" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="75" t="s">
+      <c r="E52" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="75" t="s">
+      <c r="F52" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="75" t="s">
+      <c r="G52" s="78" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86"/>
-      <c r="G53" s="86"/>
+      <c r="C53" s="79"/>
+      <c r="D53" s="79"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="79"/>
+      <c r="G53" s="79"/>
     </row>
     <row r="54" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -2920,30 +4201,30 @@
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="77" t="s">
+      <c r="C59" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="84"/>
-      <c r="E59" s="75" t="s">
+      <c r="D59" s="92"/>
+      <c r="E59" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="77" t="s">
+      <c r="F59" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="83"/>
+      <c r="G59" s="91"/>
     </row>
     <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="83"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="76"/>
-      <c r="F60" s="78"/>
-      <c r="G60" s="83"/>
+      <c r="C60" s="91"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="95"/>
+      <c r="F60" s="81"/>
+      <c r="G60" s="91"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="79" t="s">
+      <c r="C61" s="96" t="s">
         <v>101</v>
       </c>
-      <c r="D61" s="80"/>
+      <c r="D61" s="97"/>
       <c r="E61" s="1" t="s">
         <v>102</v>
       </c>
@@ -2952,14 +4233,14 @@
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="81"/>
-      <c r="D62" s="82"/>
+      <c r="C62" s="98"/>
+      <c r="D62" s="99"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
+      <c r="C63" s="94"/>
+      <c r="D63" s="94"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="4"/>
@@ -2970,30 +4251,82 @@
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="74" t="s">
+      <c r="C65" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="74"/>
+      <c r="D65" s="94"/>
       <c r="E65" s="54">
         <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="74" t="s">
+      <c r="C66" s="94" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="74"/>
+      <c r="D66" s="94"/>
       <c r="E66" s="54">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="C59:D60"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
     <mergeCell ref="R29:R30"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
@@ -3010,74 +4343,22 @@
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="C59:D60"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -3104,11 +4385,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="100" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
       <c r="E1" s="20" t="s">
         <v>78</v>
       </c>
@@ -3512,7 +4793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
@@ -3534,12 +4815,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="100" t="s">
         <v>108</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J14" s="20"/>
@@ -3595,10 +4876,10 @@
       <c r="K19" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="95" t="s">
+      <c r="L19" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="95"/>
+      <c r="M19" s="101"/>
       <c r="N19" s="59" t="s">
         <v>30</v>
       </c>
@@ -3714,10 +4995,10 @@
       <c r="K31" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="95" t="s">
+      <c r="L31" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="M31" s="95"/>
+      <c r="M31" s="101"/>
       <c r="N31" s="59" t="s">
         <v>30</v>
       </c>
@@ -3775,7 +5056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
@@ -3806,12 +5087,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="100" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="94"/>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E2" s="20">
@@ -3968,46 +5249,46 @@
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="80" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="84"/>
-      <c r="D17" s="75" t="s">
+      <c r="C17" s="92"/>
+      <c r="D17" s="78" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="75" t="s">
+      <c r="E17" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="75" t="s">
+      <c r="F17" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="75" t="s">
+      <c r="G17" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="75" t="s">
+      <c r="H17" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="I17" s="75" t="s">
+      <c r="I17" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="J17" s="75" t="s">
+      <c r="J17" s="78" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="86"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="96"/>
-      <c r="D18" s="86"/>
-      <c r="E18" s="86"/>
-      <c r="F18" s="86"/>
-      <c r="G18" s="86"/>
-      <c r="H18" s="86"/>
-      <c r="I18" s="86"/>
-      <c r="J18" s="86"/>
+      <c r="A18" s="79"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="102"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
     </row>
     <row r="19" spans="1:10" s="65" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60">
@@ -4049,8 +5330,8 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="82"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="99"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
@@ -4368,24 +5649,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="I17:I18"/>
     <mergeCell ref="J17:J18"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="F17:F18"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4399,7 +5680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
update proses crud menu transaksi excel
</commit_message>
<xml_diff>
--- a/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
+++ b/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="205">
   <si>
     <t>REKENING</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>4.PEMBAYARAN IURAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
   </si>
 </sst>
 </file>
@@ -1274,84 +1277,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1363,12 +1288,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,6 +1316,90 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -3054,34 +3057,34 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="93" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="59"/>
-      <c r="F6" s="74" t="s">
+      <c r="F6" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="74" t="s">
+      <c r="G6" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="74" t="s">
+      <c r="H6" s="93" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="73"/>
-      <c r="C7" s="73"/>
-      <c r="D7" s="75"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="73"/>
-      <c r="H7" s="75"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="94"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="66">
@@ -3229,13 +3232,13 @@
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="72" t="s">
+      <c r="F17" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="72" t="s">
+      <c r="G17" s="96" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="72" t="s">
+      <c r="H17" s="96" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3248,9 +3251,9 @@
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="73"/>
-      <c r="H18" s="73"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="66">
@@ -3636,13 +3639,13 @@
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="74" t="s">
+      <c r="B42" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="74" t="s">
+      <c r="C42" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="74" t="s">
+      <c r="D42" s="93" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="71"/>
@@ -3651,9 +3654,9 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
       <c r="E43" s="71"/>
       <c r="F43" s="69"/>
       <c r="G43" s="70"/>
@@ -4013,18 +4016,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4094,48 +4097,48 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="74" t="s">
+      <c r="D8" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="74" t="s">
+      <c r="E8" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="74" t="s">
+      <c r="G8" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="74" t="s">
+      <c r="H8" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="74" t="s">
+      <c r="I8" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="74" t="s">
+      <c r="J8" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="74" t="s">
+      <c r="K8" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="90"/>
+      <c r="L8" s="105"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="87"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="90"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="107"/>
+      <c r="G9" s="94"/>
+      <c r="H9" s="94"/>
+      <c r="I9" s="94"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="105"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
@@ -4210,50 +4213,50 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="74" t="s">
+      <c r="D15" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="74" t="s">
+      <c r="E15" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="74" t="s">
+      <c r="G15" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="74" t="s">
+      <c r="H15" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="77" t="s">
+      <c r="I15" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="91" t="s">
+      <c r="J15" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="90"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="90"/>
-      <c r="O15" s="90"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
+      <c r="M15" s="105"/>
+      <c r="N15" s="105"/>
+      <c r="O15" s="105"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="87"/>
-      <c r="D16" s="75"/>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
-      <c r="I16" s="78"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="90"/>
-      <c r="L16" s="90"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="90"/>
-      <c r="O16" s="90"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="94"/>
+      <c r="E16" s="94"/>
+      <c r="F16" s="94"/>
+      <c r="G16" s="94"/>
+      <c r="H16" s="94"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
+      <c r="M16" s="105"/>
+      <c r="N16" s="105"/>
+      <c r="O16" s="105"/>
     </row>
     <row r="17" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="45" t="s">
@@ -4337,76 +4340,76 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="86" t="s">
+      <c r="D22" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="74" t="s">
+      <c r="E22" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="74" t="s">
+      <c r="F22" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="74" t="s">
+      <c r="G22" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="74" t="s">
+      <c r="H22" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="74" t="s">
+      <c r="I22" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="77" t="s">
+      <c r="J22" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="91" t="s">
+      <c r="K22" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="74" t="s">
+      <c r="L22" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="74" t="s">
+      <c r="M22" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="77" t="s">
+      <c r="N22" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="77" t="s">
+      <c r="O22" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="74" t="s">
+      <c r="P22" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="77" t="s">
+      <c r="Q22" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="R22" s="77" t="s">
+      <c r="R22" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="74" t="s">
+      <c r="S22" s="93" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="75"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
-      <c r="I23" s="75"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="92"/>
-      <c r="L23" s="75"/>
-      <c r="M23" s="75"/>
-      <c r="N23" s="78"/>
-      <c r="O23" s="78"/>
-      <c r="P23" s="75"/>
-      <c r="Q23" s="78"/>
-      <c r="R23" s="78"/>
-      <c r="S23" s="75"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="102"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="98"/>
+      <c r="K23" s="104"/>
+      <c r="L23" s="94"/>
+      <c r="M23" s="94"/>
+      <c r="N23" s="98"/>
+      <c r="O23" s="98"/>
+      <c r="P23" s="94"/>
+      <c r="Q23" s="98"/>
+      <c r="R23" s="98"/>
+      <c r="S23" s="94"/>
     </row>
     <row r="24" spans="3:19" s="48" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C24" s="45" t="s">
@@ -4516,72 +4519,72 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="86" t="s">
+      <c r="D29" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="74" t="s">
+      <c r="E29" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="74" t="s">
+      <c r="F29" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="91" t="s">
+      <c r="G29" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="74" t="s">
+      <c r="H29" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="74" t="s">
+      <c r="I29" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="77" t="s">
+      <c r="J29" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="77" t="s">
+      <c r="K29" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="74" t="s">
+      <c r="L29" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="M29" s="77" t="s">
+      <c r="M29" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="77" t="s">
+      <c r="N29" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="74" t="s">
+      <c r="O29" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="P29" s="74" t="s">
+      <c r="P29" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="74" t="s">
+      <c r="Q29" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="74" t="s">
+      <c r="R29" s="93" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="75"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="92"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="75"/>
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
-      <c r="L30" s="75"/>
-      <c r="M30" s="78"/>
-      <c r="N30" s="78"/>
-      <c r="O30" s="75"/>
-      <c r="P30" s="75"/>
-      <c r="Q30" s="75"/>
-      <c r="R30" s="75"/>
+      <c r="C30" s="94"/>
+      <c r="D30" s="102"/>
+      <c r="E30" s="94"/>
+      <c r="F30" s="94"/>
+      <c r="G30" s="104"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="94"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="94"/>
+      <c r="M30" s="98"/>
+      <c r="N30" s="98"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="94"/>
+      <c r="Q30" s="94"/>
+      <c r="R30" s="94"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="45" t="s">
@@ -4684,13 +4687,13 @@
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="74" t="s">
+      <c r="D36" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="74" t="s">
+      <c r="E36" s="93" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="12"/>
@@ -4701,9 +4704,9 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="75"/>
-      <c r="D37" s="75"/>
-      <c r="E37" s="75"/>
+      <c r="C37" s="94"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="94"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -4781,19 +4784,19 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="74" t="s">
+      <c r="C44" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="74" t="s">
+      <c r="D44" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="74" t="s">
+      <c r="E44" s="93" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="77" t="s">
+      <c r="F44" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="93" t="s">
+      <c r="G44" s="99" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="4"/>
@@ -4803,11 +4806,11 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="75"/>
-      <c r="D45" s="75"/>
-      <c r="E45" s="75"/>
-      <c r="F45" s="78"/>
-      <c r="G45" s="94"/>
+      <c r="C45" s="94"/>
+      <c r="D45" s="94"/>
+      <c r="E45" s="94"/>
+      <c r="F45" s="98"/>
+      <c r="G45" s="100"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -4852,28 +4855,28 @@
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="74" t="s">
+      <c r="C52" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="74" t="s">
+      <c r="D52" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="74" t="s">
+      <c r="E52" s="93" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="74" t="s">
+      <c r="F52" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="74" t="s">
+      <c r="G52" s="93" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="75"/>
-      <c r="D53" s="75"/>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
+      <c r="C53" s="94"/>
+      <c r="D53" s="94"/>
+      <c r="E53" s="94"/>
+      <c r="F53" s="94"/>
+      <c r="G53" s="94"/>
     </row>
     <row r="54" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -4911,30 +4914,30 @@
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="77" t="s">
+      <c r="C59" s="97" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="84"/>
-      <c r="E59" s="74" t="s">
+      <c r="D59" s="109"/>
+      <c r="E59" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="77" t="s">
+      <c r="F59" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="83"/>
+      <c r="G59" s="108"/>
     </row>
     <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="83"/>
-      <c r="D60" s="85"/>
-      <c r="E60" s="73"/>
-      <c r="F60" s="78"/>
-      <c r="G60" s="83"/>
+      <c r="C60" s="108"/>
+      <c r="D60" s="110"/>
+      <c r="E60" s="95"/>
+      <c r="F60" s="98"/>
+      <c r="G60" s="108"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="79" t="s">
+      <c r="C61" s="112" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="80"/>
+      <c r="D61" s="113"/>
       <c r="E61" s="1" t="s">
         <v>98</v>
       </c>
@@ -4943,14 +4946,14 @@
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="81"/>
-      <c r="D62" s="82"/>
+      <c r="C62" s="114"/>
+      <c r="D62" s="115"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="76"/>
-      <c r="D63" s="76"/>
+      <c r="C63" s="111"/>
+      <c r="D63" s="111"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="4"/>
@@ -4961,30 +4964,82 @@
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="76" t="s">
+      <c r="C65" s="111" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="76"/>
+      <c r="D65" s="111"/>
       <c r="E65" s="49">
         <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="76" t="s">
+      <c r="C66" s="111" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="76"/>
+      <c r="D66" s="111"/>
       <c r="E66" s="49">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="C59:D60"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
     <mergeCell ref="R29:R30"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
@@ -5001,63 +5056,11 @@
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="C59:D60"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -5068,8 +5071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N96" sqref="N96"/>
+    <sheetView tabSelected="1" topLeftCell="F79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L84" sqref="L84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,7 +5085,7 @@
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="101" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" style="75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
@@ -5096,15 +5099,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="116" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B2" s="63"/>
@@ -5120,7 +5123,7 @@
       </c>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
-      <c r="I3" s="102"/>
+      <c r="I3" s="76"/>
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5132,7 +5135,7 @@
       <c r="H4" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="100" t="s">
+      <c r="I4" s="74" t="s">
         <v>192</v>
       </c>
       <c r="J4" s="16"/>
@@ -5146,7 +5149,7 @@
       <c r="H5" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="103" t="s">
+      <c r="I5" s="77" t="s">
         <v>45</v>
       </c>
       <c r="J5" s="14"/>
@@ -5160,7 +5163,7 @@
       <c r="H6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="103" t="s">
+      <c r="I6" s="77" t="s">
         <v>49</v>
       </c>
       <c r="J6" s="14"/>
@@ -5174,7 +5177,7 @@
       <c r="H7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="103" t="s">
+      <c r="I7" s="77" t="s">
         <v>46</v>
       </c>
       <c r="J7" s="14"/>
@@ -5188,7 +5191,7 @@
       <c r="H8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="103" t="s">
+      <c r="I8" s="77" t="s">
         <v>50</v>
       </c>
       <c r="J8" s="14"/>
@@ -5202,7 +5205,7 @@
       <c r="H9" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I9" s="103" t="s">
+      <c r="I9" s="77" t="s">
         <v>51</v>
       </c>
       <c r="J9" s="14"/>
@@ -5216,7 +5219,7 @@
       <c r="H10" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="103" t="s">
+      <c r="I10" s="77" t="s">
         <v>47</v>
       </c>
       <c r="J10" s="14"/>
@@ -5230,7 +5233,7 @@
       <c r="H11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I11" s="103" t="s">
+      <c r="I11" s="77" t="s">
         <v>52</v>
       </c>
       <c r="J11" s="14"/>
@@ -5244,7 +5247,7 @@
       <c r="H12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="100">
+      <c r="I12" s="74">
         <v>812345678</v>
       </c>
       <c r="J12" s="14"/>
@@ -5254,7 +5257,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
-      <c r="I13" s="102"/>
+      <c r="I13" s="76"/>
       <c r="J13" s="13"/>
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5262,50 +5265,50 @@
         <v>107</v>
       </c>
       <c r="H15" s="4"/>
-      <c r="I15" s="104"/>
+      <c r="I15" s="78"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="77" t="s">
+      <c r="B16" s="97" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="84"/>
-      <c r="D16" s="74" t="s">
+      <c r="C16" s="109"/>
+      <c r="D16" s="93" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="74" t="s">
+      <c r="E16" s="93" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="74" t="s">
+      <c r="F16" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="74" t="s">
+      <c r="G16" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="74" t="s">
+      <c r="H16" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="105" t="s">
+      <c r="I16" s="118" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="74" t="s">
+      <c r="J16" s="93" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
-      <c r="B17" s="78"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="75"/>
+      <c r="A17" s="94"/>
+      <c r="B17" s="98"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="94"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="119"/>
+      <c r="J17" s="94"/>
     </row>
     <row r="18" spans="1:10" s="57" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52">
@@ -5336,7 +5339,7 @@
         <f>+I10</f>
         <v>0286 325303</v>
       </c>
-      <c r="I18" s="107" t="str">
+      <c r="I18" s="79" t="str">
         <f>+I11</f>
         <v>TRI WURYANTO</v>
       </c>
@@ -5347,14 +5350,14 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="82"/>
+      <c r="B19" s="114"/>
+      <c r="C19" s="115"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="108"/>
+      <c r="I19" s="80"/>
       <c r="J19" s="2"/>
     </row>
     <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -5366,7 +5369,7 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="17"/>
-      <c r="I21" s="102"/>
+      <c r="I21" s="76"/>
       <c r="J21" s="13"/>
     </row>
     <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -5378,7 +5381,7 @@
       <c r="H22" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="113" t="s">
+      <c r="I22" s="85" t="s">
         <v>10</v>
       </c>
       <c r="J22" s="25"/>
@@ -5392,7 +5395,7 @@
       <c r="H23" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="109" t="s">
+      <c r="I23" s="81" t="s">
         <v>44</v>
       </c>
       <c r="J23" s="16"/>
@@ -5406,7 +5409,7 @@
       <c r="H24" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="103" t="s">
+      <c r="I24" s="77" t="s">
         <v>45</v>
       </c>
       <c r="J24" s="14"/>
@@ -5420,7 +5423,7 @@
       <c r="H25" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="103" t="s">
+      <c r="I25" s="77" t="s">
         <v>49</v>
       </c>
       <c r="J25" s="14"/>
@@ -5434,7 +5437,7 @@
       <c r="H26" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="103" t="s">
+      <c r="I26" s="77" t="s">
         <v>46</v>
       </c>
       <c r="J26" s="14"/>
@@ -5448,7 +5451,7 @@
       <c r="H27" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="103" t="s">
+      <c r="I27" s="77" t="s">
         <v>50</v>
       </c>
       <c r="J27" s="14"/>
@@ -5462,7 +5465,7 @@
       <c r="H28" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="103" t="s">
+      <c r="I28" s="77" t="s">
         <v>51</v>
       </c>
       <c r="J28" s="14"/>
@@ -5476,7 +5479,7 @@
       <c r="H29" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I29" s="103" t="s">
+      <c r="I29" s="77" t="s">
         <v>47</v>
       </c>
       <c r="J29" s="14"/>
@@ -5490,7 +5493,7 @@
       <c r="H30" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I30" s="103" t="s">
+      <c r="I30" s="77" t="s">
         <v>52</v>
       </c>
       <c r="J30" s="14"/>
@@ -5504,7 +5507,7 @@
       <c r="H31" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="100">
+      <c r="I31" s="74">
         <v>812345678</v>
       </c>
       <c r="J31" s="14"/>
@@ -5514,25 +5517,25 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
-      <c r="I32" s="102"/>
+      <c r="I32" s="76"/>
       <c r="J32" s="13"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="115"/>
-      <c r="B34" s="115"/>
-      <c r="C34" s="115"/>
-      <c r="D34" s="115"/>
-      <c r="E34" s="115"/>
-      <c r="F34" s="115"/>
-      <c r="G34" s="115"/>
-      <c r="H34" s="115"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="115"/>
-      <c r="K34" s="115"/>
-      <c r="L34" s="115"/>
+      <c r="A34" s="87"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="87"/>
+      <c r="E34" s="87"/>
+      <c r="F34" s="87"/>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="88"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="87"/>
+      <c r="L34" s="87"/>
     </row>
     <row r="35" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="99" t="s">
+      <c r="A35" s="73" t="s">
         <v>183</v>
       </c>
     </row>
@@ -5545,7 +5548,7 @@
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
-      <c r="I36" s="102"/>
+      <c r="I36" s="76"/>
       <c r="J36" s="13"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
@@ -5557,7 +5560,7 @@
       <c r="H37" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I37" s="100" t="s">
+      <c r="I37" s="74" t="s">
         <v>188</v>
       </c>
       <c r="J37" s="16"/>
@@ -5571,7 +5574,7 @@
       <c r="H38" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="103" t="s">
+      <c r="I38" s="77" t="s">
         <v>45</v>
       </c>
       <c r="J38" s="14"/>
@@ -5585,7 +5588,7 @@
       <c r="H39" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="103" t="s">
+      <c r="I39" s="77" t="s">
         <v>49</v>
       </c>
       <c r="J39" s="14"/>
@@ -5599,7 +5602,7 @@
       <c r="H40" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I40" s="103" t="s">
+      <c r="I40" s="77" t="s">
         <v>189</v>
       </c>
       <c r="J40" s="14"/>
@@ -5613,7 +5616,7 @@
       <c r="H41" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I41" s="103" t="s">
+      <c r="I41" s="77" t="s">
         <v>190</v>
       </c>
       <c r="J41" s="14"/>
@@ -5627,7 +5630,7 @@
       <c r="H42" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I42" s="103" t="s">
+      <c r="I42" s="77" t="s">
         <v>51</v>
       </c>
       <c r="J42" s="14"/>
@@ -5641,7 +5644,7 @@
       <c r="H43" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I43" s="103" t="s">
+      <c r="I43" s="77" t="s">
         <v>191</v>
       </c>
       <c r="J43" s="14"/>
@@ -5655,7 +5658,7 @@
       <c r="H44" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I44" s="103" t="s">
+      <c r="I44" s="77" t="s">
         <v>192</v>
       </c>
       <c r="J44" s="14"/>
@@ -5666,64 +5669,64 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="86" t="s">
+      <c r="A51" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="74" t="s">
+      <c r="B51" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="74" t="s">
+      <c r="C51" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="74" t="s">
+      <c r="D51" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="74" t="s">
+      <c r="E51" s="93" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="74" t="s">
+      <c r="F51" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="77" t="s">
+      <c r="G51" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="91" t="s">
+      <c r="H51" s="103" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="87"/>
-      <c r="B52" s="75"/>
-      <c r="C52" s="75"/>
-      <c r="D52" s="75"/>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="78"/>
-      <c r="H52" s="92"/>
+      <c r="A52" s="102"/>
+      <c r="B52" s="94"/>
+      <c r="C52" s="94"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="94"/>
+      <c r="F52" s="94"/>
+      <c r="G52" s="98"/>
+      <c r="H52" s="104"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="110" t="s">
+      <c r="A53" s="82" t="s">
         <v>188</v>
       </c>
-      <c r="B53" s="111" t="s">
+      <c r="B53" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="C53" s="111" t="s">
+      <c r="C53" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="111" t="s">
+      <c r="D53" s="83" t="s">
         <v>189</v>
       </c>
-      <c r="E53" s="112">
+      <c r="E53" s="84">
         <v>27740</v>
       </c>
-      <c r="F53" s="111" t="s">
+      <c r="F53" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="G53" s="111" t="s">
+      <c r="G53" s="83" t="s">
         <v>191</v>
       </c>
-      <c r="H53" s="111">
+      <c r="H53" s="83">
         <v>700409</v>
       </c>
     </row>
@@ -5736,7 +5739,7 @@
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="17"/>
-      <c r="I55" s="102"/>
+      <c r="I55" s="76"/>
       <c r="J55" s="13"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
@@ -5748,7 +5751,7 @@
       <c r="H56" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I56" s="114" t="s">
+      <c r="I56" s="86" t="s">
         <v>188</v>
       </c>
       <c r="J56" s="16"/>
@@ -5762,7 +5765,7 @@
       <c r="H57" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I57" s="103" t="s">
+      <c r="I57" s="77" t="s">
         <v>45</v>
       </c>
       <c r="J57" s="14"/>
@@ -5776,7 +5779,7 @@
       <c r="H58" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I58" s="103" t="s">
+      <c r="I58" s="77" t="s">
         <v>49</v>
       </c>
       <c r="J58" s="14"/>
@@ -5790,7 +5793,7 @@
       <c r="H59" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I59" s="103" t="s">
+      <c r="I59" s="77" t="s">
         <v>189</v>
       </c>
       <c r="J59" s="14"/>
@@ -5804,7 +5807,7 @@
       <c r="H60" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I60" s="103" t="s">
+      <c r="I60" s="77" t="s">
         <v>190</v>
       </c>
       <c r="J60" s="14"/>
@@ -5818,7 +5821,7 @@
       <c r="H61" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I61" s="103" t="s">
+      <c r="I61" s="77" t="s">
         <v>51</v>
       </c>
       <c r="J61" s="14"/>
@@ -5832,7 +5835,7 @@
       <c r="H62" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I62" s="103" t="s">
+      <c r="I62" s="77" t="s">
         <v>191</v>
       </c>
       <c r="J62" s="14"/>
@@ -5846,27 +5849,27 @@
       <c r="H63" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I63" s="103" t="s">
+      <c r="I63" s="77" t="s">
         <v>192</v>
       </c>
       <c r="J63" s="14"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A69" s="115"/>
-      <c r="B69" s="115"/>
-      <c r="C69" s="115"/>
-      <c r="D69" s="115"/>
-      <c r="E69" s="115"/>
-      <c r="F69" s="115"/>
-      <c r="G69" s="115"/>
-      <c r="H69" s="115"/>
-      <c r="I69" s="116"/>
-      <c r="J69" s="115"/>
-      <c r="K69" s="115"/>
-      <c r="L69" s="115"/>
+      <c r="A69" s="87"/>
+      <c r="B69" s="87"/>
+      <c r="C69" s="87"/>
+      <c r="D69" s="87"/>
+      <c r="E69" s="87"/>
+      <c r="F69" s="87"/>
+      <c r="G69" s="87"/>
+      <c r="H69" s="87"/>
+      <c r="I69" s="88"/>
+      <c r="J69" s="87"/>
+      <c r="K69" s="87"/>
+      <c r="L69" s="87"/>
     </row>
     <row r="70" spans="1:12" ht="21" x14ac:dyDescent="0.35">
-      <c r="A70" s="99" t="s">
+      <c r="A70" s="73" t="s">
         <v>193</v>
       </c>
     </row>
@@ -5921,7 +5924,7 @@
       <c r="H74" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I74" s="117" t="s">
+      <c r="I74" s="89" t="s">
         <v>48</v>
       </c>
       <c r="J74" s="14"/>
@@ -6065,6 +6068,9 @@
         <v>42449</v>
       </c>
       <c r="J84" s="14"/>
+      <c r="K84" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="E85" s="14"/>
@@ -6165,1016 +6171,1027 @@
       <c r="J91" s="13"/>
     </row>
     <row r="93" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="101"/>
-      <c r="B93" s="101"/>
-      <c r="C93" s="101"/>
-      <c r="D93" s="101"/>
-      <c r="E93" s="101"/>
-      <c r="F93" s="101"/>
-      <c r="G93" s="101"/>
-      <c r="H93" s="101"/>
-      <c r="J93" s="101"/>
-      <c r="K93" s="101"/>
-      <c r="L93" s="101"/>
-      <c r="M93" s="101"/>
-      <c r="N93" s="101"/>
-      <c r="O93" s="101"/>
-      <c r="P93" s="101"/>
-      <c r="Q93" s="101"/>
-      <c r="R93" s="101"/>
-      <c r="S93" s="101"/>
-      <c r="T93" s="101"/>
-      <c r="U93" s="101"/>
-      <c r="V93" s="101"/>
-      <c r="W93" s="101"/>
-      <c r="X93" s="101"/>
+      <c r="A93" s="75"/>
+      <c r="B93" s="75"/>
+      <c r="C93" s="75"/>
+      <c r="D93" s="75"/>
+      <c r="E93" s="75"/>
+      <c r="F93" s="75"/>
+      <c r="G93" s="75"/>
+      <c r="H93" s="75"/>
+      <c r="J93" s="75"/>
+      <c r="K93" s="75"/>
+      <c r="L93" s="75"/>
+      <c r="M93" s="75"/>
+      <c r="N93" s="75"/>
+      <c r="O93" s="75"/>
+      <c r="P93" s="75"/>
+      <c r="Q93" s="75"/>
+      <c r="R93" s="75"/>
+      <c r="S93" s="75"/>
+      <c r="T93" s="75"/>
+      <c r="U93" s="75"/>
+      <c r="V93" s="75"/>
+      <c r="W93" s="75"/>
+      <c r="X93" s="75"/>
     </row>
     <row r="94" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="101"/>
-      <c r="B94" s="101"/>
-      <c r="C94" s="101"/>
-      <c r="D94" s="101"/>
-      <c r="E94" s="101"/>
-      <c r="F94" s="101"/>
-      <c r="G94" s="101"/>
-      <c r="H94" s="101"/>
-      <c r="J94" s="101"/>
-      <c r="K94" s="101"/>
-      <c r="L94" s="101"/>
-      <c r="M94" s="101"/>
-      <c r="N94" s="101"/>
-      <c r="O94" s="101"/>
-      <c r="P94" s="101"/>
-      <c r="Q94" s="101"/>
-      <c r="R94" s="101"/>
-      <c r="S94" s="101"/>
-      <c r="T94" s="101"/>
-      <c r="U94" s="101"/>
-      <c r="V94" s="101"/>
-      <c r="W94" s="101"/>
-      <c r="X94" s="101"/>
+      <c r="A94" s="75"/>
+      <c r="B94" s="75"/>
+      <c r="C94" s="75"/>
+      <c r="D94" s="75"/>
+      <c r="E94" s="75"/>
+      <c r="F94" s="75"/>
+      <c r="G94" s="75"/>
+      <c r="H94" s="75"/>
+      <c r="J94" s="75"/>
+      <c r="K94" s="75"/>
+      <c r="L94" s="75"/>
+      <c r="M94" s="75"/>
+      <c r="N94" s="75"/>
+      <c r="O94" s="75"/>
+      <c r="P94" s="75"/>
+      <c r="Q94" s="75"/>
+      <c r="R94" s="75"/>
+      <c r="S94" s="75"/>
+      <c r="T94" s="75"/>
+      <c r="U94" s="75"/>
+      <c r="V94" s="75"/>
+      <c r="W94" s="75"/>
+      <c r="X94" s="75"/>
     </row>
     <row r="95" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="101"/>
-      <c r="B95" s="101"/>
-      <c r="C95" s="101"/>
-      <c r="D95" s="101"/>
-      <c r="E95" s="101"/>
-      <c r="F95" s="101"/>
-      <c r="G95" s="101"/>
-      <c r="H95" s="101"/>
-      <c r="J95" s="101"/>
-      <c r="K95" s="101"/>
-      <c r="L95" s="101"/>
-      <c r="M95" s="101"/>
-      <c r="N95" s="101"/>
-      <c r="O95" s="101"/>
-      <c r="P95" s="101"/>
-      <c r="Q95" s="101"/>
-      <c r="R95" s="101"/>
-      <c r="S95" s="101"/>
-      <c r="T95" s="101"/>
-      <c r="U95" s="101"/>
-      <c r="V95" s="101"/>
-      <c r="W95" s="101"/>
-      <c r="X95" s="101"/>
+      <c r="A95" s="75"/>
+      <c r="B95" s="75"/>
+      <c r="C95" s="75"/>
+      <c r="D95" s="75"/>
+      <c r="E95" s="75"/>
+      <c r="F95" s="75"/>
+      <c r="G95" s="75"/>
+      <c r="H95" s="75"/>
+      <c r="J95" s="75"/>
+      <c r="K95" s="75"/>
+      <c r="L95" s="75"/>
+      <c r="M95" s="75"/>
+      <c r="N95" s="75"/>
+      <c r="O95" s="75"/>
+      <c r="P95" s="75"/>
+      <c r="Q95" s="75"/>
+      <c r="R95" s="75"/>
+      <c r="S95" s="75"/>
+      <c r="T95" s="75"/>
+      <c r="U95" s="75"/>
+      <c r="V95" s="75"/>
+      <c r="W95" s="75"/>
+      <c r="X95" s="75"/>
     </row>
     <row r="96" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="101"/>
-      <c r="B96" s="101"/>
-      <c r="C96" s="101"/>
-      <c r="D96" s="101"/>
-      <c r="E96" s="101"/>
-      <c r="F96" s="101"/>
-      <c r="G96" s="101"/>
-      <c r="H96" s="101"/>
-      <c r="J96" s="101"/>
-      <c r="K96" s="101"/>
-      <c r="L96" s="101"/>
-      <c r="M96" s="101"/>
-      <c r="N96" s="101"/>
-      <c r="O96" s="101"/>
-      <c r="P96" s="101"/>
-      <c r="Q96" s="101"/>
-      <c r="R96" s="101"/>
-      <c r="S96" s="101"/>
-      <c r="T96" s="101"/>
-      <c r="U96" s="101"/>
-      <c r="V96" s="101"/>
-      <c r="W96" s="101"/>
-      <c r="X96" s="101"/>
+      <c r="A96" s="75"/>
+      <c r="B96" s="75"/>
+      <c r="C96" s="75"/>
+      <c r="D96" s="75"/>
+      <c r="E96" s="75"/>
+      <c r="F96" s="75"/>
+      <c r="G96" s="75"/>
+      <c r="H96" s="75"/>
+      <c r="J96" s="75"/>
+      <c r="K96" s="75"/>
+      <c r="L96" s="75"/>
+      <c r="M96" s="75"/>
+      <c r="N96" s="75"/>
+      <c r="O96" s="75"/>
+      <c r="P96" s="75"/>
+      <c r="Q96" s="75"/>
+      <c r="R96" s="75"/>
+      <c r="S96" s="75"/>
+      <c r="T96" s="75"/>
+      <c r="U96" s="75"/>
+      <c r="V96" s="75"/>
+      <c r="W96" s="75"/>
+      <c r="X96" s="75"/>
     </row>
     <row r="97" spans="1:24" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="101"/>
-      <c r="B97" s="101"/>
-      <c r="C97" s="101"/>
-      <c r="D97" s="101"/>
-      <c r="E97" s="101"/>
-      <c r="F97" s="101"/>
-      <c r="G97" s="101"/>
-      <c r="H97" s="101"/>
-      <c r="J97" s="101"/>
-      <c r="K97" s="101"/>
-      <c r="L97" s="101"/>
-      <c r="M97" s="101"/>
-      <c r="N97" s="101"/>
-      <c r="O97" s="101"/>
-      <c r="P97" s="101"/>
-      <c r="Q97" s="101"/>
-      <c r="R97" s="101"/>
-      <c r="S97" s="101"/>
-      <c r="T97" s="101"/>
-      <c r="U97" s="101"/>
-      <c r="V97" s="101"/>
-      <c r="W97" s="101"/>
-      <c r="X97" s="101"/>
+      <c r="A97" s="75"/>
+      <c r="B97" s="75"/>
+      <c r="C97" s="75"/>
+      <c r="D97" s="75"/>
+      <c r="E97" s="75"/>
+      <c r="F97" s="75"/>
+      <c r="G97" s="75"/>
+      <c r="H97" s="75"/>
+      <c r="J97" s="75"/>
+      <c r="K97" s="75"/>
+      <c r="L97" s="75"/>
+      <c r="M97" s="75"/>
+      <c r="N97" s="75"/>
+      <c r="O97" s="75"/>
+      <c r="P97" s="75"/>
+      <c r="Q97" s="75"/>
+      <c r="R97" s="75"/>
+      <c r="S97" s="75"/>
+      <c r="T97" s="75"/>
+      <c r="U97" s="75"/>
+      <c r="V97" s="75"/>
+      <c r="W97" s="75"/>
+      <c r="X97" s="75"/>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A98" s="119" t="s">
+      <c r="A98" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="B98" s="101"/>
-      <c r="C98" s="101"/>
-      <c r="D98" s="101"/>
-      <c r="E98" s="101"/>
-      <c r="F98" s="101"/>
-      <c r="G98" s="101"/>
-      <c r="H98" s="101"/>
-      <c r="J98" s="101"/>
-      <c r="K98" s="101"/>
-      <c r="L98" s="101"/>
-      <c r="M98" s="101"/>
-      <c r="N98" s="101"/>
-      <c r="O98" s="101"/>
-      <c r="P98" s="101"/>
-      <c r="Q98" s="101"/>
-      <c r="R98" s="101"/>
-      <c r="S98" s="101"/>
-      <c r="T98" s="101"/>
-      <c r="U98" s="101"/>
-      <c r="V98" s="101"/>
-      <c r="W98" s="101"/>
-      <c r="X98" s="101"/>
+      <c r="B98" s="75"/>
+      <c r="C98" s="75"/>
+      <c r="D98" s="75"/>
+      <c r="E98" s="75"/>
+      <c r="F98" s="75"/>
+      <c r="G98" s="75"/>
+      <c r="H98" s="75"/>
+      <c r="J98" s="75"/>
+      <c r="K98" s="75"/>
+      <c r="L98" s="75"/>
+      <c r="M98" s="75"/>
+      <c r="N98" s="75"/>
+      <c r="O98" s="75"/>
+      <c r="P98" s="75"/>
+      <c r="Q98" s="75"/>
+      <c r="R98" s="75"/>
+      <c r="S98" s="75"/>
+      <c r="T98" s="75"/>
+      <c r="U98" s="75"/>
+      <c r="V98" s="75"/>
+      <c r="W98" s="75"/>
+      <c r="X98" s="75"/>
     </row>
     <row r="99" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A99" s="118" t="s">
+      <c r="A99" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B99" s="118" t="s">
+      <c r="B99" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C99" s="118" t="s">
+      <c r="C99" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="D99" s="118" t="s">
+      <c r="D99" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="E99" s="118" t="s">
+      <c r="E99" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="F99" s="101"/>
-      <c r="G99" s="101"/>
-      <c r="H99" s="101"/>
-      <c r="J99" s="101"/>
-      <c r="K99" s="101"/>
-      <c r="L99" s="101"/>
-      <c r="M99" s="101"/>
-      <c r="N99" s="101"/>
-      <c r="O99" s="101"/>
-      <c r="P99" s="101"/>
-      <c r="Q99" s="101"/>
-      <c r="R99" s="101"/>
-      <c r="S99" s="101"/>
-      <c r="T99" s="101"/>
-      <c r="U99" s="101"/>
-      <c r="V99" s="101"/>
-      <c r="W99" s="101"/>
+      <c r="F99" s="75"/>
+      <c r="G99" s="75"/>
+      <c r="H99" s="75"/>
+      <c r="J99" s="75"/>
+      <c r="K99" s="75"/>
+      <c r="L99" s="75"/>
+      <c r="M99" s="75"/>
+      <c r="N99" s="75"/>
+      <c r="O99" s="75"/>
+      <c r="P99" s="75"/>
+      <c r="Q99" s="75"/>
+      <c r="R99" s="75"/>
+      <c r="S99" s="75"/>
+      <c r="T99" s="75"/>
+      <c r="U99" s="75"/>
+      <c r="V99" s="75"/>
+      <c r="W99" s="75"/>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A100" s="118" t="s">
+      <c r="A100" s="90" t="s">
         <v>195</v>
       </c>
-      <c r="B100" s="118">
+      <c r="B100" s="90">
         <v>114001</v>
       </c>
-      <c r="C100" s="118" t="s">
+      <c r="C100" s="90" t="s">
         <v>196</v>
       </c>
-      <c r="D100" s="118" t="s">
+      <c r="D100" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="E100" s="118">
+      <c r="E100" s="90">
         <v>100000</v>
       </c>
-      <c r="F100" s="101"/>
-      <c r="G100" s="101"/>
-      <c r="H100" s="101"/>
-      <c r="J100" s="101"/>
-      <c r="K100" s="101"/>
-      <c r="L100" s="101"/>
-      <c r="M100" s="101"/>
-      <c r="N100" s="101"/>
-      <c r="O100" s="101"/>
-      <c r="P100" s="101"/>
-      <c r="Q100" s="101"/>
-      <c r="R100" s="101"/>
-      <c r="S100" s="101"/>
-      <c r="T100" s="101"/>
-      <c r="U100" s="101"/>
-      <c r="V100" s="101"/>
-      <c r="W100" s="101"/>
+      <c r="F100" s="75"/>
+      <c r="G100" s="75"/>
+      <c r="H100" s="75"/>
+      <c r="J100" s="75"/>
+      <c r="K100" s="75"/>
+      <c r="L100" s="75"/>
+      <c r="M100" s="75"/>
+      <c r="N100" s="75"/>
+      <c r="O100" s="75"/>
+      <c r="P100" s="75"/>
+      <c r="Q100" s="75"/>
+      <c r="R100" s="75"/>
+      <c r="S100" s="75"/>
+      <c r="T100" s="75"/>
+      <c r="U100" s="75"/>
+      <c r="V100" s="75"/>
+      <c r="W100" s="75"/>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A101" s="118"/>
-      <c r="B101" s="118">
+      <c r="A101" s="90"/>
+      <c r="B101" s="90">
         <v>220001</v>
       </c>
-      <c r="C101" s="118" t="s">
+      <c r="C101" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="D101" s="118" t="s">
+      <c r="D101" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="E101" s="118">
+      <c r="E101" s="90">
         <v>40000</v>
       </c>
-      <c r="F101" s="101"/>
-      <c r="G101" s="101"/>
-      <c r="H101" s="101"/>
-      <c r="J101" s="101"/>
-      <c r="K101" s="101"/>
-      <c r="L101" s="101"/>
-      <c r="M101" s="101"/>
-      <c r="N101" s="101"/>
-      <c r="O101" s="101"/>
-      <c r="P101" s="101"/>
-      <c r="Q101" s="101"/>
-      <c r="R101" s="101"/>
-      <c r="S101" s="101"/>
-      <c r="T101" s="101"/>
-      <c r="U101" s="101"/>
-      <c r="V101" s="101"/>
-      <c r="W101" s="101"/>
+      <c r="F101" s="75"/>
+      <c r="G101" s="75"/>
+      <c r="H101" s="75"/>
+      <c r="J101" s="75"/>
+      <c r="K101" s="75"/>
+      <c r="L101" s="75"/>
+      <c r="M101" s="75"/>
+      <c r="N101" s="75"/>
+      <c r="O101" s="75"/>
+      <c r="P101" s="75"/>
+      <c r="Q101" s="75"/>
+      <c r="R101" s="75"/>
+      <c r="S101" s="75"/>
+      <c r="T101" s="75"/>
+      <c r="U101" s="75"/>
+      <c r="V101" s="75"/>
+      <c r="W101" s="75"/>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A102" s="118"/>
-      <c r="B102" s="118">
+      <c r="A102" s="90"/>
+      <c r="B102" s="90">
         <v>220002</v>
       </c>
-      <c r="C102" s="118" t="s">
+      <c r="C102" s="90" t="s">
         <v>198</v>
       </c>
-      <c r="D102" s="118" t="s">
+      <c r="D102" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="E102" s="118">
+      <c r="E102" s="90">
         <v>60000</v>
       </c>
-      <c r="F102" s="101"/>
-      <c r="G102" s="101"/>
-      <c r="H102" s="101"/>
-      <c r="J102" s="101"/>
-      <c r="K102" s="101"/>
-      <c r="L102" s="101"/>
-      <c r="M102" s="101"/>
-      <c r="N102" s="101"/>
-      <c r="O102" s="101"/>
-      <c r="P102" s="101"/>
-      <c r="Q102" s="101"/>
-      <c r="R102" s="101"/>
-      <c r="S102" s="101"/>
-      <c r="T102" s="101"/>
-      <c r="U102" s="101"/>
-      <c r="V102" s="101"/>
-      <c r="W102" s="101"/>
+      <c r="F102" s="75"/>
+      <c r="G102" s="75"/>
+      <c r="H102" s="75"/>
+      <c r="J102" s="75"/>
+      <c r="K102" s="75"/>
+      <c r="L102" s="75"/>
+      <c r="M102" s="75"/>
+      <c r="N102" s="75"/>
+      <c r="O102" s="75"/>
+      <c r="P102" s="75"/>
+      <c r="Q102" s="75"/>
+      <c r="R102" s="75"/>
+      <c r="S102" s="75"/>
+      <c r="T102" s="75"/>
+      <c r="U102" s="75"/>
+      <c r="V102" s="75"/>
+      <c r="W102" s="75"/>
     </row>
     <row r="103" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="101"/>
-      <c r="B103" s="101"/>
-      <c r="C103" s="101"/>
-      <c r="D103" s="101"/>
-      <c r="E103" s="101"/>
-      <c r="F103" s="101"/>
-      <c r="G103" s="101"/>
-      <c r="H103" s="101"/>
-      <c r="J103" s="101"/>
-      <c r="K103" s="101"/>
-      <c r="L103" s="101"/>
-      <c r="M103" s="101"/>
-      <c r="N103" s="101"/>
-      <c r="O103" s="101"/>
-      <c r="P103" s="101"/>
-      <c r="Q103" s="101"/>
-      <c r="R103" s="101"/>
-      <c r="S103" s="101"/>
-      <c r="T103" s="101"/>
-      <c r="U103" s="101"/>
-      <c r="V103" s="101"/>
-      <c r="W103" s="101"/>
-      <c r="X103" s="101"/>
+      <c r="A103" s="75"/>
+      <c r="B103" s="75"/>
+      <c r="C103" s="75"/>
+      <c r="D103" s="75"/>
+      <c r="E103" s="75"/>
+      <c r="F103" s="75"/>
+      <c r="G103" s="75"/>
+      <c r="H103" s="75"/>
+      <c r="J103" s="75"/>
+      <c r="K103" s="75"/>
+      <c r="L103" s="75"/>
+      <c r="M103" s="75"/>
+      <c r="N103" s="75"/>
+      <c r="O103" s="75"/>
+      <c r="P103" s="75"/>
+      <c r="Q103" s="75"/>
+      <c r="R103" s="75"/>
+      <c r="S103" s="75"/>
+      <c r="T103" s="75"/>
+      <c r="U103" s="75"/>
+      <c r="V103" s="75"/>
+      <c r="W103" s="75"/>
+      <c r="X103" s="75"/>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A104" s="119" t="s">
+      <c r="A104" s="91" t="s">
         <v>199</v>
       </c>
-      <c r="B104" s="101"/>
-      <c r="C104" s="101"/>
-      <c r="D104" s="101"/>
-      <c r="E104" s="101"/>
-      <c r="F104" s="101"/>
-      <c r="G104" s="101"/>
-      <c r="H104" s="101"/>
-      <c r="J104" s="101"/>
-      <c r="K104" s="101"/>
-      <c r="L104" s="101"/>
-      <c r="M104" s="101"/>
-      <c r="N104" s="101"/>
-      <c r="O104" s="101"/>
-      <c r="P104" s="101"/>
-      <c r="Q104" s="101"/>
-      <c r="R104" s="101"/>
-      <c r="S104" s="101"/>
-      <c r="T104" s="101"/>
-      <c r="U104" s="101"/>
-      <c r="V104" s="101"/>
-      <c r="W104" s="101"/>
-      <c r="X104" s="101"/>
+      <c r="B104" s="75"/>
+      <c r="C104" s="75"/>
+      <c r="D104" s="75"/>
+      <c r="E104" s="75"/>
+      <c r="F104" s="75"/>
+      <c r="G104" s="75"/>
+      <c r="H104" s="75"/>
+      <c r="J104" s="75"/>
+      <c r="K104" s="75"/>
+      <c r="L104" s="75"/>
+      <c r="M104" s="75"/>
+      <c r="N104" s="75"/>
+      <c r="O104" s="75"/>
+      <c r="P104" s="75"/>
+      <c r="Q104" s="75"/>
+      <c r="R104" s="75"/>
+      <c r="S104" s="75"/>
+      <c r="T104" s="75"/>
+      <c r="U104" s="75"/>
+      <c r="V104" s="75"/>
+      <c r="W104" s="75"/>
+      <c r="X104" s="75"/>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A105" s="118" t="s">
+      <c r="A105" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="B105" s="118" t="s">
+      <c r="B105" s="90" t="s">
         <v>38</v>
       </c>
-      <c r="C105" s="118" t="s">
+      <c r="C105" s="90" t="s">
         <v>34</v>
       </c>
-      <c r="D105" s="101"/>
-      <c r="E105" s="101"/>
-      <c r="F105" s="101"/>
-      <c r="G105" s="101"/>
-      <c r="H105" s="101"/>
-      <c r="J105" s="101"/>
-      <c r="K105" s="101"/>
-      <c r="L105" s="101"/>
-      <c r="M105" s="101"/>
-      <c r="N105" s="101"/>
-      <c r="O105" s="101"/>
-      <c r="P105" s="101"/>
-      <c r="Q105" s="101"/>
-      <c r="R105" s="101"/>
-      <c r="S105" s="101"/>
-      <c r="T105" s="101"/>
-      <c r="U105" s="101"/>
-      <c r="V105" s="101"/>
-      <c r="W105" s="101"/>
+      <c r="D105" s="75"/>
+      <c r="E105" s="75"/>
+      <c r="F105" s="75"/>
+      <c r="G105" s="75"/>
+      <c r="H105" s="75"/>
+      <c r="J105" s="75"/>
+      <c r="K105" s="75"/>
+      <c r="L105" s="75"/>
+      <c r="M105" s="75"/>
+      <c r="N105" s="75"/>
+      <c r="O105" s="75"/>
+      <c r="P105" s="75"/>
+      <c r="Q105" s="75"/>
+      <c r="R105" s="75"/>
+      <c r="S105" s="75"/>
+      <c r="T105" s="75"/>
+      <c r="U105" s="75"/>
+      <c r="V105" s="75"/>
+      <c r="W105" s="75"/>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A106" s="118">
+      <c r="A106" s="90">
         <v>114001</v>
       </c>
-      <c r="B106" s="118" t="s">
+      <c r="B106" s="90" t="s">
         <v>130</v>
       </c>
-      <c r="C106" s="118"/>
-      <c r="D106" s="101" t="s">
+      <c r="C106" s="90"/>
+      <c r="D106" s="75" t="s">
         <v>200</v>
       </c>
-      <c r="E106" s="101"/>
-      <c r="F106" s="101"/>
-      <c r="G106" s="101"/>
-      <c r="H106" s="101"/>
-      <c r="J106" s="101"/>
-      <c r="K106" s="101"/>
-      <c r="L106" s="101"/>
-      <c r="M106" s="101"/>
-      <c r="N106" s="101"/>
-      <c r="O106" s="101"/>
-      <c r="P106" s="101"/>
-      <c r="Q106" s="101"/>
-      <c r="R106" s="101"/>
-      <c r="S106" s="101"/>
-      <c r="T106" s="101"/>
-      <c r="U106" s="101"/>
-      <c r="V106" s="101"/>
-      <c r="W106" s="101"/>
+      <c r="E106" s="75"/>
+      <c r="F106" s="75"/>
+      <c r="G106" s="75"/>
+      <c r="H106" s="75"/>
+      <c r="J106" s="75"/>
+      <c r="K106" s="75"/>
+      <c r="L106" s="75"/>
+      <c r="M106" s="75"/>
+      <c r="N106" s="75"/>
+      <c r="O106" s="75"/>
+      <c r="P106" s="75"/>
+      <c r="Q106" s="75"/>
+      <c r="R106" s="75"/>
+      <c r="S106" s="75"/>
+      <c r="T106" s="75"/>
+      <c r="U106" s="75"/>
+      <c r="V106" s="75"/>
+      <c r="W106" s="75"/>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A107" s="118">
+      <c r="A107" s="90">
         <v>220001</v>
       </c>
-      <c r="B107" s="118" t="s">
+      <c r="B107" s="90" t="s">
         <v>177</v>
       </c>
-      <c r="C107" s="118"/>
-      <c r="D107" s="101" t="s">
+      <c r="C107" s="90"/>
+      <c r="D107" s="75" t="s">
         <v>201</v>
       </c>
-      <c r="E107" s="101"/>
-      <c r="F107" s="101"/>
-      <c r="G107" s="101"/>
-      <c r="H107" s="101"/>
-      <c r="J107" s="101"/>
-      <c r="K107" s="101"/>
-      <c r="L107" s="101"/>
-      <c r="M107" s="101"/>
-      <c r="N107" s="101"/>
-      <c r="O107" s="101"/>
-      <c r="P107" s="101"/>
-      <c r="Q107" s="101"/>
-      <c r="R107" s="101"/>
-      <c r="S107" s="101"/>
-      <c r="T107" s="101"/>
-      <c r="U107" s="101"/>
-      <c r="V107" s="101"/>
-      <c r="W107" s="101"/>
+      <c r="E107" s="75"/>
+      <c r="F107" s="75"/>
+      <c r="G107" s="75"/>
+      <c r="H107" s="75"/>
+      <c r="J107" s="75"/>
+      <c r="K107" s="75"/>
+      <c r="L107" s="75"/>
+      <c r="M107" s="75"/>
+      <c r="N107" s="75"/>
+      <c r="O107" s="75"/>
+      <c r="P107" s="75"/>
+      <c r="Q107" s="75"/>
+      <c r="R107" s="75"/>
+      <c r="S107" s="75"/>
+      <c r="T107" s="75"/>
+      <c r="U107" s="75"/>
+      <c r="V107" s="75"/>
+      <c r="W107" s="75"/>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A108" s="118">
+      <c r="A108" s="90">
         <v>220002</v>
       </c>
-      <c r="B108" s="118" t="s">
+      <c r="B108" s="90" t="s">
         <v>178</v>
       </c>
-      <c r="C108" s="118"/>
-      <c r="D108" s="101" t="s">
+      <c r="C108" s="90"/>
+      <c r="D108" s="75" t="s">
         <v>202</v>
       </c>
-      <c r="E108" s="101"/>
-      <c r="F108" s="101"/>
-      <c r="G108" s="101"/>
-      <c r="H108" s="101"/>
-      <c r="J108" s="101"/>
-      <c r="K108" s="101"/>
-      <c r="L108" s="101"/>
-      <c r="M108" s="101"/>
-      <c r="N108" s="101"/>
-      <c r="O108" s="101"/>
-      <c r="P108" s="101"/>
-      <c r="Q108" s="101"/>
-      <c r="R108" s="101"/>
-      <c r="S108" s="101"/>
-      <c r="T108" s="101"/>
-      <c r="U108" s="101"/>
-      <c r="V108" s="101"/>
-      <c r="W108" s="101"/>
+      <c r="E108" s="75"/>
+      <c r="F108" s="75"/>
+      <c r="G108" s="75"/>
+      <c r="H108" s="75"/>
+      <c r="J108" s="75"/>
+      <c r="K108" s="75"/>
+      <c r="L108" s="75"/>
+      <c r="M108" s="75"/>
+      <c r="N108" s="75"/>
+      <c r="O108" s="75"/>
+      <c r="P108" s="75"/>
+      <c r="Q108" s="75"/>
+      <c r="R108" s="75"/>
+      <c r="S108" s="75"/>
+      <c r="T108" s="75"/>
+      <c r="U108" s="75"/>
+      <c r="V108" s="75"/>
+      <c r="W108" s="75"/>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A109" s="101"/>
-      <c r="B109" s="101"/>
-      <c r="C109" s="101"/>
-      <c r="D109" s="101"/>
-      <c r="E109" s="101"/>
-      <c r="F109" s="101"/>
-      <c r="G109" s="101"/>
-      <c r="H109" s="101"/>
-      <c r="J109" s="101"/>
-      <c r="K109" s="101"/>
-      <c r="L109" s="101"/>
-      <c r="M109" s="101"/>
-      <c r="N109" s="101"/>
-      <c r="O109" s="101"/>
-      <c r="P109" s="101"/>
-      <c r="Q109" s="101"/>
-      <c r="R109" s="101"/>
-      <c r="S109" s="101"/>
-      <c r="T109" s="101"/>
-      <c r="U109" s="101"/>
-      <c r="V109" s="101"/>
-      <c r="W109" s="101"/>
-      <c r="X109" s="101"/>
+      <c r="A109" s="75"/>
+      <c r="B109" s="75"/>
+      <c r="C109" s="75"/>
+      <c r="D109" s="75"/>
+      <c r="E109" s="75"/>
+      <c r="F109" s="75"/>
+      <c r="G109" s="75"/>
+      <c r="H109" s="75"/>
+      <c r="J109" s="75"/>
+      <c r="K109" s="75"/>
+      <c r="L109" s="75"/>
+      <c r="M109" s="75"/>
+      <c r="N109" s="75"/>
+      <c r="O109" s="75"/>
+      <c r="P109" s="75"/>
+      <c r="Q109" s="75"/>
+      <c r="R109" s="75"/>
+      <c r="S109" s="75"/>
+      <c r="T109" s="75"/>
+      <c r="U109" s="75"/>
+      <c r="V109" s="75"/>
+      <c r="W109" s="75"/>
+      <c r="X109" s="75"/>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A110" s="101"/>
-      <c r="B110" s="101"/>
-      <c r="C110" s="101"/>
-      <c r="D110" s="101"/>
-      <c r="E110" s="101"/>
-      <c r="F110" s="101"/>
-      <c r="G110" s="101"/>
-      <c r="H110" s="101"/>
-      <c r="J110" s="101"/>
-      <c r="K110" s="101"/>
-      <c r="L110" s="101"/>
-      <c r="M110" s="101"/>
-      <c r="N110" s="101"/>
-      <c r="O110" s="101"/>
-      <c r="P110" s="101"/>
-      <c r="Q110" s="101"/>
-      <c r="R110" s="101"/>
-      <c r="S110" s="101"/>
-      <c r="T110" s="101"/>
-      <c r="U110" s="101"/>
-      <c r="V110" s="101"/>
-      <c r="W110" s="101"/>
-      <c r="X110" s="101"/>
+      <c r="A110" s="75"/>
+      <c r="B110" s="75"/>
+      <c r="C110" s="75"/>
+      <c r="D110" s="75"/>
+      <c r="E110" s="75"/>
+      <c r="F110" s="75"/>
+      <c r="G110" s="75"/>
+      <c r="H110" s="75"/>
+      <c r="J110" s="75"/>
+      <c r="K110" s="75"/>
+      <c r="L110" s="75"/>
+      <c r="M110" s="75"/>
+      <c r="N110" s="75"/>
+      <c r="O110" s="75"/>
+      <c r="P110" s="75"/>
+      <c r="Q110" s="75"/>
+      <c r="R110" s="75"/>
+      <c r="S110" s="75"/>
+      <c r="T110" s="75"/>
+      <c r="U110" s="75"/>
+      <c r="V110" s="75"/>
+      <c r="W110" s="75"/>
+      <c r="X110" s="75"/>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A111" s="116"/>
-      <c r="B111" s="116"/>
-      <c r="C111" s="116"/>
-      <c r="D111" s="116"/>
-      <c r="E111" s="116"/>
-      <c r="F111" s="116"/>
-      <c r="G111" s="116"/>
-      <c r="H111" s="116"/>
-      <c r="I111" s="116"/>
-      <c r="J111" s="116"/>
-      <c r="K111" s="116"/>
-      <c r="L111" s="116"/>
-      <c r="M111" s="116"/>
-      <c r="N111" s="116"/>
-      <c r="O111" s="101"/>
-      <c r="P111" s="101"/>
-      <c r="Q111" s="101"/>
-      <c r="R111" s="101"/>
-      <c r="S111" s="101"/>
-      <c r="T111" s="101"/>
-      <c r="U111" s="101"/>
-      <c r="V111" s="101"/>
-      <c r="W111" s="101"/>
-      <c r="X111" s="101"/>
+      <c r="A111" s="88"/>
+      <c r="B111" s="88"/>
+      <c r="C111" s="88"/>
+      <c r="D111" s="88"/>
+      <c r="E111" s="88"/>
+      <c r="F111" s="88"/>
+      <c r="G111" s="88"/>
+      <c r="H111" s="88"/>
+      <c r="I111" s="88"/>
+      <c r="J111" s="88"/>
+      <c r="K111" s="88"/>
+      <c r="L111" s="88"/>
+      <c r="M111" s="88"/>
+      <c r="N111" s="88"/>
+      <c r="O111" s="75"/>
+      <c r="P111" s="75"/>
+      <c r="Q111" s="75"/>
+      <c r="R111" s="75"/>
+      <c r="S111" s="75"/>
+      <c r="T111" s="75"/>
+      <c r="U111" s="75"/>
+      <c r="V111" s="75"/>
+      <c r="W111" s="75"/>
+      <c r="X111" s="75"/>
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A112" s="101"/>
-      <c r="B112" s="101"/>
-      <c r="C112" s="101"/>
-      <c r="D112" s="101"/>
-      <c r="E112" s="101"/>
-      <c r="F112" s="101"/>
-      <c r="G112" s="101"/>
-      <c r="H112" s="101"/>
-      <c r="J112" s="101"/>
-      <c r="K112" s="101"/>
-      <c r="L112" s="101"/>
-      <c r="M112" s="101"/>
-      <c r="N112" s="101"/>
-      <c r="O112" s="101"/>
-      <c r="P112" s="101"/>
-      <c r="Q112" s="101"/>
-      <c r="R112" s="101"/>
-      <c r="S112" s="101"/>
-      <c r="T112" s="101"/>
-      <c r="U112" s="101"/>
-      <c r="V112" s="101"/>
-      <c r="W112" s="101"/>
-      <c r="X112" s="101"/>
+      <c r="A112" s="75"/>
+      <c r="B112" s="75"/>
+      <c r="C112" s="75"/>
+      <c r="D112" s="75"/>
+      <c r="E112" s="75"/>
+      <c r="F112" s="75"/>
+      <c r="G112" s="75"/>
+      <c r="H112" s="75"/>
+      <c r="J112" s="75"/>
+      <c r="K112" s="75"/>
+      <c r="L112" s="75"/>
+      <c r="M112" s="75"/>
+      <c r="N112" s="75"/>
+      <c r="O112" s="75"/>
+      <c r="P112" s="75"/>
+      <c r="Q112" s="75"/>
+      <c r="R112" s="75"/>
+      <c r="S112" s="75"/>
+      <c r="T112" s="75"/>
+      <c r="U112" s="75"/>
+      <c r="V112" s="75"/>
+      <c r="W112" s="75"/>
+      <c r="X112" s="75"/>
     </row>
     <row r="113" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A113" s="120" t="s">
+      <c r="A113" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="B113" s="101"/>
-      <c r="C113" s="101"/>
-      <c r="D113" s="101"/>
-      <c r="E113" s="101"/>
-      <c r="F113" s="101"/>
-      <c r="G113" s="101"/>
-      <c r="H113" s="101"/>
-      <c r="J113" s="101"/>
-      <c r="K113" s="101"/>
-      <c r="L113" s="101"/>
-      <c r="M113" s="101"/>
-      <c r="N113" s="101"/>
-      <c r="O113" s="101"/>
-      <c r="P113" s="101"/>
-      <c r="Q113" s="101"/>
-      <c r="R113" s="101"/>
-      <c r="S113" s="101"/>
-      <c r="T113" s="101"/>
-      <c r="U113" s="101"/>
-      <c r="V113" s="101"/>
-      <c r="W113" s="101"/>
-      <c r="X113" s="101"/>
+      <c r="B113" s="75"/>
+      <c r="C113" s="75"/>
+      <c r="D113" s="75"/>
+      <c r="E113" s="75"/>
+      <c r="F113" s="75"/>
+      <c r="G113" s="75"/>
+      <c r="H113" s="75"/>
+      <c r="J113" s="75"/>
+      <c r="K113" s="75"/>
+      <c r="L113" s="75"/>
+      <c r="M113" s="75"/>
+      <c r="N113" s="75"/>
+      <c r="O113" s="75"/>
+      <c r="P113" s="75"/>
+      <c r="Q113" s="75"/>
+      <c r="R113" s="75"/>
+      <c r="S113" s="75"/>
+      <c r="T113" s="75"/>
+      <c r="U113" s="75"/>
+      <c r="V113" s="75"/>
+      <c r="W113" s="75"/>
+      <c r="X113" s="75"/>
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A114" s="101"/>
-      <c r="B114" s="101"/>
-      <c r="C114" s="101"/>
-      <c r="D114" s="101"/>
-      <c r="E114" s="101"/>
-      <c r="F114" s="101"/>
-      <c r="G114" s="101"/>
-      <c r="H114" s="101"/>
-      <c r="J114" s="101"/>
-      <c r="K114" s="101"/>
-      <c r="L114" s="101"/>
-      <c r="M114" s="101"/>
-      <c r="N114" s="101"/>
-      <c r="O114" s="101"/>
-      <c r="P114" s="101"/>
-      <c r="Q114" s="101"/>
-      <c r="R114" s="101"/>
-      <c r="S114" s="101"/>
-      <c r="T114" s="101"/>
-      <c r="U114" s="101"/>
-      <c r="V114" s="101"/>
-      <c r="W114" s="101"/>
-      <c r="X114" s="101"/>
+      <c r="A114" s="75"/>
+      <c r="B114" s="75"/>
+      <c r="C114" s="75"/>
+      <c r="D114" s="75"/>
+      <c r="E114" s="75"/>
+      <c r="F114" s="75"/>
+      <c r="G114" s="75"/>
+      <c r="H114" s="75"/>
+      <c r="J114" s="75"/>
+      <c r="K114" s="75"/>
+      <c r="L114" s="75"/>
+      <c r="M114" s="75"/>
+      <c r="N114" s="75"/>
+      <c r="O114" s="75"/>
+      <c r="P114" s="75"/>
+      <c r="Q114" s="75"/>
+      <c r="R114" s="75"/>
+      <c r="S114" s="75"/>
+      <c r="T114" s="75"/>
+      <c r="U114" s="75"/>
+      <c r="V114" s="75"/>
+      <c r="W114" s="75"/>
+      <c r="X114" s="75"/>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A115" s="101"/>
-      <c r="B115" s="101"/>
-      <c r="C115" s="101"/>
-      <c r="D115" s="101"/>
-      <c r="E115" s="101"/>
-      <c r="F115" s="101"/>
-      <c r="G115" s="101"/>
-      <c r="H115" s="101"/>
-      <c r="J115" s="101"/>
-      <c r="K115" s="101"/>
-      <c r="L115" s="101"/>
-      <c r="M115" s="101"/>
-      <c r="N115" s="101"/>
-      <c r="O115" s="101"/>
-      <c r="P115" s="101"/>
-      <c r="Q115" s="101"/>
-      <c r="R115" s="101"/>
-      <c r="S115" s="101"/>
-      <c r="T115" s="101"/>
-      <c r="U115" s="101"/>
-      <c r="V115" s="101"/>
-      <c r="W115" s="101"/>
-      <c r="X115" s="101"/>
+      <c r="A115" s="75"/>
+      <c r="B115" s="75"/>
+      <c r="C115" s="75"/>
+      <c r="D115" s="75"/>
+      <c r="E115" s="75"/>
+      <c r="F115" s="75"/>
+      <c r="G115" s="75"/>
+      <c r="H115" s="75"/>
+      <c r="J115" s="75"/>
+      <c r="K115" s="75"/>
+      <c r="L115" s="75"/>
+      <c r="M115" s="75"/>
+      <c r="N115" s="75"/>
+      <c r="O115" s="75"/>
+      <c r="P115" s="75"/>
+      <c r="Q115" s="75"/>
+      <c r="R115" s="75"/>
+      <c r="S115" s="75"/>
+      <c r="T115" s="75"/>
+      <c r="U115" s="75"/>
+      <c r="V115" s="75"/>
+      <c r="W115" s="75"/>
+      <c r="X115" s="75"/>
     </row>
     <row r="116" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A116" s="101"/>
-      <c r="B116" s="101"/>
-      <c r="C116" s="101"/>
-      <c r="D116" s="101"/>
-      <c r="E116" s="101"/>
-      <c r="F116" s="101"/>
-      <c r="G116" s="101"/>
-      <c r="H116" s="101"/>
-      <c r="J116" s="101"/>
-      <c r="K116" s="101"/>
-      <c r="L116" s="101"/>
-      <c r="M116" s="101"/>
-      <c r="N116" s="101"/>
-      <c r="O116" s="101"/>
-      <c r="P116" s="101"/>
-      <c r="Q116" s="101"/>
-      <c r="R116" s="101"/>
-      <c r="S116" s="101"/>
-      <c r="T116" s="101"/>
-      <c r="U116" s="101"/>
-      <c r="V116" s="101"/>
-      <c r="W116" s="101"/>
-      <c r="X116" s="101"/>
+      <c r="A116" s="75"/>
+      <c r="B116" s="75"/>
+      <c r="C116" s="75"/>
+      <c r="D116" s="75"/>
+      <c r="E116" s="75"/>
+      <c r="F116" s="75"/>
+      <c r="G116" s="75"/>
+      <c r="H116" s="75"/>
+      <c r="J116" s="75"/>
+      <c r="K116" s="75"/>
+      <c r="L116" s="75"/>
+      <c r="M116" s="75"/>
+      <c r="N116" s="75"/>
+      <c r="O116" s="75"/>
+      <c r="P116" s="75"/>
+      <c r="Q116" s="75"/>
+      <c r="R116" s="75"/>
+      <c r="S116" s="75"/>
+      <c r="T116" s="75"/>
+      <c r="U116" s="75"/>
+      <c r="V116" s="75"/>
+      <c r="W116" s="75"/>
+      <c r="X116" s="75"/>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A117" s="101"/>
-      <c r="B117" s="101"/>
-      <c r="C117" s="101"/>
-      <c r="D117" s="101"/>
-      <c r="E117" s="101"/>
-      <c r="F117" s="101"/>
-      <c r="G117" s="101"/>
-      <c r="H117" s="101"/>
-      <c r="J117" s="101"/>
-      <c r="K117" s="101"/>
-      <c r="L117" s="101"/>
-      <c r="M117" s="101"/>
-      <c r="N117" s="101"/>
-      <c r="O117" s="101"/>
-      <c r="P117" s="101"/>
-      <c r="Q117" s="101"/>
-      <c r="R117" s="101"/>
-      <c r="S117" s="101"/>
-      <c r="T117" s="101"/>
-      <c r="U117" s="101"/>
-      <c r="V117" s="101"/>
-      <c r="W117" s="101"/>
-      <c r="X117" s="101"/>
+      <c r="A117" s="75"/>
+      <c r="B117" s="75"/>
+      <c r="C117" s="75"/>
+      <c r="D117" s="75"/>
+      <c r="E117" s="75"/>
+      <c r="F117" s="75"/>
+      <c r="G117" s="75"/>
+      <c r="H117" s="75"/>
+      <c r="J117" s="75"/>
+      <c r="K117" s="75"/>
+      <c r="L117" s="75"/>
+      <c r="M117" s="75"/>
+      <c r="N117" s="75"/>
+      <c r="O117" s="75"/>
+      <c r="P117" s="75"/>
+      <c r="Q117" s="75"/>
+      <c r="R117" s="75"/>
+      <c r="S117" s="75"/>
+      <c r="T117" s="75"/>
+      <c r="U117" s="75"/>
+      <c r="V117" s="75"/>
+      <c r="W117" s="75"/>
+      <c r="X117" s="75"/>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A118" s="101"/>
-      <c r="B118" s="101"/>
-      <c r="C118" s="101"/>
-      <c r="D118" s="101"/>
-      <c r="E118" s="101"/>
-      <c r="F118" s="101"/>
-      <c r="G118" s="101"/>
-      <c r="H118" s="101"/>
-      <c r="J118" s="101"/>
-      <c r="K118" s="101"/>
-      <c r="L118" s="101"/>
-      <c r="M118" s="101"/>
-      <c r="N118" s="101"/>
-      <c r="O118" s="101"/>
-      <c r="P118" s="101"/>
-      <c r="Q118" s="101"/>
-      <c r="R118" s="101"/>
-      <c r="S118" s="101"/>
-      <c r="T118" s="101"/>
-      <c r="U118" s="101"/>
-      <c r="V118" s="101"/>
-      <c r="W118" s="101"/>
-      <c r="X118" s="101"/>
+      <c r="A118" s="75"/>
+      <c r="B118" s="75"/>
+      <c r="C118" s="75"/>
+      <c r="D118" s="75"/>
+      <c r="E118" s="75"/>
+      <c r="F118" s="75"/>
+      <c r="G118" s="75"/>
+      <c r="H118" s="75"/>
+      <c r="J118" s="75"/>
+      <c r="K118" s="75"/>
+      <c r="L118" s="75"/>
+      <c r="M118" s="75"/>
+      <c r="N118" s="75"/>
+      <c r="O118" s="75"/>
+      <c r="P118" s="75"/>
+      <c r="Q118" s="75"/>
+      <c r="R118" s="75"/>
+      <c r="S118" s="75"/>
+      <c r="T118" s="75"/>
+      <c r="U118" s="75"/>
+      <c r="V118" s="75"/>
+      <c r="W118" s="75"/>
+      <c r="X118" s="75"/>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A119" s="101"/>
-      <c r="B119" s="101"/>
-      <c r="C119" s="101"/>
-      <c r="D119" s="101"/>
-      <c r="E119" s="101"/>
-      <c r="F119" s="101"/>
-      <c r="G119" s="101"/>
-      <c r="H119" s="101"/>
-      <c r="J119" s="101"/>
-      <c r="K119" s="101"/>
-      <c r="L119" s="101"/>
-      <c r="M119" s="101"/>
-      <c r="N119" s="101"/>
-      <c r="O119" s="101"/>
-      <c r="P119" s="101"/>
-      <c r="Q119" s="101"/>
-      <c r="R119" s="101"/>
-      <c r="S119" s="101"/>
-      <c r="T119" s="101"/>
-      <c r="U119" s="101"/>
-      <c r="V119" s="101"/>
-      <c r="W119" s="101"/>
-      <c r="X119" s="101"/>
+      <c r="A119" s="75"/>
+      <c r="B119" s="75"/>
+      <c r="C119" s="75"/>
+      <c r="D119" s="75"/>
+      <c r="E119" s="75"/>
+      <c r="F119" s="75"/>
+      <c r="G119" s="75"/>
+      <c r="H119" s="75"/>
+      <c r="J119" s="75"/>
+      <c r="K119" s="75"/>
+      <c r="L119" s="75"/>
+      <c r="M119" s="75"/>
+      <c r="N119" s="75"/>
+      <c r="O119" s="75"/>
+      <c r="P119" s="75"/>
+      <c r="Q119" s="75"/>
+      <c r="R119" s="75"/>
+      <c r="S119" s="75"/>
+      <c r="T119" s="75"/>
+      <c r="U119" s="75"/>
+      <c r="V119" s="75"/>
+      <c r="W119" s="75"/>
+      <c r="X119" s="75"/>
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A120" s="101"/>
-      <c r="B120" s="101"/>
-      <c r="C120" s="101"/>
-      <c r="D120" s="101"/>
-      <c r="E120" s="101"/>
-      <c r="F120" s="101"/>
-      <c r="G120" s="101"/>
-      <c r="H120" s="101"/>
-      <c r="J120" s="101"/>
-      <c r="K120" s="101"/>
-      <c r="L120" s="101"/>
-      <c r="M120" s="101"/>
-      <c r="N120" s="101"/>
-      <c r="O120" s="101"/>
-      <c r="P120" s="101"/>
-      <c r="Q120" s="101"/>
-      <c r="R120" s="101"/>
-      <c r="S120" s="101"/>
-      <c r="T120" s="101"/>
-      <c r="U120" s="101"/>
-      <c r="V120" s="101"/>
-      <c r="W120" s="101"/>
-      <c r="X120" s="101"/>
+      <c r="A120" s="75"/>
+      <c r="B120" s="75"/>
+      <c r="C120" s="75"/>
+      <c r="D120" s="75"/>
+      <c r="E120" s="75"/>
+      <c r="F120" s="75"/>
+      <c r="G120" s="75"/>
+      <c r="H120" s="75"/>
+      <c r="J120" s="75"/>
+      <c r="K120" s="75"/>
+      <c r="L120" s="75"/>
+      <c r="M120" s="75"/>
+      <c r="N120" s="75"/>
+      <c r="O120" s="75"/>
+      <c r="P120" s="75"/>
+      <c r="Q120" s="75"/>
+      <c r="R120" s="75"/>
+      <c r="S120" s="75"/>
+      <c r="T120" s="75"/>
+      <c r="U120" s="75"/>
+      <c r="V120" s="75"/>
+      <c r="W120" s="75"/>
+      <c r="X120" s="75"/>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A121" s="101"/>
-      <c r="B121" s="101"/>
-      <c r="C121" s="101"/>
-      <c r="D121" s="101"/>
-      <c r="E121" s="101"/>
-      <c r="F121" s="101"/>
-      <c r="G121" s="101"/>
-      <c r="H121" s="101"/>
-      <c r="J121" s="101"/>
-      <c r="K121" s="101"/>
-      <c r="L121" s="101"/>
-      <c r="M121" s="101"/>
-      <c r="N121" s="101"/>
-      <c r="O121" s="101"/>
-      <c r="P121" s="101"/>
-      <c r="Q121" s="101"/>
-      <c r="R121" s="101"/>
-      <c r="S121" s="101"/>
-      <c r="T121" s="101"/>
-      <c r="U121" s="101"/>
-      <c r="V121" s="101"/>
-      <c r="W121" s="101"/>
-      <c r="X121" s="101"/>
+      <c r="A121" s="75"/>
+      <c r="B121" s="75"/>
+      <c r="C121" s="75"/>
+      <c r="D121" s="75"/>
+      <c r="E121" s="75"/>
+      <c r="F121" s="75"/>
+      <c r="G121" s="75"/>
+      <c r="H121" s="75"/>
+      <c r="J121" s="75"/>
+      <c r="K121" s="75"/>
+      <c r="L121" s="75"/>
+      <c r="M121" s="75"/>
+      <c r="N121" s="75"/>
+      <c r="O121" s="75"/>
+      <c r="P121" s="75"/>
+      <c r="Q121" s="75"/>
+      <c r="R121" s="75"/>
+      <c r="S121" s="75"/>
+      <c r="T121" s="75"/>
+      <c r="U121" s="75"/>
+      <c r="V121" s="75"/>
+      <c r="W121" s="75"/>
+      <c r="X121" s="75"/>
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A122" s="101"/>
-      <c r="B122" s="101"/>
-      <c r="C122" s="101"/>
-      <c r="D122" s="101"/>
-      <c r="E122" s="101"/>
-      <c r="F122" s="101"/>
-      <c r="G122" s="101"/>
-      <c r="H122" s="101"/>
-      <c r="J122" s="101"/>
-      <c r="K122" s="101"/>
-      <c r="L122" s="101"/>
-      <c r="M122" s="101"/>
-      <c r="N122" s="101"/>
-      <c r="O122" s="101"/>
-      <c r="P122" s="101"/>
-      <c r="Q122" s="101"/>
-      <c r="R122" s="101"/>
-      <c r="S122" s="101"/>
-      <c r="T122" s="101"/>
-      <c r="U122" s="101"/>
-      <c r="V122" s="101"/>
-      <c r="W122" s="101"/>
-      <c r="X122" s="101"/>
+      <c r="A122" s="75"/>
+      <c r="B122" s="75"/>
+      <c r="C122" s="75"/>
+      <c r="D122" s="75"/>
+      <c r="E122" s="75"/>
+      <c r="F122" s="75"/>
+      <c r="G122" s="75"/>
+      <c r="H122" s="75"/>
+      <c r="J122" s="75"/>
+      <c r="K122" s="75"/>
+      <c r="L122" s="75"/>
+      <c r="M122" s="75"/>
+      <c r="N122" s="75"/>
+      <c r="O122" s="75"/>
+      <c r="P122" s="75"/>
+      <c r="Q122" s="75"/>
+      <c r="R122" s="75"/>
+      <c r="S122" s="75"/>
+      <c r="T122" s="75"/>
+      <c r="U122" s="75"/>
+      <c r="V122" s="75"/>
+      <c r="W122" s="75"/>
+      <c r="X122" s="75"/>
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A123" s="101"/>
-      <c r="B123" s="101"/>
-      <c r="C123" s="101"/>
-      <c r="D123" s="101"/>
-      <c r="E123" s="101"/>
-      <c r="F123" s="101"/>
-      <c r="G123" s="101"/>
-      <c r="H123" s="101"/>
-      <c r="J123" s="101"/>
-      <c r="K123" s="101"/>
-      <c r="L123" s="101"/>
-      <c r="M123" s="101"/>
-      <c r="N123" s="101"/>
-      <c r="O123" s="101"/>
-      <c r="P123" s="101"/>
-      <c r="Q123" s="101"/>
-      <c r="R123" s="101"/>
-      <c r="S123" s="101"/>
-      <c r="T123" s="101"/>
-      <c r="U123" s="101"/>
-      <c r="V123" s="101"/>
-      <c r="W123" s="101"/>
-      <c r="X123" s="101"/>
+      <c r="A123" s="75"/>
+      <c r="B123" s="75"/>
+      <c r="C123" s="75"/>
+      <c r="D123" s="75"/>
+      <c r="E123" s="75"/>
+      <c r="F123" s="75"/>
+      <c r="G123" s="75"/>
+      <c r="H123" s="75"/>
+      <c r="J123" s="75"/>
+      <c r="K123" s="75"/>
+      <c r="L123" s="75"/>
+      <c r="M123" s="75"/>
+      <c r="N123" s="75"/>
+      <c r="O123" s="75"/>
+      <c r="P123" s="75"/>
+      <c r="Q123" s="75"/>
+      <c r="R123" s="75"/>
+      <c r="S123" s="75"/>
+      <c r="T123" s="75"/>
+      <c r="U123" s="75"/>
+      <c r="V123" s="75"/>
+      <c r="W123" s="75"/>
+      <c r="X123" s="75"/>
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A124" s="101"/>
-      <c r="B124" s="101"/>
-      <c r="C124" s="101"/>
-      <c r="D124" s="101"/>
-      <c r="E124" s="101"/>
-      <c r="F124" s="101"/>
-      <c r="G124" s="101"/>
-      <c r="H124" s="101"/>
-      <c r="J124" s="101"/>
-      <c r="K124" s="101"/>
-      <c r="L124" s="101"/>
-      <c r="M124" s="101"/>
-      <c r="N124" s="101"/>
-      <c r="O124" s="101"/>
-      <c r="P124" s="101"/>
-      <c r="Q124" s="101"/>
-      <c r="R124" s="101"/>
-      <c r="S124" s="101"/>
-      <c r="T124" s="101"/>
-      <c r="U124" s="101"/>
-      <c r="V124" s="101"/>
-      <c r="W124" s="101"/>
-      <c r="X124" s="101"/>
+      <c r="A124" s="75"/>
+      <c r="B124" s="75"/>
+      <c r="C124" s="75"/>
+      <c r="D124" s="75"/>
+      <c r="E124" s="75"/>
+      <c r="F124" s="75"/>
+      <c r="G124" s="75"/>
+      <c r="H124" s="75"/>
+      <c r="J124" s="75"/>
+      <c r="K124" s="75"/>
+      <c r="L124" s="75"/>
+      <c r="M124" s="75"/>
+      <c r="N124" s="75"/>
+      <c r="O124" s="75"/>
+      <c r="P124" s="75"/>
+      <c r="Q124" s="75"/>
+      <c r="R124" s="75"/>
+      <c r="S124" s="75"/>
+      <c r="T124" s="75"/>
+      <c r="U124" s="75"/>
+      <c r="V124" s="75"/>
+      <c r="W124" s="75"/>
+      <c r="X124" s="75"/>
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A125" s="101"/>
-      <c r="B125" s="101"/>
-      <c r="C125" s="101"/>
-      <c r="D125" s="101"/>
-      <c r="E125" s="101"/>
-      <c r="F125" s="101"/>
-      <c r="G125" s="101"/>
-      <c r="H125" s="101"/>
-      <c r="J125" s="101"/>
-      <c r="K125" s="101"/>
-      <c r="L125" s="101"/>
-      <c r="M125" s="101"/>
-      <c r="N125" s="101"/>
-      <c r="O125" s="101"/>
-      <c r="P125" s="101"/>
-      <c r="Q125" s="101"/>
-      <c r="R125" s="101"/>
-      <c r="S125" s="101"/>
-      <c r="T125" s="101"/>
-      <c r="U125" s="101"/>
-      <c r="V125" s="101"/>
-      <c r="W125" s="101"/>
-      <c r="X125" s="101"/>
+      <c r="A125" s="75"/>
+      <c r="B125" s="75"/>
+      <c r="C125" s="75"/>
+      <c r="D125" s="75"/>
+      <c r="E125" s="75"/>
+      <c r="F125" s="75"/>
+      <c r="G125" s="75"/>
+      <c r="H125" s="75"/>
+      <c r="J125" s="75"/>
+      <c r="K125" s="75"/>
+      <c r="L125" s="75"/>
+      <c r="M125" s="75"/>
+      <c r="N125" s="75"/>
+      <c r="O125" s="75"/>
+      <c r="P125" s="75"/>
+      <c r="Q125" s="75"/>
+      <c r="R125" s="75"/>
+      <c r="S125" s="75"/>
+      <c r="T125" s="75"/>
+      <c r="U125" s="75"/>
+      <c r="V125" s="75"/>
+      <c r="W125" s="75"/>
+      <c r="X125" s="75"/>
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A126" s="101"/>
-      <c r="B126" s="101"/>
-      <c r="C126" s="101"/>
-      <c r="D126" s="101"/>
-      <c r="E126" s="101"/>
-      <c r="F126" s="101"/>
-      <c r="G126" s="101"/>
-      <c r="H126" s="101"/>
-      <c r="J126" s="101"/>
-      <c r="K126" s="101"/>
-      <c r="L126" s="101"/>
-      <c r="M126" s="101"/>
-      <c r="N126" s="101"/>
-      <c r="O126" s="101"/>
-      <c r="P126" s="101"/>
-      <c r="Q126" s="101"/>
-      <c r="R126" s="101"/>
-      <c r="S126" s="101"/>
-      <c r="T126" s="101"/>
-      <c r="U126" s="101"/>
-      <c r="V126" s="101"/>
-      <c r="W126" s="101"/>
-      <c r="X126" s="101"/>
+      <c r="A126" s="75"/>
+      <c r="B126" s="75"/>
+      <c r="C126" s="75"/>
+      <c r="D126" s="75"/>
+      <c r="E126" s="75"/>
+      <c r="F126" s="75"/>
+      <c r="G126" s="75"/>
+      <c r="H126" s="75"/>
+      <c r="J126" s="75"/>
+      <c r="K126" s="75"/>
+      <c r="L126" s="75"/>
+      <c r="M126" s="75"/>
+      <c r="N126" s="75"/>
+      <c r="O126" s="75"/>
+      <c r="P126" s="75"/>
+      <c r="Q126" s="75"/>
+      <c r="R126" s="75"/>
+      <c r="S126" s="75"/>
+      <c r="T126" s="75"/>
+      <c r="U126" s="75"/>
+      <c r="V126" s="75"/>
+      <c r="W126" s="75"/>
+      <c r="X126" s="75"/>
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A127" s="101"/>
-      <c r="B127" s="101"/>
-      <c r="C127" s="101"/>
-      <c r="D127" s="101"/>
-      <c r="E127" s="101"/>
-      <c r="F127" s="101"/>
-      <c r="G127" s="101"/>
-      <c r="H127" s="101"/>
-      <c r="J127" s="101"/>
-      <c r="K127" s="101"/>
-      <c r="L127" s="101"/>
-      <c r="M127" s="101"/>
-      <c r="N127" s="101"/>
-      <c r="O127" s="101"/>
-      <c r="P127" s="101"/>
-      <c r="Q127" s="101"/>
-      <c r="R127" s="101"/>
-      <c r="S127" s="101"/>
-      <c r="T127" s="101"/>
-      <c r="U127" s="101"/>
-      <c r="V127" s="101"/>
-      <c r="W127" s="101"/>
-      <c r="X127" s="101"/>
+      <c r="A127" s="75"/>
+      <c r="B127" s="75"/>
+      <c r="C127" s="75"/>
+      <c r="D127" s="75"/>
+      <c r="E127" s="75"/>
+      <c r="F127" s="75"/>
+      <c r="G127" s="75"/>
+      <c r="H127" s="75"/>
+      <c r="J127" s="75"/>
+      <c r="K127" s="75"/>
+      <c r="L127" s="75"/>
+      <c r="M127" s="75"/>
+      <c r="N127" s="75"/>
+      <c r="O127" s="75"/>
+      <c r="P127" s="75"/>
+      <c r="Q127" s="75"/>
+      <c r="R127" s="75"/>
+      <c r="S127" s="75"/>
+      <c r="T127" s="75"/>
+      <c r="U127" s="75"/>
+      <c r="V127" s="75"/>
+      <c r="W127" s="75"/>
+      <c r="X127" s="75"/>
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A128" s="101"/>
-      <c r="B128" s="101"/>
-      <c r="C128" s="101"/>
-      <c r="D128" s="101"/>
-      <c r="E128" s="101"/>
-      <c r="F128" s="101"/>
-      <c r="G128" s="101"/>
-      <c r="H128" s="101"/>
-      <c r="J128" s="101"/>
-      <c r="K128" s="101"/>
-      <c r="L128" s="101"/>
-      <c r="M128" s="101"/>
-      <c r="N128" s="101"/>
-      <c r="O128" s="101"/>
-      <c r="P128" s="101"/>
-      <c r="Q128" s="101"/>
-      <c r="R128" s="101"/>
-      <c r="S128" s="101"/>
-      <c r="T128" s="101"/>
-      <c r="U128" s="101"/>
-      <c r="V128" s="101"/>
-      <c r="W128" s="101"/>
-      <c r="X128" s="101"/>
+      <c r="A128" s="75"/>
+      <c r="B128" s="75"/>
+      <c r="C128" s="75"/>
+      <c r="D128" s="75"/>
+      <c r="E128" s="75"/>
+      <c r="F128" s="75"/>
+      <c r="G128" s="75"/>
+      <c r="H128" s="75"/>
+      <c r="J128" s="75"/>
+      <c r="K128" s="75"/>
+      <c r="L128" s="75"/>
+      <c r="M128" s="75"/>
+      <c r="N128" s="75"/>
+      <c r="O128" s="75"/>
+      <c r="P128" s="75"/>
+      <c r="Q128" s="75"/>
+      <c r="R128" s="75"/>
+      <c r="S128" s="75"/>
+      <c r="T128" s="75"/>
+      <c r="U128" s="75"/>
+      <c r="V128" s="75"/>
+      <c r="W128" s="75"/>
+      <c r="X128" s="75"/>
     </row>
     <row r="129" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A129" s="101"/>
-      <c r="B129" s="101"/>
-      <c r="C129" s="101"/>
-      <c r="D129" s="101"/>
-      <c r="E129" s="101"/>
-      <c r="F129" s="101"/>
-      <c r="G129" s="101"/>
-      <c r="H129" s="101"/>
-      <c r="J129" s="101"/>
-      <c r="K129" s="101"/>
-      <c r="L129" s="101"/>
-      <c r="M129" s="101"/>
-      <c r="N129" s="101"/>
-      <c r="O129" s="101"/>
-      <c r="P129" s="101"/>
-      <c r="Q129" s="101"/>
-      <c r="R129" s="101"/>
-      <c r="S129" s="101"/>
-      <c r="T129" s="101"/>
-      <c r="U129" s="101"/>
-      <c r="V129" s="101"/>
-      <c r="W129" s="101"/>
-      <c r="X129" s="101"/>
+      <c r="A129" s="75"/>
+      <c r="B129" s="75"/>
+      <c r="C129" s="75"/>
+      <c r="D129" s="75"/>
+      <c r="E129" s="75"/>
+      <c r="F129" s="75"/>
+      <c r="G129" s="75"/>
+      <c r="H129" s="75"/>
+      <c r="J129" s="75"/>
+      <c r="K129" s="75"/>
+      <c r="L129" s="75"/>
+      <c r="M129" s="75"/>
+      <c r="N129" s="75"/>
+      <c r="O129" s="75"/>
+      <c r="P129" s="75"/>
+      <c r="Q129" s="75"/>
+      <c r="R129" s="75"/>
+      <c r="S129" s="75"/>
+      <c r="T129" s="75"/>
+      <c r="U129" s="75"/>
+      <c r="V129" s="75"/>
+      <c r="W129" s="75"/>
+      <c r="X129" s="75"/>
     </row>
     <row r="130" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A130" s="101"/>
-      <c r="B130" s="101"/>
-      <c r="C130" s="101"/>
-      <c r="D130" s="101"/>
-      <c r="E130" s="101"/>
-      <c r="F130" s="101"/>
-      <c r="G130" s="101"/>
-      <c r="H130" s="101"/>
-      <c r="J130" s="101"/>
-      <c r="K130" s="101"/>
-      <c r="L130" s="101"/>
-      <c r="M130" s="101"/>
-      <c r="N130" s="101"/>
-      <c r="O130" s="101"/>
-      <c r="P130" s="101"/>
-      <c r="Q130" s="101"/>
-      <c r="R130" s="101"/>
-      <c r="S130" s="101"/>
-      <c r="T130" s="101"/>
-      <c r="U130" s="101"/>
-      <c r="V130" s="101"/>
-      <c r="W130" s="101"/>
-      <c r="X130" s="101"/>
+      <c r="A130" s="75"/>
+      <c r="B130" s="75"/>
+      <c r="C130" s="75"/>
+      <c r="D130" s="75"/>
+      <c r="E130" s="75"/>
+      <c r="F130" s="75"/>
+      <c r="G130" s="75"/>
+      <c r="H130" s="75"/>
+      <c r="J130" s="75"/>
+      <c r="K130" s="75"/>
+      <c r="L130" s="75"/>
+      <c r="M130" s="75"/>
+      <c r="N130" s="75"/>
+      <c r="O130" s="75"/>
+      <c r="P130" s="75"/>
+      <c r="Q130" s="75"/>
+      <c r="R130" s="75"/>
+      <c r="S130" s="75"/>
+      <c r="T130" s="75"/>
+      <c r="U130" s="75"/>
+      <c r="V130" s="75"/>
+      <c r="W130" s="75"/>
+      <c r="X130" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
@@ -7183,17 +7200,6 @@
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7235,12 +7241,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="116" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
+      <c r="B1" s="116"/>
+      <c r="C1" s="116"/>
+      <c r="D1" s="116"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J14" s="20"/>
@@ -7296,10 +7302,10 @@
       <c r="K19" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="96" t="s">
+      <c r="L19" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="M19" s="96"/>
+      <c r="M19" s="120"/>
       <c r="N19" s="51" t="s">
         <v>30</v>
       </c>
@@ -7415,10 +7421,10 @@
       <c r="K31" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="L31" s="96" t="s">
+      <c r="L31" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="M31" s="96"/>
+      <c r="M31" s="120"/>
       <c r="N31" s="51" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
tes koneksi sql server-failed
</commit_message>
<xml_diff>
--- a/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
+++ b/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="215">
   <si>
     <t>REKENING</t>
   </si>
@@ -640,6 +640,36 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>PEMBAYARAN IURAN</t>
+  </si>
+  <si>
+    <t>(cek NO_KTP di database "DAFTAR PESERTA", jika sudah ada dan BELUM bayar</t>
+  </si>
+  <si>
+    <t>BMT</t>
+  </si>
+  <si>
+    <t>JUMLAH TAGIHAN</t>
+  </si>
+  <si>
+    <t>PEMBAYARAN TRANSFER</t>
+  </si>
+  <si>
+    <t>DATA BASE : "DAFTAR PESERTA"</t>
+  </si>
+  <si>
+    <t>SUDAH</t>
+  </si>
+  <si>
+    <t>Pembayaran Iuran</t>
+  </si>
+  <si>
+    <t>saldo-100.000</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1150,7 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1316,62 +1346,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1385,10 +1379,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1397,9 +1421,22 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="41" fontId="5" fillId="2" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -1552,8 +1589,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12782550" y="4067175"/>
-          <a:ext cx="2415556" cy="1876284"/>
+          <a:off x="12792075" y="4064794"/>
+          <a:ext cx="2410794" cy="1881046"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -1792,8 +1829,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12787993" y="10846253"/>
-          <a:ext cx="2415556" cy="1880366"/>
+          <a:off x="12797518" y="10853397"/>
+          <a:ext cx="2410794" cy="1882747"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -2084,8 +2121,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>625475</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>18256</xdr:colOff>
       <xdr:row>96</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
@@ -2151,8 +2188,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8362950" y="19878675"/>
-          <a:ext cx="10953750" cy="1889891"/>
+          <a:off x="8382000" y="19895344"/>
+          <a:ext cx="8882063" cy="1894653"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -2316,15 +2353,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>113</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1321594</xdr:colOff>
+      <xdr:row>123</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2341,14 +2378,88 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="22939375"/>
-          <a:ext cx="6048375" cy="2095500"/>
+          <a:off x="1" y="22848094"/>
+          <a:ext cx="6012656" cy="2095500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>120</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Rounded Rectangle 19"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5419725" y="13649325"/>
+          <a:ext cx="1476375" cy="200025"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="165100" prst="coolSlant"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>BAYAR</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3057,34 +3168,34 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="93" t="s">
+      <c r="B6" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="95" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="59"/>
-      <c r="F6" s="93" t="s">
+      <c r="F6" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="93" t="s">
+      <c r="G6" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="93" t="s">
+      <c r="H6" s="95" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="96"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="96"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="66">
@@ -3232,13 +3343,13 @@
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="96" t="s">
+      <c r="F17" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="96" t="s">
+      <c r="G17" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="96" t="s">
+      <c r="H17" s="93" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3251,9 +3362,9 @@
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95"/>
-      <c r="H18" s="95"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="66">
@@ -3639,13 +3750,13 @@
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="93" t="s">
+      <c r="B42" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="93" t="s">
+      <c r="C42" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="93" t="s">
+      <c r="D42" s="95" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="71"/>
@@ -3654,9 +3765,9 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="95"/>
-      <c r="C43" s="95"/>
-      <c r="D43" s="95"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="94"/>
+      <c r="D43" s="94"/>
       <c r="E43" s="71"/>
       <c r="F43" s="69"/>
       <c r="G43" s="70"/>
@@ -4016,18 +4127,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D43"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4097,48 +4208,48 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="101" t="s">
+      <c r="C8" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="93" t="s">
+      <c r="D8" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="93" t="s">
+      <c r="E8" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="106" t="s">
+      <c r="F8" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="93" t="s">
+      <c r="G8" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="93" t="s">
+      <c r="H8" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="93" t="s">
+      <c r="I8" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="93" t="s">
+      <c r="J8" s="95" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="93" t="s">
+      <c r="K8" s="95" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="105"/>
+      <c r="L8" s="111"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="102"/>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="107"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="105"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="110"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="111"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
@@ -4213,50 +4324,50 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="101" t="s">
+      <c r="C15" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="93" t="s">
+      <c r="E15" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="93" t="s">
+      <c r="F15" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="93" t="s">
+      <c r="G15" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="93" t="s">
+      <c r="H15" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="97" t="s">
+      <c r="I15" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="103" t="s">
+      <c r="J15" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
-      <c r="M15" s="105"/>
-      <c r="N15" s="105"/>
-      <c r="O15" s="105"/>
+      <c r="K15" s="111"/>
+      <c r="L15" s="111"/>
+      <c r="M15" s="111"/>
+      <c r="N15" s="111"/>
+      <c r="O15" s="111"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="102"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="94"/>
-      <c r="H16" s="94"/>
-      <c r="I16" s="98"/>
-      <c r="J16" s="104"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
-      <c r="M16" s="105"/>
-      <c r="N16" s="105"/>
-      <c r="O16" s="105"/>
+      <c r="C16" s="108"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+      <c r="I16" s="99"/>
+      <c r="J16" s="113"/>
+      <c r="K16" s="111"/>
+      <c r="L16" s="111"/>
+      <c r="M16" s="111"/>
+      <c r="N16" s="111"/>
+      <c r="O16" s="111"/>
     </row>
     <row r="17" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="45" t="s">
@@ -4340,76 +4451,76 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="93" t="s">
+      <c r="C22" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="101" t="s">
+      <c r="D22" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="93" t="s">
+      <c r="E22" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="93" t="s">
+      <c r="F22" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="93" t="s">
+      <c r="G22" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="93" t="s">
+      <c r="H22" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="93" t="s">
+      <c r="I22" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="97" t="s">
+      <c r="J22" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="103" t="s">
+      <c r="K22" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="93" t="s">
+      <c r="L22" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="93" t="s">
+      <c r="M22" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="97" t="s">
+      <c r="N22" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="97" t="s">
+      <c r="O22" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="93" t="s">
+      <c r="P22" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="97" t="s">
+      <c r="Q22" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="R22" s="97" t="s">
+      <c r="R22" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="93" t="s">
+      <c r="S22" s="95" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="94"/>
-      <c r="D23" s="102"/>
-      <c r="E23" s="94"/>
-      <c r="F23" s="94"/>
-      <c r="G23" s="94"/>
-      <c r="H23" s="94"/>
-      <c r="I23" s="94"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="104"/>
-      <c r="L23" s="94"/>
-      <c r="M23" s="94"/>
-      <c r="N23" s="98"/>
-      <c r="O23" s="98"/>
-      <c r="P23" s="94"/>
-      <c r="Q23" s="98"/>
-      <c r="R23" s="98"/>
-      <c r="S23" s="94"/>
+      <c r="C23" s="96"/>
+      <c r="D23" s="108"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="96"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="96"/>
+      <c r="I23" s="96"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="96"/>
+      <c r="M23" s="96"/>
+      <c r="N23" s="99"/>
+      <c r="O23" s="99"/>
+      <c r="P23" s="96"/>
+      <c r="Q23" s="99"/>
+      <c r="R23" s="99"/>
+      <c r="S23" s="96"/>
     </row>
     <row r="24" spans="3:19" s="48" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C24" s="45" t="s">
@@ -4519,72 +4630,72 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="93" t="s">
+      <c r="C29" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="101" t="s">
+      <c r="D29" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="93" t="s">
+      <c r="E29" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="93" t="s">
+      <c r="F29" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="103" t="s">
+      <c r="G29" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="93" t="s">
+      <c r="H29" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="93" t="s">
+      <c r="I29" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="97" t="s">
+      <c r="J29" s="98" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="97" t="s">
+      <c r="K29" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="93" t="s">
+      <c r="L29" s="95" t="s">
         <v>6</v>
       </c>
-      <c r="M29" s="97" t="s">
+      <c r="M29" s="98" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="97" t="s">
+      <c r="N29" s="98" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="93" t="s">
+      <c r="O29" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="P29" s="93" t="s">
+      <c r="P29" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="93" t="s">
+      <c r="Q29" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="93" t="s">
+      <c r="R29" s="95" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="94"/>
-      <c r="D30" s="102"/>
-      <c r="E30" s="94"/>
-      <c r="F30" s="94"/>
-      <c r="G30" s="104"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="94"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="98"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="98"/>
-      <c r="N30" s="98"/>
-      <c r="O30" s="94"/>
-      <c r="P30" s="94"/>
-      <c r="Q30" s="94"/>
-      <c r="R30" s="94"/>
+      <c r="C30" s="96"/>
+      <c r="D30" s="108"/>
+      <c r="E30" s="96"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="96"/>
+      <c r="I30" s="96"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="99"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="99"/>
+      <c r="N30" s="99"/>
+      <c r="O30" s="96"/>
+      <c r="P30" s="96"/>
+      <c r="Q30" s="96"/>
+      <c r="R30" s="96"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="45" t="s">
@@ -4687,13 +4798,13 @@
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="93" t="s">
+      <c r="C36" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="93" t="s">
+      <c r="D36" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="93" t="s">
+      <c r="E36" s="95" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="12"/>
@@ -4704,9 +4815,9 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="94"/>
-      <c r="D37" s="94"/>
-      <c r="E37" s="94"/>
+      <c r="C37" s="96"/>
+      <c r="D37" s="96"/>
+      <c r="E37" s="96"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -4784,19 +4895,19 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="93" t="s">
+      <c r="C44" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="93" t="s">
+      <c r="D44" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="93" t="s">
+      <c r="E44" s="95" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="97" t="s">
+      <c r="F44" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="99" t="s">
+      <c r="G44" s="114" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="4"/>
@@ -4806,11 +4917,11 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="94"/>
-      <c r="D45" s="94"/>
-      <c r="E45" s="94"/>
-      <c r="F45" s="98"/>
-      <c r="G45" s="100"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="96"/>
+      <c r="F45" s="99"/>
+      <c r="G45" s="115"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -4855,28 +4966,28 @@
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="93" t="s">
+      <c r="C52" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="93" t="s">
+      <c r="D52" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="93" t="s">
+      <c r="E52" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="93" t="s">
+      <c r="F52" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="93" t="s">
+      <c r="G52" s="95" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="94"/>
-      <c r="D53" s="94"/>
-      <c r="E53" s="94"/>
-      <c r="F53" s="94"/>
-      <c r="G53" s="94"/>
+      <c r="C53" s="96"/>
+      <c r="D53" s="96"/>
+      <c r="E53" s="96"/>
+      <c r="F53" s="96"/>
+      <c r="G53" s="96"/>
     </row>
     <row r="54" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -4914,30 +5025,30 @@
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="97" t="s">
+      <c r="C59" s="98" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="109"/>
-      <c r="E59" s="93" t="s">
+      <c r="D59" s="105"/>
+      <c r="E59" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="97" t="s">
+      <c r="F59" s="98" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="108"/>
+      <c r="G59" s="104"/>
     </row>
     <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="108"/>
-      <c r="D60" s="110"/>
-      <c r="E60" s="95"/>
-      <c r="F60" s="98"/>
-      <c r="G60" s="108"/>
+      <c r="C60" s="104"/>
+      <c r="D60" s="106"/>
+      <c r="E60" s="94"/>
+      <c r="F60" s="99"/>
+      <c r="G60" s="104"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="112" t="s">
+      <c r="C61" s="100" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="113"/>
+      <c r="D61" s="101"/>
       <c r="E61" s="1" t="s">
         <v>98</v>
       </c>
@@ -4946,14 +5057,14 @@
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="114"/>
-      <c r="D62" s="115"/>
+      <c r="C62" s="102"/>
+      <c r="D62" s="103"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="111"/>
-      <c r="D63" s="111"/>
+      <c r="C63" s="97"/>
+      <c r="D63" s="97"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="4"/>
@@ -4964,82 +5075,30 @@
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="111" t="s">
+      <c r="C65" s="97" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="111"/>
+      <c r="D65" s="97"/>
       <c r="E65" s="49">
         <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="111" t="s">
+      <c r="C66" s="97" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="111"/>
+      <c r="D66" s="97"/>
       <c r="E66" s="49">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="C59:D60"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
     <mergeCell ref="R29:R30"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
@@ -5056,11 +5115,63 @@
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="C59:D60"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -5069,10 +5180,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X130"/>
+  <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F79" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L84" sqref="L84"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:XFD128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5088,23 +5199,24 @@
     <col min="9" max="9" width="20.5703125" style="75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="27" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
     <col min="18" max="18" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="72" t="s">
@@ -5269,46 +5381,46 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="93" t="s">
+      <c r="A16" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="97" t="s">
+      <c r="B16" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="109"/>
-      <c r="D16" s="93" t="s">
+      <c r="C16" s="105"/>
+      <c r="D16" s="95" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="93" t="s">
+      <c r="E16" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="93" t="s">
+      <c r="F16" s="95" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="93" t="s">
+      <c r="G16" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="93" t="s">
+      <c r="H16" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="118" t="s">
+      <c r="I16" s="116" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="93" t="s">
+      <c r="J16" s="95" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="94"/>
-      <c r="B17" s="98"/>
-      <c r="C17" s="117"/>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="94"/>
-      <c r="G17" s="94"/>
-      <c r="H17" s="94"/>
-      <c r="I17" s="119"/>
-      <c r="J17" s="94"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="119"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="96"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+      <c r="I17" s="117"/>
+      <c r="J17" s="96"/>
     </row>
     <row r="18" spans="1:10" s="57" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52">
@@ -5350,8 +5462,8 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="115"/>
+      <c r="B19" s="102"/>
+      <c r="C19" s="103"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -5669,40 +5781,40 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="101" t="s">
+      <c r="A51" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="93" t="s">
+      <c r="B51" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="93" t="s">
+      <c r="C51" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="93" t="s">
+      <c r="D51" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="93" t="s">
+      <c r="E51" s="95" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="93" t="s">
+      <c r="F51" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="97" t="s">
+      <c r="G51" s="98" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="103" t="s">
+      <c r="H51" s="112" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="102"/>
-      <c r="B52" s="94"/>
-      <c r="C52" s="94"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="94"/>
-      <c r="F52" s="94"/>
-      <c r="G52" s="98"/>
-      <c r="H52" s="104"/>
+      <c r="A52" s="108"/>
+      <c r="B52" s="96"/>
+      <c r="C52" s="96"/>
+      <c r="D52" s="96"/>
+      <c r="E52" s="96"/>
+      <c r="F52" s="96"/>
+      <c r="G52" s="99"/>
+      <c r="H52" s="113"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A53" s="82" t="s">
@@ -6754,16 +6866,21 @@
       <c r="W113" s="75"/>
       <c r="X113" s="75"/>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="75"/>
       <c r="B114" s="75"/>
       <c r="C114" s="75"/>
       <c r="D114" s="75"/>
-      <c r="E114" s="75"/>
-      <c r="F114" s="75"/>
-      <c r="G114" s="75"/>
-      <c r="H114" s="75"/>
-      <c r="J114" s="75"/>
+      <c r="E114" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="F114" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="G114" s="19"/>
+      <c r="H114" s="19"/>
+      <c r="I114" s="13"/>
+      <c r="J114" s="13"/>
       <c r="K114" s="75"/>
       <c r="L114" s="75"/>
       <c r="M114" s="75"/>
@@ -6779,16 +6896,25 @@
       <c r="W114" s="75"/>
       <c r="X114" s="75"/>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="75"/>
       <c r="B115" s="75"/>
       <c r="C115" s="75"/>
       <c r="D115" s="75"/>
-      <c r="E115" s="75"/>
-      <c r="F115" s="75"/>
-      <c r="G115" s="75"/>
-      <c r="H115" s="75"/>
-      <c r="J115" s="75"/>
+      <c r="E115" s="23"/>
+      <c r="F115" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G115" s="24"/>
+      <c r="H115" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="I115" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="J115" s="25" t="s">
+        <v>207</v>
+      </c>
       <c r="K115" s="75"/>
       <c r="L115" s="75"/>
       <c r="M115" s="75"/>
@@ -6809,11 +6935,18 @@
       <c r="B116" s="75"/>
       <c r="C116" s="75"/>
       <c r="D116" s="75"/>
-      <c r="E116" s="75"/>
-      <c r="F116" s="75"/>
-      <c r="G116" s="75"/>
-      <c r="H116" s="75"/>
-      <c r="J116" s="75"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I116" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J116" s="16"/>
       <c r="K116" s="75"/>
       <c r="L116" s="75"/>
       <c r="M116" s="75"/>
@@ -6834,11 +6967,18 @@
       <c r="B117" s="75"/>
       <c r="C117" s="75"/>
       <c r="D117" s="75"/>
-      <c r="E117" s="75"/>
-      <c r="F117" s="75"/>
-      <c r="G117" s="75"/>
-      <c r="H117" s="75"/>
-      <c r="J117" s="75"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I117" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="J117" s="14"/>
       <c r="K117" s="75"/>
       <c r="L117" s="75"/>
       <c r="M117" s="75"/>
@@ -6859,11 +6999,18 @@
       <c r="B118" s="75"/>
       <c r="C118" s="75"/>
       <c r="D118" s="75"/>
-      <c r="E118" s="75"/>
-      <c r="F118" s="75"/>
-      <c r="G118" s="75"/>
-      <c r="H118" s="75"/>
-      <c r="J118" s="75"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G118" s="14"/>
+      <c r="H118" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I118" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="J118" s="14"/>
       <c r="K118" s="75"/>
       <c r="L118" s="75"/>
       <c r="M118" s="75"/>
@@ -6884,11 +7031,16 @@
       <c r="B119" s="75"/>
       <c r="C119" s="75"/>
       <c r="D119" s="75"/>
-      <c r="E119" s="75"/>
-      <c r="F119" s="75"/>
-      <c r="G119" s="75"/>
-      <c r="H119" s="75"/>
-      <c r="J119" s="75"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="G119" s="14"/>
+      <c r="H119" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I119" s="14"/>
+      <c r="J119" s="14"/>
       <c r="K119" s="75"/>
       <c r="L119" s="75"/>
       <c r="M119" s="75"/>
@@ -6909,11 +7061,19 @@
       <c r="B120" s="75"/>
       <c r="C120" s="75"/>
       <c r="D120" s="75"/>
-      <c r="E120" s="75"/>
-      <c r="F120" s="75"/>
-      <c r="G120" s="75"/>
-      <c r="H120" s="75"/>
-      <c r="J120" s="75"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I120" s="121">
+        <f>+K100</f>
+        <v>0</v>
+      </c>
+      <c r="J120" s="14"/>
       <c r="K120" s="75"/>
       <c r="L120" s="75"/>
       <c r="M120" s="75"/>
@@ -6934,11 +7094,18 @@
       <c r="B121" s="75"/>
       <c r="C121" s="75"/>
       <c r="D121" s="75"/>
-      <c r="E121" s="75"/>
-      <c r="F121" s="75"/>
-      <c r="G121" s="75"/>
-      <c r="H121" s="75"/>
-      <c r="J121" s="75"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="I121" s="121"/>
+      <c r="J121" s="32" t="s">
+        <v>10</v>
+      </c>
       <c r="K121" s="75"/>
       <c r="L121" s="75"/>
       <c r="M121" s="75"/>
@@ -7055,7 +7222,9 @@
       <c r="X125" s="75"/>
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A126" s="75"/>
+      <c r="A126" s="122" t="s">
+        <v>211</v>
+      </c>
       <c r="B126" s="75"/>
       <c r="C126" s="75"/>
       <c r="D126" s="75"/>
@@ -7079,55 +7248,127 @@
       <c r="W126" s="75"/>
       <c r="X126" s="75"/>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A127" s="75"/>
-      <c r="B127" s="75"/>
-      <c r="C127" s="75"/>
-      <c r="D127" s="75"/>
-      <c r="E127" s="75"/>
-      <c r="F127" s="75"/>
-      <c r="G127" s="75"/>
-      <c r="H127" s="75"/>
-      <c r="J127" s="75"/>
-      <c r="K127" s="75"/>
-      <c r="L127" s="75"/>
-      <c r="M127" s="75"/>
-      <c r="N127" s="75"/>
-      <c r="O127" s="75"/>
-      <c r="P127" s="75"/>
-      <c r="Q127" s="75"/>
-      <c r="R127" s="75"/>
-      <c r="S127" s="75"/>
+    <row r="127" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="90" t="s">
+        <v>4</v>
+      </c>
+      <c r="B127" s="90" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127" s="90" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127" s="90" t="s">
+        <v>2</v>
+      </c>
+      <c r="E127" s="90" t="s">
+        <v>28</v>
+      </c>
+      <c r="F127" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="G127" s="90" t="s">
+        <v>27</v>
+      </c>
+      <c r="H127" s="90" t="s">
+        <v>30</v>
+      </c>
+      <c r="I127" s="90" t="s">
+        <v>16</v>
+      </c>
+      <c r="J127" s="90" t="s">
+        <v>0</v>
+      </c>
+      <c r="K127" s="90" t="s">
+        <v>5</v>
+      </c>
+      <c r="L127" s="90" t="s">
+        <v>22</v>
+      </c>
+      <c r="M127" s="90" t="s">
+        <v>6</v>
+      </c>
+      <c r="N127" s="90" t="s">
+        <v>23</v>
+      </c>
+      <c r="O127" s="90" t="s">
+        <v>24</v>
+      </c>
+      <c r="P127" s="90" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q127" s="90" t="s">
+        <v>25</v>
+      </c>
+      <c r="R127" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="S127" s="90"/>
       <c r="T127" s="75"/>
       <c r="U127" s="75"/>
       <c r="V127" s="75"/>
       <c r="W127" s="75"/>
-      <c r="X127" s="75"/>
-    </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A128" s="75"/>
-      <c r="B128" s="75"/>
-      <c r="C128" s="75"/>
-      <c r="D128" s="75"/>
-      <c r="E128" s="75"/>
-      <c r="F128" s="75"/>
-      <c r="G128" s="75"/>
-      <c r="H128" s="75"/>
-      <c r="J128" s="75"/>
-      <c r="K128" s="75"/>
-      <c r="L128" s="75"/>
-      <c r="M128" s="75"/>
-      <c r="N128" s="75"/>
-      <c r="O128" s="75"/>
-      <c r="P128" s="75"/>
-      <c r="Q128" s="75"/>
-      <c r="R128" s="75"/>
-      <c r="S128" s="75"/>
-      <c r="T128" s="75"/>
-      <c r="U128" s="75"/>
-      <c r="V128" s="75"/>
-      <c r="W128" s="75"/>
-      <c r="X128" s="75"/>
+    </row>
+    <row r="128" spans="1:24" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="123" t="s">
+        <v>57</v>
+      </c>
+      <c r="B128" s="123" t="s">
+        <v>48</v>
+      </c>
+      <c r="C128" s="123" t="s">
+        <v>53</v>
+      </c>
+      <c r="D128" s="123" t="s">
+        <v>54</v>
+      </c>
+      <c r="E128" s="123" t="s">
+        <v>50</v>
+      </c>
+      <c r="F128" s="124">
+        <v>27419</v>
+      </c>
+      <c r="G128" s="123" t="s">
+        <v>55</v>
+      </c>
+      <c r="H128" s="123" t="s">
+        <v>56</v>
+      </c>
+      <c r="I128" s="123" t="s">
+        <v>73</v>
+      </c>
+      <c r="J128" s="123" t="s">
+        <v>58</v>
+      </c>
+      <c r="K128" s="123">
+        <v>20000000</v>
+      </c>
+      <c r="L128" s="124">
+        <v>42449</v>
+      </c>
+      <c r="M128" s="123">
+        <v>12</v>
+      </c>
+      <c r="N128" s="124">
+        <v>42809</v>
+      </c>
+      <c r="O128" s="123">
+        <v>40000</v>
+      </c>
+      <c r="P128" s="123">
+        <v>60000</v>
+      </c>
+      <c r="Q128" s="123">
+        <v>100000</v>
+      </c>
+      <c r="R128" s="126" t="s">
+        <v>212</v>
+      </c>
+      <c r="S128" s="127"/>
+      <c r="T128" s="125"/>
+      <c r="U128" s="125"/>
+      <c r="V128" s="125"/>
+      <c r="W128" s="125"/>
     </row>
     <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="75"/>
@@ -7154,44 +7395,114 @@
       <c r="W129" s="75"/>
       <c r="X129" s="75"/>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A130" s="75"/>
-      <c r="B130" s="75"/>
-      <c r="C130" s="75"/>
-      <c r="D130" s="75"/>
-      <c r="E130" s="75"/>
-      <c r="F130" s="75"/>
-      <c r="G130" s="75"/>
-      <c r="H130" s="75"/>
-      <c r="J130" s="75"/>
-      <c r="K130" s="75"/>
-      <c r="L130" s="75"/>
-      <c r="M130" s="75"/>
-      <c r="N130" s="75"/>
-      <c r="O130" s="75"/>
-      <c r="P130" s="75"/>
-      <c r="Q130" s="75"/>
-      <c r="R130" s="75"/>
-      <c r="S130" s="75"/>
-      <c r="T130" s="75"/>
-      <c r="U130" s="75"/>
-      <c r="V130" s="75"/>
-      <c r="W130" s="75"/>
-      <c r="X130" s="75"/>
+    <row r="132" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A132" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A133" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H133" s="75"/>
+      <c r="I133"/>
+    </row>
+    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B134" s="1">
+        <v>111001</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E134" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H134" s="75"/>
+      <c r="I134"/>
+    </row>
+    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="1">
+        <v>114001</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E135" s="1">
+        <v>100000</v>
+      </c>
+      <c r="H135" s="75"/>
+      <c r="I135"/>
+    </row>
+    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A138" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H139" s="75"/>
+      <c r="I139"/>
+    </row>
+    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>111001</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C140" s="1"/>
+      <c r="D140" t="s">
+        <v>200</v>
+      </c>
+      <c r="H140" s="75"/>
+      <c r="I140"/>
+    </row>
+    <row r="141" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>114001</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C141" s="1"/>
+      <c r="D141" t="s">
+        <v>214</v>
+      </c>
+      <c r="H141" s="75"/>
+      <c r="I141"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
@@ -7200,6 +7511,17 @@
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7241,12 +7563,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="118" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="116"/>
-      <c r="C1" s="116"/>
-      <c r="D1" s="116"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J14" s="20"/>

</xml_diff>

<commit_message>
tes koneksi sql server-percobaan ke2
</commit_message>
<xml_diff>
--- a/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
+++ b/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="COA" sheetId="13" r:id="rId1"/>
     <sheet name="DATABASE" sheetId="5" r:id="rId2"/>
     <sheet name="Menu Transaksi" sheetId="11" r:id="rId3"/>
-    <sheet name="Menu Properti" sheetId="14" r:id="rId4"/>
-    <sheet name="Menu Informasi" sheetId="9" r:id="rId5"/>
+    <sheet name="Menu Informasi" sheetId="9" r:id="rId4"/>
+    <sheet name="Menu Properti" sheetId="14" r:id="rId5"/>
     <sheet name="Menu Cetak" sheetId="10" r:id="rId6"/>
     <sheet name="Menu Administrasi" sheetId="12" r:id="rId7"/>
   </sheets>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="212">
   <si>
     <t>REKENING</t>
   </si>
@@ -270,18 +270,12 @@
     <t>PENDAFTARAN PESERTA</t>
   </si>
   <si>
-    <t>INFORMASI PESERTA TAAWUN</t>
-  </si>
-  <si>
     <t>PER BMT</t>
   </si>
   <si>
     <t>BAYAR</t>
   </si>
   <si>
-    <t>(filter berdasar kode BMT dan tanggal jatuh tempo &gt; tanggal sekarang)</t>
-  </si>
-  <si>
     <t>Nama BMT</t>
   </si>
   <si>
@@ -340,9 +334,6 @@
   </si>
   <si>
     <t>Proses Menu Informasi</t>
-  </si>
-  <si>
-    <t>Tampilkan : kolom2 di tabel aplikasi sesuai dengan kolom di bawah ini.</t>
   </si>
   <si>
     <t>Tampilkan :kolom2 di tabel aplikasi sesuai dengan kolom di bawah ini.</t>
@@ -1346,6 +1337,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="5" fillId="2" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1430,13 +1428,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="5" fillId="2" borderId="14" xfId="4" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
@@ -1589,8 +1580,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12792075" y="4064794"/>
-          <a:ext cx="2410794" cy="1881046"/>
+          <a:off x="12786783" y="4066117"/>
+          <a:ext cx="2418731" cy="1878400"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -1829,8 +1820,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12797518" y="10853397"/>
-          <a:ext cx="2410794" cy="1882747"/>
+          <a:off x="12792226" y="10849428"/>
+          <a:ext cx="2418731" cy="1881424"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -2188,8 +2179,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8382000" y="19895344"/>
-          <a:ext cx="8882063" cy="1894653"/>
+          <a:off x="8360833" y="19886083"/>
+          <a:ext cx="8905875" cy="1892008"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -2462,99 +2453,264 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>202407</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>190498</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>381001</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>154779</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7774782" y="26122311"/>
+          <a:ext cx="8882063" cy="3202781"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:scene3d>
+          <a:camera prst="orthographicFront">
+            <a:rot lat="0" lon="0" rev="0"/>
+          </a:camera>
+          <a:lightRig rig="contrasting" dir="t">
+            <a:rot lat="0" lon="0" rev="1200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d contourW="19050" prstMaterial="metal">
+          <a:bevelT w="88900" h="203200"/>
+          <a:bevelB w="165100" h="254000"/>
+        </a:sp3d>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent2">
+            <a:tint val="40000"/>
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2">
+            <a:tint val="40000"/>
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2">
+            <a:tint val="40000"/>
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>&gt; </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>pembayaran iuran ini merupakan kelanjutan proses setelah pendaftaran peserta. Pada pembayaran iuran ini setelah mengisi KTP di dapatkan data  pendaftaran peserta,  setelah ketemu datanya isi ke Nama, BMT dan jumlah Tagihan, untuk tanggal di default hari ini, jadi pembayaran ini akan menampilkan berapa jumlah tagihan dari peserta BMT Tersebut, user nantinya mengisi pembayaran, data di simpan di dalam Tabel Jurnal.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:hueOff val="0"/>
+                <a:satOff val="0"/>
+                <a:lumOff val="0"/>
+                <a:alphaOff val="0"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>tanggal akan terisi tanggal pembayaran, nomor rekening  diambil dari tabel peserta BMT. D/K sedang  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>di</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>tanyakan ke client, jumlah adalah berapa banyak pembayaranya.</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>setelah tabel jurnal terisi proses berikutnya mengisi Tabel Buku Besar.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>22933</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="266701"/>
-          <a:ext cx="4899733" cy="2038350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>19051</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>122505</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1" y="2552700"/>
-          <a:ext cx="4895850" cy="2237055"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>266698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>160467</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104664</xdr:rowOff>
+      <xdr:colOff>112842</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -2563,10 +2719,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5486400" y="266700"/>
-          <a:ext cx="3246567" cy="1819164"/>
-          <a:chOff x="2207012" y="565128"/>
-          <a:chExt cx="1989267" cy="1819164"/>
+          <a:off x="5486400" y="266698"/>
+          <a:ext cx="3246567" cy="3000377"/>
+          <a:chOff x="2207012" y="565126"/>
+          <a:chExt cx="1989267" cy="3000377"/>
         </a:xfrm>
         <a:scene3d>
           <a:camera prst="orthographicFront">
@@ -2584,8 +2740,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2207012" y="565128"/>
-            <a:ext cx="1989267" cy="1819164"/>
+            <a:off x="2207012" y="565127"/>
+            <a:ext cx="1989267" cy="3000376"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2643,8 +2799,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="2207012" y="565128"/>
-            <a:ext cx="1989267" cy="1819164"/>
+            <a:off x="2207012" y="565126"/>
+            <a:ext cx="1989267" cy="2952751"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -2694,9 +2850,336 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" sz="1300" kern="1200" baseline="0"/>
-              <a:t> menu informasi peserta dan tagihan, ditampilkan ke dalam tabel aplikasi dengan menarik data dari beberapa tabel di DB.(Join table query)</a:t>
+              <a:t> menu informasi peserta dan tagihan, ditampilkan ke dalam tabel aplikasi dengan menarik data dari beberapa tabel di DB.(Join table query) tampilan tabel aplikasi nya berubah sesuai data yg ditarik.</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1300" kern="1200"/>
+          </a:p>
+          <a:p>
+            <a:pPr lvl="0"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>&gt;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Filter “Data Peserta” </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+                <a:sym typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+              </a:rPr>
+              <a:t></a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> NoKTP, Nama, Alamat, Lokasi Usaha, Jenis Usaha.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr lvl="0"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>&gt;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Filter “Rekening” </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+                <a:sym typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+              </a:rPr>
+              <a:t></a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> Nama,NomorBMT, Rekening.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr lvl="0"/>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>&gt;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Filter “Pembiayaan” </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+                <a:sym typeface="Wingdings" panose="05000000000000000000" pitchFamily="2" charset="2"/>
+              </a:rPr>
+              <a:t></a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> Nama,TglAkad,JangkaWaktu,JatuhTempo,JumlahPembiayaan,IuranKebakaran,Iuran</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1400">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Jiwa, Jumlah Iuran, Status(bayar/Belum)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="1400">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:r>
+              <a:rPr lang="id-ID" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t/>
+            </a:r>
+            <a:br>
+              <a:rPr lang="id-ID" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:hueOff val="0"/>
+                    <a:satOff val="0"/>
+                    <a:lumOff val="0"/>
+                    <a:alphaOff val="0"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+            </a:br>
+            <a:endParaRPr lang="en-US" sz="1200" kern="1200"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -2707,87 +3190,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>105642</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>866</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rounded Rectangle 6"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2552700" y="19840575"/>
-          <a:ext cx="1410567" cy="200891"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx2">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="threePt" dir="t"/>
-        </a:scene3d>
-        <a:sp3d>
-          <a:bevelT w="165100" prst="coolSlant"/>
-        </a:sp3d>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="id-ID" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>NAMA BMT</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>105642</xdr:colOff>
-      <xdr:row>26</xdr:row>
       <xdr:rowOff>866</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2849,6 +3258,61 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>144886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1" y="266700"/>
+          <a:ext cx="4895850" cy="3002386"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3143,8 +3607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3158,51 +3622,51 @@
   <sheetData>
     <row r="3" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="64" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="65" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="95" t="s">
+      <c r="C6" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="95" t="s">
+      <c r="D6" s="102" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="59"/>
-      <c r="F6" s="95" t="s">
+      <c r="F6" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="G6" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="H6" s="102" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="96"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="103"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="96"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="66">
         <v>110001</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D8" s="68"/>
       <c r="E8" s="11"/>
@@ -3210,7 +3674,7 @@
         <v>650001</v>
       </c>
       <c r="G8" s="67" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="H8" s="68"/>
     </row>
@@ -3219,7 +3683,7 @@
         <v>110002</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D9" s="68"/>
       <c r="E9" s="4"/>
@@ -3227,7 +3691,7 @@
         <v>650002</v>
       </c>
       <c r="G9" s="67" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H9" s="68"/>
     </row>
@@ -3236,7 +3700,7 @@
         <v>111001</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D10" s="68"/>
       <c r="E10" s="4"/>
@@ -3244,7 +3708,7 @@
         <v>651001</v>
       </c>
       <c r="G10" s="67" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H10" s="68"/>
     </row>
@@ -3253,7 +3717,7 @@
         <v>111002</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D11" s="68"/>
       <c r="E11" s="4"/>
@@ -3261,7 +3725,7 @@
         <v>651002</v>
       </c>
       <c r="G11" s="67" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H11" s="68"/>
     </row>
@@ -3270,7 +3734,7 @@
         <v>111003</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D12" s="68"/>
       <c r="E12" s="4"/>
@@ -3278,7 +3742,7 @@
         <v>652001</v>
       </c>
       <c r="G12" s="67" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H12" s="29"/>
     </row>
@@ -3287,7 +3751,7 @@
         <v>111888</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D13" s="68"/>
       <c r="E13" s="4"/>
@@ -3300,7 +3764,7 @@
         <v>111999</v>
       </c>
       <c r="C14" s="67" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D14" s="68"/>
       <c r="E14" s="4"/>
@@ -3313,7 +3777,7 @@
         <v>112001</v>
       </c>
       <c r="C15" s="67" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D15" s="68"/>
       <c r="E15" s="4"/>
@@ -3326,7 +3790,7 @@
         <v>112002</v>
       </c>
       <c r="C16" s="67" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D16" s="68"/>
       <c r="E16" s="4"/>
@@ -3339,17 +3803,17 @@
         <v>112999</v>
       </c>
       <c r="C17" s="67" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="93" t="s">
+      <c r="F17" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="93" t="s">
+      <c r="G17" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="93" t="s">
+      <c r="H17" s="100" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3358,20 +3822,20 @@
         <v>113001</v>
       </c>
       <c r="C18" s="67" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="94"/>
-      <c r="H18" s="94"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="101"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="66">
         <v>113002</v>
       </c>
       <c r="C19" s="67" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="4"/>
@@ -3379,7 +3843,7 @@
         <v>770001</v>
       </c>
       <c r="G19" s="67" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -3388,7 +3852,7 @@
         <v>113999</v>
       </c>
       <c r="C20" s="67" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="4"/>
@@ -3396,7 +3860,7 @@
         <v>771001</v>
       </c>
       <c r="G20" s="67" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -3405,7 +3869,7 @@
         <v>114001</v>
       </c>
       <c r="C21" s="67" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="4"/>
@@ -3413,7 +3877,7 @@
         <v>772001</v>
       </c>
       <c r="G21" s="67" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H21" s="68"/>
     </row>
@@ -3422,7 +3886,7 @@
         <v>114002</v>
       </c>
       <c r="C22" s="67" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D22" s="29"/>
       <c r="E22" s="4"/>
@@ -3430,7 +3894,7 @@
         <v>772002</v>
       </c>
       <c r="G22" s="67" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H22" s="68"/>
     </row>
@@ -3439,7 +3903,7 @@
         <v>114999</v>
       </c>
       <c r="C23" s="67" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="4"/>
@@ -3447,7 +3911,7 @@
         <v>772003</v>
       </c>
       <c r="G23" s="67" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H23" s="68"/>
     </row>
@@ -3456,7 +3920,7 @@
         <v>115001</v>
       </c>
       <c r="C24" s="67" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="4"/>
@@ -3464,7 +3928,7 @@
         <v>772004</v>
       </c>
       <c r="G24" s="67" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="H24" s="68"/>
     </row>
@@ -3473,7 +3937,7 @@
         <v>116001</v>
       </c>
       <c r="C25" s="67" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="4"/>
@@ -3481,7 +3945,7 @@
         <v>772005</v>
       </c>
       <c r="G25" s="67" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="H25" s="68"/>
     </row>
@@ -3490,7 +3954,7 @@
         <v>117001</v>
       </c>
       <c r="C26" s="67" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D26" s="29"/>
       <c r="E26" s="4"/>
@@ -3498,7 +3962,7 @@
         <v>773001</v>
       </c>
       <c r="G26" s="67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="H26" s="68"/>
     </row>
@@ -3507,7 +3971,7 @@
         <v>117002</v>
       </c>
       <c r="C27" s="67" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D27" s="29"/>
       <c r="E27" s="4"/>
@@ -3515,7 +3979,7 @@
         <v>773001</v>
       </c>
       <c r="G27" s="67" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="H27" s="68"/>
     </row>
@@ -3524,7 +3988,7 @@
         <v>117003</v>
       </c>
       <c r="C28" s="67" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="4"/>
@@ -3532,7 +3996,7 @@
         <v>774008</v>
       </c>
       <c r="G28" s="67" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H28" s="68"/>
     </row>
@@ -3541,7 +4005,7 @@
         <v>117004</v>
       </c>
       <c r="C29" s="67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="4"/>
@@ -3549,7 +4013,7 @@
         <v>775001</v>
       </c>
       <c r="G29" s="67" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="H29" s="68"/>
     </row>
@@ -3558,7 +4022,7 @@
         <v>117888</v>
       </c>
       <c r="C30" s="67" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D30" s="29"/>
       <c r="E30" s="4"/>
@@ -3566,7 +4030,7 @@
         <v>775002</v>
       </c>
       <c r="G30" s="67" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H30" s="68"/>
     </row>
@@ -3575,7 +4039,7 @@
         <v>118001</v>
       </c>
       <c r="C31" s="67" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="4"/>
@@ -3583,7 +4047,7 @@
         <v>776001</v>
       </c>
       <c r="G31" s="67" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="H31" s="68"/>
     </row>
@@ -3592,7 +4056,7 @@
         <v>118002</v>
       </c>
       <c r="C32" s="67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D32" s="29"/>
       <c r="E32" s="4"/>
@@ -3600,7 +4064,7 @@
         <v>777001</v>
       </c>
       <c r="G32" s="67" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H32" s="68"/>
     </row>
@@ -3609,7 +4073,7 @@
         <v>118999</v>
       </c>
       <c r="C33" s="67" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="4"/>
@@ -3617,7 +4081,7 @@
         <v>778001</v>
       </c>
       <c r="G33" s="67" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H33" s="68"/>
     </row>
@@ -3626,7 +4090,7 @@
         <v>119001</v>
       </c>
       <c r="C34" s="67" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D34" s="29"/>
       <c r="E34" s="4"/>
@@ -3634,7 +4098,7 @@
         <v>778002</v>
       </c>
       <c r="G34" s="67" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H34" s="68"/>
     </row>
@@ -3643,7 +4107,7 @@
         <v>119002</v>
       </c>
       <c r="C35" s="67" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="4"/>
@@ -3651,7 +4115,7 @@
         <v>778003</v>
       </c>
       <c r="G35" s="67" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H35" s="68"/>
     </row>
@@ -3660,7 +4124,7 @@
         <v>119999</v>
       </c>
       <c r="C36" s="67" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="4"/>
@@ -3668,7 +4132,7 @@
         <v>779888</v>
       </c>
       <c r="G36" s="67" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="H36" s="68"/>
     </row>
@@ -3677,7 +4141,7 @@
         <v>120001</v>
       </c>
       <c r="C37" s="67" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D37" s="29"/>
       <c r="E37" s="4"/>
@@ -3685,7 +4149,7 @@
         <v>780001</v>
       </c>
       <c r="G37" s="67" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="H37" s="68"/>
     </row>
@@ -3694,7 +4158,7 @@
         <v>120999</v>
       </c>
       <c r="C38" s="67" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D38" s="29"/>
       <c r="E38" s="4"/>
@@ -3702,7 +4166,7 @@
         <v>781001</v>
       </c>
       <c r="G38" s="67" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H38" s="68"/>
     </row>
@@ -3711,7 +4175,7 @@
         <v>122001</v>
       </c>
       <c r="C39" s="67" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="4"/>
@@ -3719,7 +4183,7 @@
         <v>781002</v>
       </c>
       <c r="G39" s="67" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="H39" s="68"/>
     </row>
@@ -3732,7 +4196,7 @@
         <v>781003</v>
       </c>
       <c r="G40" s="67" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="H40" s="68"/>
     </row>
@@ -3745,18 +4209,18 @@
         <v>783001</v>
       </c>
       <c r="G41" s="67" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="95" t="s">
+      <c r="B42" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="95" t="s">
+      <c r="C42" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="95" t="s">
+      <c r="D42" s="102" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="71"/>
@@ -3765,9 +4229,9 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="94"/>
-      <c r="C43" s="94"/>
-      <c r="D43" s="94"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="101"/>
       <c r="E43" s="71"/>
       <c r="F43" s="69"/>
       <c r="G43" s="70"/>
@@ -3778,7 +4242,7 @@
         <v>210001</v>
       </c>
       <c r="C44" s="67" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="4"/>
@@ -3791,7 +4255,7 @@
         <v>210002</v>
       </c>
       <c r="C45" s="67" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="4"/>
@@ -3804,7 +4268,7 @@
         <v>211001</v>
       </c>
       <c r="C46" s="67" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="4"/>
@@ -3817,7 +4281,7 @@
         <v>211002</v>
       </c>
       <c r="C47" s="67" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="4"/>
@@ -3830,7 +4294,7 @@
         <v>211003</v>
       </c>
       <c r="C48" s="67" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="4"/>
@@ -3843,7 +4307,7 @@
         <v>212001</v>
       </c>
       <c r="C49" s="67" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="4"/>
@@ -3856,7 +4320,7 @@
         <v>219001</v>
       </c>
       <c r="C50" s="67" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="4"/>
@@ -3869,7 +4333,7 @@
         <v>220001</v>
       </c>
       <c r="C51" s="67" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="4"/>
@@ -3882,7 +4346,7 @@
         <v>220002</v>
       </c>
       <c r="C52" s="67" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="4"/>
@@ -3895,7 +4359,7 @@
         <v>230001</v>
       </c>
       <c r="C53" s="67" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="4"/>
@@ -3908,7 +4372,7 @@
         <v>230001</v>
       </c>
       <c r="C54" s="67" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="4"/>
@@ -4177,12 +4641,12 @@
     </row>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" s="47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C4" s="46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="3:15" x14ac:dyDescent="0.25">
@@ -4208,78 +4672,78 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="95" t="s">
+      <c r="D8" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="95" t="s">
+      <c r="E8" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="109" t="s">
+      <c r="F8" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="95" t="s">
+      <c r="G8" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="95" t="s">
+      <c r="H8" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="95" t="s">
+      <c r="I8" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="95" t="s">
+      <c r="J8" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="95" t="s">
+      <c r="K8" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="111"/>
+      <c r="L8" s="118"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="108"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="96"/>
-      <c r="J9" s="96"/>
-      <c r="K9" s="96"/>
-      <c r="L9" s="111"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="118"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
     <row r="10" spans="3:15" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="G10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="60" t="s">
-        <v>92</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="H10" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="J10" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L10" s="8"/>
       <c r="M10" s="7"/>
@@ -4324,75 +4788,75 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="107" t="s">
+      <c r="C15" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="95" t="s">
+      <c r="E15" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="95" t="s">
+      <c r="F15" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="95" t="s">
+      <c r="G15" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="95" t="s">
+      <c r="H15" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="98" t="s">
+      <c r="I15" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="112" t="s">
+      <c r="J15" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="111"/>
-      <c r="L15" s="111"/>
-      <c r="M15" s="111"/>
-      <c r="N15" s="111"/>
-      <c r="O15" s="111"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="108"/>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="99"/>
-      <c r="J16" s="113"/>
-      <c r="K16" s="111"/>
-      <c r="L16" s="111"/>
-      <c r="M16" s="111"/>
-      <c r="N16" s="111"/>
-      <c r="O16" s="111"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
     </row>
     <row r="17" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="G17" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="H17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>92</v>
-      </c>
       <c r="J17" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="K17" s="11"/>
       <c r="L17" s="11"/>
@@ -4451,128 +4915,128 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="95" t="s">
+      <c r="C22" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="107" t="s">
+      <c r="D22" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="95" t="s">
+      <c r="E22" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="95" t="s">
+      <c r="F22" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="95" t="s">
+      <c r="G22" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="95" t="s">
+      <c r="H22" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="95" t="s">
+      <c r="I22" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="98" t="s">
+      <c r="J22" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="112" t="s">
+      <c r="K22" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="95" t="s">
+      <c r="L22" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="95" t="s">
+      <c r="M22" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="98" t="s">
+      <c r="N22" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="98" t="s">
+      <c r="O22" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="95" t="s">
+      <c r="P22" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="98" t="s">
+      <c r="Q22" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="R22" s="98" t="s">
+      <c r="R22" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="95" t="s">
+      <c r="S22" s="102" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="96"/>
-      <c r="D23" s="108"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="96"/>
-      <c r="H23" s="96"/>
-      <c r="I23" s="96"/>
-      <c r="J23" s="99"/>
-      <c r="K23" s="113"/>
-      <c r="L23" s="96"/>
-      <c r="M23" s="96"/>
-      <c r="N23" s="99"/>
-      <c r="O23" s="99"/>
-      <c r="P23" s="96"/>
-      <c r="Q23" s="99"/>
-      <c r="R23" s="99"/>
-      <c r="S23" s="96"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="103"/>
+      <c r="Q23" s="106"/>
+      <c r="R23" s="106"/>
+      <c r="S23" s="103"/>
     </row>
     <row r="24" spans="3:19" s="48" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C24" s="45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="K24" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M24" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H24" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="J24" s="6" t="s">
+      <c r="N24" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L24" s="6" t="s">
+      <c r="O24" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="M24" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="N24" s="45" t="s">
-        <v>94</v>
-      </c>
-      <c r="O24" s="45" t="s">
-        <v>94</v>
-      </c>
       <c r="P24" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Q24" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R24" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S24" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="3:19" x14ac:dyDescent="0.25">
@@ -4630,121 +5094,121 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="95" t="s">
+      <c r="C29" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="107" t="s">
+      <c r="D29" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="95" t="s">
+      <c r="E29" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="95" t="s">
+      <c r="F29" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="112" t="s">
+      <c r="G29" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="95" t="s">
+      <c r="H29" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="95" t="s">
+      <c r="I29" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="98" t="s">
+      <c r="J29" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="98" t="s">
+      <c r="K29" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="95" t="s">
+      <c r="L29" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="M29" s="98" t="s">
+      <c r="M29" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="98" t="s">
+      <c r="N29" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="95" t="s">
+      <c r="O29" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="P29" s="95" t="s">
+      <c r="P29" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="95" t="s">
+      <c r="Q29" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="95" t="s">
+      <c r="R29" s="102" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="96"/>
-      <c r="D30" s="108"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="113"/>
-      <c r="H30" s="96"/>
-      <c r="I30" s="96"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="99"/>
-      <c r="N30" s="99"/>
-      <c r="O30" s="96"/>
-      <c r="P30" s="96"/>
-      <c r="Q30" s="96"/>
-      <c r="R30" s="96"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="115"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
+      <c r="J30" s="106"/>
+      <c r="K30" s="106"/>
+      <c r="L30" s="103"/>
+      <c r="M30" s="106"/>
+      <c r="N30" s="106"/>
+      <c r="O30" s="103"/>
+      <c r="P30" s="103"/>
+      <c r="Q30" s="103"/>
+      <c r="R30" s="103"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D31" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="I31" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>90</v>
-      </c>
-      <c r="H31" s="6" t="s">
+      <c r="J31" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="I31" s="45" t="s">
-        <v>99</v>
-      </c>
-      <c r="J31" s="45" t="s">
-        <v>94</v>
-      </c>
       <c r="K31" s="45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L31" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="M31" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N31" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O31" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="P31" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="Q31" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="R31" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="3:19" x14ac:dyDescent="0.25">
@@ -4794,17 +5258,17 @@
     </row>
     <row r="35" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="95" t="s">
+      <c r="C36" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="95" t="s">
+      <c r="D36" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="95" t="s">
+      <c r="E36" s="102" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="12"/>
@@ -4815,9 +5279,9 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="96"/>
-      <c r="D37" s="96"/>
-      <c r="E37" s="96"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="103"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -4827,13 +5291,13 @@
     </row>
     <row r="38" spans="3:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C38" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E38" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F38" s="4"/>
       <c r="G38" s="4"/>
@@ -4895,19 +5359,19 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="95" t="s">
+      <c r="C44" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="95" t="s">
+      <c r="D44" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="95" t="s">
+      <c r="E44" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="98" t="s">
+      <c r="F44" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="114" t="s">
+      <c r="G44" s="121" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="4"/>
@@ -4917,11 +5381,11 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="96"/>
-      <c r="D45" s="96"/>
-      <c r="E45" s="96"/>
-      <c r="F45" s="99"/>
-      <c r="G45" s="115"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="103"/>
+      <c r="E45" s="103"/>
+      <c r="F45" s="106"/>
+      <c r="G45" s="122"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -4930,19 +5394,19 @@
     </row>
     <row r="46" spans="3:14" s="48" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C46" s="45" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E46" s="45" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G46" s="45" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="3:14" x14ac:dyDescent="0.25">
@@ -4966,42 +5430,42 @@
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="95" t="s">
+      <c r="C52" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="95" t="s">
+      <c r="D52" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="95" t="s">
+      <c r="E52" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="95" t="s">
+      <c r="F52" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="95" t="s">
+      <c r="G52" s="102" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="96"/>
-      <c r="D53" s="96"/>
-      <c r="E53" s="96"/>
-      <c r="F53" s="96"/>
-      <c r="G53" s="96"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="103"/>
+      <c r="F53" s="103"/>
+      <c r="G53" s="103"/>
     </row>
     <row r="54" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="3:7" x14ac:dyDescent="0.25">
@@ -5025,69 +5489,69 @@
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="98" t="s">
+      <c r="C59" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="105"/>
-      <c r="E59" s="95" t="s">
+      <c r="D59" s="112"/>
+      <c r="E59" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="98" t="s">
+      <c r="F59" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="104"/>
+      <c r="G59" s="111"/>
     </row>
     <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="104"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="94"/>
-      <c r="F60" s="99"/>
-      <c r="G60" s="104"/>
+      <c r="C60" s="111"/>
+      <c r="D60" s="113"/>
+      <c r="E60" s="101"/>
+      <c r="F60" s="106"/>
+      <c r="G60" s="111"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="100" t="s">
-        <v>97</v>
-      </c>
-      <c r="D61" s="101"/>
+      <c r="C61" s="107" t="s">
+        <v>95</v>
+      </c>
+      <c r="D61" s="108"/>
       <c r="E61" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="102"/>
-      <c r="D62" s="103"/>
+      <c r="C62" s="109"/>
+      <c r="D62" s="110"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="97"/>
-      <c r="D63" s="97"/>
+      <c r="C63" s="104"/>
+      <c r="D63" s="104"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="4"/>
     </row>
     <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="97" t="s">
+      <c r="C65" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="97"/>
+      <c r="D65" s="104"/>
       <c r="E65" s="49">
         <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="97" t="s">
+      <c r="C66" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="97"/>
+      <c r="D66" s="104"/>
       <c r="E66" s="49">
         <v>0.3</v>
       </c>
@@ -5182,8 +5646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A128" sqref="A128:XFD128"/>
+    <sheetView topLeftCell="A127" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O143" sqref="O143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5211,16 +5675,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
-        <v>103</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
+      <c r="A1" s="125" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="72" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B2" s="63"/>
       <c r="C2" s="63"/>
@@ -5248,7 +5712,7 @@
         <v>43</v>
       </c>
       <c r="I4" s="74" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J4" s="16"/>
     </row>
@@ -5283,7 +5747,7 @@
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E7" s="14"/>
       <c r="F7" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
@@ -5374,53 +5838,53 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="78"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="95" t="s">
+      <c r="A16" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="98" t="s">
+      <c r="B16" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="105"/>
-      <c r="D16" s="95" t="s">
+      <c r="C16" s="112"/>
+      <c r="D16" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="95" t="s">
+      <c r="E16" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="95" t="s">
+      <c r="G16" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="95" t="s">
+      <c r="H16" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="116" t="s">
+      <c r="I16" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="95" t="s">
+      <c r="J16" s="102" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="96"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="119"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="117"/>
-      <c r="J17" s="96"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="103"/>
     </row>
     <row r="18" spans="1:10" s="57" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52">
@@ -5462,8 +5926,8 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="102"/>
-      <c r="C19" s="103"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -5648,7 +6112,7 @@
     </row>
     <row r="35" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A35" s="73" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -5656,7 +6120,7 @@
         <v>2.1</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G36" s="17"/>
       <c r="H36" s="17"/>
@@ -5666,21 +6130,21 @@
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E37" s="14"/>
       <c r="F37" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="14" t="s">
         <v>43</v>
       </c>
       <c r="I37" s="74" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J37" s="16"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E38" s="14"/>
       <c r="F38" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="14" t="s">
@@ -5715,7 +6179,7 @@
         <v>43</v>
       </c>
       <c r="I40" s="77" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J40" s="14"/>
     </row>
@@ -5729,7 +6193,7 @@
         <v>43</v>
       </c>
       <c r="I41" s="77" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J41" s="14"/>
     </row>
@@ -5757,21 +6221,21 @@
         <v>43</v>
       </c>
       <c r="I43" s="77" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J43" s="14"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E44" s="14"/>
       <c r="F44" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14" t="s">
         <v>43</v>
       </c>
       <c r="I44" s="77" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J44" s="14"/>
     </row>
@@ -5781,44 +6245,44 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="107" t="s">
+      <c r="A51" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="95" t="s">
+      <c r="B51" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="95" t="s">
+      <c r="C51" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="95" t="s">
+      <c r="D51" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="95" t="s">
+      <c r="E51" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="95" t="s">
+      <c r="F51" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="98" t="s">
+      <c r="G51" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="112" t="s">
+      <c r="H51" s="119" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="108"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="96"/>
-      <c r="D52" s="96"/>
-      <c r="E52" s="96"/>
-      <c r="F52" s="96"/>
-      <c r="G52" s="99"/>
-      <c r="H52" s="113"/>
+      <c r="A52" s="115"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="106"/>
+      <c r="H52" s="120"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A53" s="82" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B53" s="83" t="s">
         <v>45</v>
@@ -5827,7 +6291,7 @@
         <v>49</v>
       </c>
       <c r="D53" s="83" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E53" s="84">
         <v>27740</v>
@@ -5836,7 +6300,7 @@
         <v>51</v>
       </c>
       <c r="G53" s="83" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H53" s="83">
         <v>700409</v>
@@ -5847,7 +6311,7 @@
         <v>2.1</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G55" s="17"/>
       <c r="H55" s="17"/>
@@ -5857,21 +6321,21 @@
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E56" s="14"/>
       <c r="F56" s="14" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="G56" s="14"/>
       <c r="H56" s="14" t="s">
         <v>43</v>
       </c>
       <c r="I56" s="86" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J56" s="16"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E57" s="14"/>
       <c r="F57" s="14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="14" t="s">
@@ -5906,7 +6370,7 @@
         <v>43</v>
       </c>
       <c r="I59" s="77" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J59" s="14"/>
     </row>
@@ -5920,7 +6384,7 @@
         <v>43</v>
       </c>
       <c r="I60" s="77" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="J60" s="14"/>
     </row>
@@ -5948,21 +6412,21 @@
         <v>43</v>
       </c>
       <c r="I62" s="77" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="J62" s="14"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E63" s="14"/>
       <c r="F63" s="14" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G63" s="14"/>
       <c r="H63" s="14" t="s">
         <v>43</v>
       </c>
       <c r="I63" s="77" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J63" s="14"/>
     </row>
@@ -5982,7 +6446,7 @@
     </row>
     <row r="70" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A70" s="73" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
@@ -6181,7 +6645,7 @@
       </c>
       <c r="J84" s="14"/>
       <c r="K84" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
@@ -6409,7 +6873,7 @@
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A98" s="91" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B98" s="75"/>
       <c r="C98" s="75"/>
@@ -6470,16 +6934,16 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="90" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B100" s="90">
         <v>114001</v>
       </c>
       <c r="C100" s="90" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D100" s="90" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E100" s="90">
         <v>100000</v>
@@ -6508,10 +6972,10 @@
         <v>220001</v>
       </c>
       <c r="C101" s="90" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D101" s="90" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E101" s="90">
         <v>40000</v>
@@ -6540,10 +7004,10 @@
         <v>220002</v>
       </c>
       <c r="C102" s="90" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D102" s="90" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E102" s="90">
         <v>60000</v>
@@ -6593,7 +7057,7 @@
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104" s="91" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B104" s="75"/>
       <c r="C104" s="75"/>
@@ -6653,11 +7117,11 @@
         <v>114001</v>
       </c>
       <c r="B106" s="90" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C106" s="90"/>
       <c r="D106" s="75" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E106" s="75"/>
       <c r="F106" s="75"/>
@@ -6683,11 +7147,11 @@
         <v>220001</v>
       </c>
       <c r="B107" s="90" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C107" s="90"/>
       <c r="D107" s="75" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E107" s="75"/>
       <c r="F107" s="75"/>
@@ -6713,11 +7177,11 @@
         <v>220002</v>
       </c>
       <c r="B108" s="90" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C108" s="90"/>
       <c r="D108" s="75" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E108" s="75"/>
       <c r="F108" s="75"/>
@@ -6841,7 +7305,7 @@
     </row>
     <row r="113" spans="1:24" ht="21" x14ac:dyDescent="0.35">
       <c r="A113" s="92" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B113" s="75"/>
       <c r="C113" s="75"/>
@@ -6872,10 +7336,10 @@
       <c r="C114" s="75"/>
       <c r="D114" s="75"/>
       <c r="E114" s="20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F114" s="21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G114" s="19"/>
       <c r="H114" s="19"/>
@@ -6913,7 +7377,7 @@
         <v>48</v>
       </c>
       <c r="J115" s="25" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K115" s="75"/>
       <c r="L115" s="75"/>
@@ -7033,7 +7497,7 @@
       <c r="D119" s="75"/>
       <c r="E119" s="14"/>
       <c r="F119" s="14" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G119" s="14"/>
       <c r="H119" s="14" t="s">
@@ -7063,13 +7527,13 @@
       <c r="D120" s="75"/>
       <c r="E120" s="14"/>
       <c r="F120" s="14" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G120" s="14"/>
       <c r="H120" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I120" s="121">
+      <c r="I120" s="93">
         <f>+K100</f>
         <v>0</v>
       </c>
@@ -7096,13 +7560,13 @@
       <c r="D121" s="75"/>
       <c r="E121" s="14"/>
       <c r="F121" s="14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G121" s="14"/>
       <c r="H121" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="I121" s="121"/>
+      <c r="I121" s="93"/>
       <c r="J121" s="32" t="s">
         <v>10</v>
       </c>
@@ -7222,8 +7686,8 @@
       <c r="X125" s="75"/>
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A126" s="122" t="s">
-        <v>211</v>
+      <c r="A126" s="94" t="s">
+        <v>208</v>
       </c>
       <c r="B126" s="75"/>
       <c r="C126" s="75"/>
@@ -7310,65 +7774,65 @@
       <c r="W127" s="75"/>
     </row>
     <row r="128" spans="1:24" s="57" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="123" t="s">
+      <c r="A128" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B128" s="123" t="s">
+      <c r="B128" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C128" s="123" t="s">
+      <c r="C128" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="D128" s="123" t="s">
+      <c r="D128" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="E128" s="123" t="s">
+      <c r="E128" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="F128" s="124">
+      <c r="F128" s="96">
         <v>27419</v>
       </c>
-      <c r="G128" s="123" t="s">
+      <c r="G128" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="H128" s="123" t="s">
+      <c r="H128" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="I128" s="123" t="s">
+      <c r="I128" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="J128" s="123" t="s">
+      <c r="J128" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="K128" s="123">
+      <c r="K128" s="95">
         <v>20000000</v>
       </c>
-      <c r="L128" s="124">
+      <c r="L128" s="96">
         <v>42449</v>
       </c>
-      <c r="M128" s="123">
+      <c r="M128" s="95">
         <v>12</v>
       </c>
-      <c r="N128" s="124">
+      <c r="N128" s="96">
         <v>42809</v>
       </c>
-      <c r="O128" s="123">
+      <c r="O128" s="95">
         <v>40000</v>
       </c>
-      <c r="P128" s="123">
+      <c r="P128" s="95">
         <v>60000</v>
       </c>
-      <c r="Q128" s="123">
+      <c r="Q128" s="95">
         <v>100000</v>
       </c>
-      <c r="R128" s="126" t="s">
-        <v>212</v>
-      </c>
-      <c r="S128" s="127"/>
-      <c r="T128" s="125"/>
-      <c r="U128" s="125"/>
-      <c r="V128" s="125"/>
-      <c r="W128" s="125"/>
+      <c r="R128" s="98" t="s">
+        <v>209</v>
+      </c>
+      <c r="S128" s="99"/>
+      <c r="T128" s="97"/>
+      <c r="U128" s="97"/>
+      <c r="V128" s="97"/>
+      <c r="W128" s="97"/>
     </row>
     <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129" s="75"/>
@@ -7397,7 +7861,7 @@
     </row>
     <row r="132" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
@@ -7421,16 +7885,16 @@
     </row>
     <row r="134" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B134" s="1">
         <v>111001</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E134" s="1">
         <v>100000</v>
@@ -7444,10 +7908,10 @@
         <v>114001</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E135" s="1">
         <v>100000</v>
@@ -7457,7 +7921,7 @@
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.25">
@@ -7478,11 +7942,11 @@
         <v>111001</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H140" s="75"/>
       <c r="I140"/>
@@ -7492,11 +7956,11 @@
         <v>114001</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="H141" s="75"/>
       <c r="I141"/>
@@ -7531,22 +7995,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+      <selection activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7562,206 +8014,112 @@
     <col min="18" max="18" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="118" t="s">
-        <v>104</v>
-      </c>
-      <c r="B1" s="118"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="118"/>
-    </row>
-    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J14" s="20"/>
-      <c r="K14" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J15" s="23"/>
-      <c r="K15" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="L15" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="M15" s="24"/>
-      <c r="N15" s="33" t="s">
-        <v>84</v>
-      </c>
-      <c r="O15" s="25"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J16" s="34"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="37"/>
-    </row>
-    <row r="17" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J17" s="38"/>
-      <c r="K17" s="39" t="s">
-        <v>105</v>
-      </c>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="38"/>
-      <c r="R17" s="4"/>
-    </row>
-    <row r="18" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K18" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="L18" s="42"/>
-      <c r="R18" s="4"/>
-    </row>
-    <row r="19" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K19" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="L19" s="120" t="s">
-        <v>27</v>
-      </c>
-      <c r="M19" s="120"/>
-      <c r="N19" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="O19" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="P19" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q19" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="R19" s="51" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K20" s="43"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-    </row>
-    <row r="21" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K21" s="43"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="125" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
     </row>
     <row r="22" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K22" s="43"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="K22" s="5"/>
+      <c r="R22" s="4"/>
     </row>
     <row r="23" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K23" s="5"/>
       <c r="R23" s="4"/>
     </row>
-    <row r="24" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K24" s="5"/>
-      <c r="R24" s="4"/>
+    <row r="24" spans="10:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J24" s="20"/>
+      <c r="K24" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
     </row>
     <row r="25" spans="10:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J25" s="20"/>
-      <c r="K25" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-    </row>
-    <row r="26" spans="10:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J26" s="23"/>
-      <c r="K26" s="26" t="s">
+      <c r="J25" s="23"/>
+      <c r="K25" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="L25" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="L26" s="32" t="s">
+      <c r="M25" s="24"/>
+      <c r="N25" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="O25" s="25"/>
+    </row>
+    <row r="26" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J26" s="34"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="37"/>
+    </row>
+    <row r="27" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="J27" s="38"/>
+      <c r="K27" s="39" t="s">
+        <v>103</v>
+      </c>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="40"/>
+      <c r="O27" s="38"/>
+      <c r="R27" s="4"/>
+    </row>
+    <row r="28" spans="10:18" x14ac:dyDescent="0.25">
+      <c r="K28" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="M26" s="24"/>
-      <c r="N26" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="O26" s="25"/>
-    </row>
-    <row r="27" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J27" s="34"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="37"/>
-    </row>
-    <row r="28" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J28" s="38"/>
-      <c r="K28" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="L28" s="38"/>
-      <c r="M28" s="38"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="38"/>
+      <c r="L28" s="42"/>
       <c r="R28" s="4"/>
     </row>
     <row r="29" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K29" s="41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="L29" s="42"/>
       <c r="R29" s="4"/>
     </row>
     <row r="30" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K30" s="41" t="s">
-        <v>88</v>
-      </c>
-      <c r="L30" s="42"/>
-      <c r="R30" s="4"/>
+      <c r="K30" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="L30" s="127" t="s">
+        <v>27</v>
+      </c>
+      <c r="M30" s="127"/>
+      <c r="N30" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" s="51" t="s">
+        <v>5</v>
+      </c>
+      <c r="P30" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q30" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="R30" s="51" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="31" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K31" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="L31" s="120" t="s">
-        <v>27</v>
-      </c>
-      <c r="M31" s="120"/>
-      <c r="N31" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="O31" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="P31" s="51" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q31" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="R31" s="51" t="s">
-        <v>25</v>
-      </c>
+      <c r="K31" s="43"/>
+      <c r="L31" s="44"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
     </row>
     <row r="32" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K32" s="43"/>
@@ -7783,24 +8141,25 @@
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="11:18" x14ac:dyDescent="0.25">
-      <c r="K34" s="43"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="29"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="L19:M19"/>
-    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L30:M30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
tes koneksi sql server(Login-useradmin-crud_rekening-koneksi) & update excel
</commit_message>
<xml_diff>
--- a/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
+++ b/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COA" sheetId="13" r:id="rId1"/>
     <sheet name="DATABASE" sheetId="5" r:id="rId2"/>
     <sheet name="Menu Transaksi" sheetId="11" r:id="rId3"/>
     <sheet name="Menu Informasi" sheetId="9" r:id="rId4"/>
-    <sheet name="Menu Properti" sheetId="14" r:id="rId5"/>
-    <sheet name="Menu Cetak" sheetId="10" r:id="rId6"/>
+    <sheet name="Menu Cetak" sheetId="10" r:id="rId5"/>
+    <sheet name="Menu Properti" sheetId="14" r:id="rId6"/>
     <sheet name="Menu Administrasi" sheetId="12" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="211">
   <si>
     <t>REKENING</t>
   </si>
@@ -631,9 +631,6 @@
   </si>
   <si>
     <t xml:space="preserve">    </t>
-  </si>
-  <si>
-    <t>1.2</t>
   </si>
   <si>
     <t>PEMBAYARAN IURAN</t>
@@ -1344,26 +1341,62 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1377,52 +1410,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2686,7 +2683,41 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>setelah tabel jurnal terisi proses berikutnya mengisi Tabel Buku Besar.</a:t>
+            <a:t>setelah tabel jurnal terisi proses berikutnya mengisi Tabel Buku Besar</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> kolom saldo tabel buku besar akan otomatis bertambah atau berkurang sesuai inputan data pada pembayaran iuran jiwa/kebakaran</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="id-ID" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:hueOff val="0"/>
+                  <a:satOff val="0"/>
+                  <a:lumOff val="0"/>
+                  <a:alphaOff val="0"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>.</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -3315,6 +3346,44 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="4457700"/>
+          <a:ext cx="4895850" cy="1838325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3607,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView topLeftCell="A27" workbookViewId="0">
       <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
@@ -3632,34 +3701,34 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="102" t="s">
+      <c r="B6" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="102" t="s">
+      <c r="C6" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="102" t="s">
+      <c r="D6" s="100" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="59"/>
-      <c r="F6" s="102" t="s">
+      <c r="F6" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="102" t="s">
+      <c r="G6" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="102" t="s">
+      <c r="H6" s="100" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="101"/>
-      <c r="C7" s="101"/>
-      <c r="D7" s="103"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="101"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="103"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="101"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="66">
@@ -3807,13 +3876,13 @@
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="100" t="s">
+      <c r="F17" s="103" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="100" t="s">
+      <c r="G17" s="103" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="100" t="s">
+      <c r="H17" s="103" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3826,9 +3895,9 @@
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="102"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="66">
@@ -4214,13 +4283,13 @@
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="102" t="s">
+      <c r="B42" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="102" t="s">
+      <c r="C42" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="102" t="s">
+      <c r="D42" s="100" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="71"/>
@@ -4229,9 +4298,9 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="101"/>
-      <c r="C43" s="101"/>
-      <c r="D43" s="101"/>
+      <c r="B43" s="102"/>
+      <c r="C43" s="102"/>
+      <c r="D43" s="102"/>
       <c r="E43" s="71"/>
       <c r="F43" s="69"/>
       <c r="G43" s="70"/>
@@ -4591,18 +4660,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="G17:G18"/>
+    <mergeCell ref="H17:H18"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
     <mergeCell ref="H6:H7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="G17:G18"/>
-    <mergeCell ref="H17:H18"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4672,48 +4741,48 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="114" t="s">
+      <c r="C8" s="108" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="102" t="s">
+      <c r="D8" s="100" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="102" t="s">
+      <c r="E8" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="116" t="s">
+      <c r="F8" s="113" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="102" t="s">
+      <c r="G8" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="102" t="s">
+      <c r="H8" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="102" t="s">
+      <c r="I8" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="102" t="s">
+      <c r="J8" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="102" t="s">
+      <c r="K8" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="118"/>
+      <c r="L8" s="112"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="115"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="117"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
-      <c r="J9" s="103"/>
-      <c r="K9" s="103"/>
-      <c r="L9" s="118"/>
+      <c r="C9" s="109"/>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="101"/>
+      <c r="J9" s="101"/>
+      <c r="K9" s="101"/>
+      <c r="L9" s="112"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
@@ -4788,50 +4857,50 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="114" t="s">
+      <c r="C15" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="102" t="s">
+      <c r="D15" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="102" t="s">
+      <c r="E15" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="102" t="s">
+      <c r="F15" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="102" t="s">
+      <c r="G15" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="102" t="s">
+      <c r="H15" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="105" t="s">
+      <c r="I15" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="119" t="s">
+      <c r="J15" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="118"/>
+      <c r="K15" s="112"/>
+      <c r="L15" s="112"/>
+      <c r="M15" s="112"/>
+      <c r="N15" s="112"/>
+      <c r="O15" s="112"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="115"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="103"/>
-      <c r="G16" s="103"/>
-      <c r="H16" s="103"/>
-      <c r="I16" s="106"/>
-      <c r="J16" s="120"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="118"/>
+      <c r="C16" s="109"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="101"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="111"/>
+      <c r="K16" s="112"/>
+      <c r="L16" s="112"/>
+      <c r="M16" s="112"/>
+      <c r="N16" s="112"/>
+      <c r="O16" s="112"/>
     </row>
     <row r="17" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="45" t="s">
@@ -4915,76 +4984,76 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="102" t="s">
+      <c r="C22" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="114" t="s">
+      <c r="D22" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="102" t="s">
+      <c r="E22" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="102" t="s">
+      <c r="F22" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="102" t="s">
+      <c r="G22" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="102" t="s">
+      <c r="H22" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="102" t="s">
+      <c r="I22" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="105" t="s">
+      <c r="J22" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="119" t="s">
+      <c r="K22" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="102" t="s">
+      <c r="L22" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="102" t="s">
+      <c r="M22" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="105" t="s">
+      <c r="N22" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="105" t="s">
+      <c r="O22" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="102" t="s">
+      <c r="P22" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="105" t="s">
+      <c r="Q22" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="R22" s="105" t="s">
+      <c r="R22" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="102" t="s">
+      <c r="S22" s="100" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="103"/>
-      <c r="D23" s="115"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="120"/>
-      <c r="L23" s="103"/>
-      <c r="M23" s="103"/>
-      <c r="N23" s="106"/>
-      <c r="O23" s="106"/>
-      <c r="P23" s="103"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="106"/>
-      <c r="S23" s="103"/>
+      <c r="C23" s="101"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="101"/>
+      <c r="G23" s="101"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="101"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="111"/>
+      <c r="L23" s="101"/>
+      <c r="M23" s="101"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="101"/>
+      <c r="Q23" s="105"/>
+      <c r="R23" s="105"/>
+      <c r="S23" s="101"/>
     </row>
     <row r="24" spans="3:19" s="48" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C24" s="45" t="s">
@@ -5094,72 +5163,72 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="102" t="s">
+      <c r="C29" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="114" t="s">
+      <c r="D29" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="102" t="s">
+      <c r="E29" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="102" t="s">
+      <c r="F29" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="119" t="s">
+      <c r="G29" s="110" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="102" t="s">
+      <c r="H29" s="100" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="102" t="s">
+      <c r="I29" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="105" t="s">
+      <c r="J29" s="104" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="105" t="s">
+      <c r="K29" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="102" t="s">
+      <c r="L29" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="M29" s="105" t="s">
+      <c r="M29" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="105" t="s">
+      <c r="N29" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="102" t="s">
+      <c r="O29" s="100" t="s">
         <v>25</v>
       </c>
-      <c r="P29" s="102" t="s">
+      <c r="P29" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="102" t="s">
+      <c r="Q29" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="102" t="s">
+      <c r="R29" s="100" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="103"/>
-      <c r="D30" s="115"/>
-      <c r="E30" s="103"/>
-      <c r="F30" s="103"/>
-      <c r="G30" s="120"/>
-      <c r="H30" s="103"/>
-      <c r="I30" s="103"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="103"/>
-      <c r="M30" s="106"/>
-      <c r="N30" s="106"/>
-      <c r="O30" s="103"/>
-      <c r="P30" s="103"/>
-      <c r="Q30" s="103"/>
-      <c r="R30" s="103"/>
+      <c r="C30" s="101"/>
+      <c r="D30" s="109"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="101"/>
+      <c r="G30" s="111"/>
+      <c r="H30" s="101"/>
+      <c r="I30" s="101"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="105"/>
+      <c r="L30" s="101"/>
+      <c r="M30" s="105"/>
+      <c r="N30" s="105"/>
+      <c r="O30" s="101"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="101"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="45" t="s">
@@ -5262,13 +5331,13 @@
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="102" t="s">
+      <c r="C36" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="102" t="s">
+      <c r="D36" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="102" t="s">
+      <c r="E36" s="100" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="12"/>
@@ -5279,9 +5348,9 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="103"/>
-      <c r="D37" s="103"/>
-      <c r="E37" s="103"/>
+      <c r="C37" s="101"/>
+      <c r="D37" s="101"/>
+      <c r="E37" s="101"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -5359,19 +5428,19 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="102" t="s">
+      <c r="C44" s="100" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="102" t="s">
+      <c r="D44" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="102" t="s">
+      <c r="E44" s="100" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="105" t="s">
+      <c r="F44" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="121" t="s">
+      <c r="G44" s="106" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="4"/>
@@ -5381,11 +5450,11 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="103"/>
-      <c r="D45" s="103"/>
-      <c r="E45" s="103"/>
-      <c r="F45" s="106"/>
-      <c r="G45" s="122"/>
+      <c r="C45" s="101"/>
+      <c r="D45" s="101"/>
+      <c r="E45" s="101"/>
+      <c r="F45" s="105"/>
+      <c r="G45" s="107"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -5430,28 +5499,28 @@
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="102" t="s">
+      <c r="C52" s="100" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="102" t="s">
+      <c r="D52" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="102" t="s">
+      <c r="E52" s="100" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="102" t="s">
+      <c r="F52" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="102" t="s">
+      <c r="G52" s="100" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="103"/>
-      <c r="D53" s="103"/>
-      <c r="E53" s="103"/>
-      <c r="F53" s="103"/>
-      <c r="G53" s="103"/>
+      <c r="C53" s="101"/>
+      <c r="D53" s="101"/>
+      <c r="E53" s="101"/>
+      <c r="F53" s="101"/>
+      <c r="G53" s="101"/>
     </row>
     <row r="54" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -5489,30 +5558,30 @@
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="105" t="s">
+      <c r="C59" s="104" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="112"/>
-      <c r="E59" s="102" t="s">
+      <c r="D59" s="116"/>
+      <c r="E59" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="105" t="s">
+      <c r="F59" s="104" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="111"/>
+      <c r="G59" s="115"/>
     </row>
     <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="111"/>
-      <c r="D60" s="113"/>
-      <c r="E60" s="101"/>
-      <c r="F60" s="106"/>
-      <c r="G60" s="111"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="117"/>
+      <c r="E60" s="102"/>
+      <c r="F60" s="105"/>
+      <c r="G60" s="115"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="107" t="s">
+      <c r="C61" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="108"/>
+      <c r="D61" s="120"/>
       <c r="E61" s="1" t="s">
         <v>96</v>
       </c>
@@ -5521,14 +5590,14 @@
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="109"/>
-      <c r="D62" s="110"/>
+      <c r="C62" s="121"/>
+      <c r="D62" s="122"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="104"/>
-      <c r="D63" s="104"/>
+      <c r="C63" s="118"/>
+      <c r="D63" s="118"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="4"/>
@@ -5539,30 +5608,82 @@
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="104" t="s">
+      <c r="C65" s="118" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="104"/>
+      <c r="D65" s="118"/>
       <c r="E65" s="49">
         <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="104" t="s">
+      <c r="C66" s="118" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="104"/>
+      <c r="D66" s="118"/>
       <c r="E66" s="49">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="C59:D60"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
     <mergeCell ref="R29:R30"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
@@ -5579,63 +5700,11 @@
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="C59:D60"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -5646,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView topLeftCell="A127" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O143" sqref="O143"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E120" sqref="E120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5675,12 +5744,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="123" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="72" t="s">
@@ -5845,46 +5914,46 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="102" t="s">
+      <c r="A16" s="100" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="105" t="s">
+      <c r="B16" s="104" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="112"/>
-      <c r="D16" s="102" t="s">
+      <c r="C16" s="116"/>
+      <c r="D16" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="102" t="s">
+      <c r="E16" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="102" t="s">
+      <c r="F16" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="102" t="s">
+      <c r="G16" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="102" t="s">
+      <c r="H16" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="123" t="s">
+      <c r="I16" s="125" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="102" t="s">
+      <c r="J16" s="100" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="103"/>
-      <c r="B17" s="106"/>
-      <c r="C17" s="126"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
-      <c r="H17" s="103"/>
-      <c r="I17" s="124"/>
-      <c r="J17" s="103"/>
+      <c r="A17" s="101"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="124"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
+      <c r="I17" s="126"/>
+      <c r="J17" s="101"/>
     </row>
     <row r="18" spans="1:10" s="57" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52">
@@ -5926,8 +5995,8 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="110"/>
+      <c r="B19" s="121"/>
+      <c r="C19" s="122"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -6245,40 +6314,40 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="114" t="s">
+      <c r="A51" s="108" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="102" t="s">
+      <c r="B51" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="102" t="s">
+      <c r="C51" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="102" t="s">
+      <c r="D51" s="100" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="102" t="s">
+      <c r="E51" s="100" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="102" t="s">
+      <c r="F51" s="100" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="105" t="s">
+      <c r="G51" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="119" t="s">
+      <c r="H51" s="110" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="115"/>
-      <c r="B52" s="103"/>
-      <c r="C52" s="103"/>
-      <c r="D52" s="103"/>
-      <c r="E52" s="103"/>
-      <c r="F52" s="103"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="120"/>
+      <c r="A52" s="109"/>
+      <c r="B52" s="101"/>
+      <c r="C52" s="101"/>
+      <c r="D52" s="101"/>
+      <c r="E52" s="101"/>
+      <c r="F52" s="101"/>
+      <c r="G52" s="105"/>
+      <c r="H52" s="111"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A53" s="82" t="s">
@@ -6308,7 +6377,7 @@
     </row>
     <row r="55" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E55" s="20">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F55" s="22" t="s">
         <v>181</v>
@@ -7335,11 +7404,11 @@
       <c r="B114" s="75"/>
       <c r="C114" s="75"/>
       <c r="D114" s="75"/>
-      <c r="E114" s="20" t="s">
+      <c r="E114" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="F114" s="21" t="s">
         <v>202</v>
-      </c>
-      <c r="F114" s="21" t="s">
-        <v>203</v>
       </c>
       <c r="G114" s="19"/>
       <c r="H114" s="19"/>
@@ -7377,7 +7446,7 @@
         <v>48</v>
       </c>
       <c r="J115" s="25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K115" s="75"/>
       <c r="L115" s="75"/>
@@ -7497,7 +7566,7 @@
       <c r="D119" s="75"/>
       <c r="E119" s="14"/>
       <c r="F119" s="14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G119" s="14"/>
       <c r="H119" s="14" t="s">
@@ -7527,7 +7596,7 @@
       <c r="D120" s="75"/>
       <c r="E120" s="14"/>
       <c r="F120" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G120" s="14"/>
       <c r="H120" s="14" t="s">
@@ -7560,7 +7629,7 @@
       <c r="D121" s="75"/>
       <c r="E121" s="14"/>
       <c r="F121" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G121" s="14"/>
       <c r="H121" s="14" t="s">
@@ -7687,7 +7756,7 @@
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A126" s="94" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B126" s="75"/>
       <c r="C126" s="75"/>
@@ -7826,7 +7895,7 @@
         <v>100000</v>
       </c>
       <c r="R128" s="98" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="S128" s="99"/>
       <c r="T128" s="97"/>
@@ -7894,7 +7963,7 @@
         <v>193</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E134" s="1">
         <v>100000</v>
@@ -7911,7 +7980,7 @@
         <v>195</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E135" s="1">
         <v>100000</v>
@@ -7960,13 +8029,24 @@
       </c>
       <c r="C141" s="1"/>
       <c r="D141" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H141" s="75"/>
       <c r="I141"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
@@ -7975,17 +8055,6 @@
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="E51:E52"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7997,8 +8066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8015,12 +8084,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="125" t="s">
+      <c r="A1" s="123" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="125"/>
-      <c r="C1" s="125"/>
-      <c r="D1" s="125"/>
+      <c r="B1" s="123"/>
+      <c r="C1" s="123"/>
+      <c r="D1" s="123"/>
     </row>
     <row r="22" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K22" s="5"/>
@@ -8155,7 +8224,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -8167,9 +8238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
workflow lagi proses pembuatan dari client.
</commit_message>
<xml_diff>
--- a/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
+++ b/update_INFO CRUD_APLIKASI PBMT TAAWUN.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="COA" sheetId="13" r:id="rId1"/>
@@ -1341,62 +1341,26 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1410,16 +1374,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1577,8 +1577,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12786783" y="4066117"/>
-          <a:ext cx="2418731" cy="1878400"/>
+          <a:off x="12792075" y="4064794"/>
+          <a:ext cx="2410794" cy="1881046"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -1817,8 +1817,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="12792226" y="10849428"/>
-          <a:ext cx="2418731" cy="1881424"/>
+          <a:off x="12797518" y="10853397"/>
+          <a:ext cx="2410794" cy="1882747"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -2176,8 +2176,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8360833" y="19886083"/>
-          <a:ext cx="8905875" cy="1892008"/>
+          <a:off x="8382000" y="19895344"/>
+          <a:ext cx="8882063" cy="1894653"/>
           <a:chOff x="61936" y="540854"/>
           <a:chExt cx="2250894" cy="1838184"/>
         </a:xfrm>
@@ -3676,8 +3676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I79"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3701,34 +3701,34 @@
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="100" t="s">
+      <c r="C6" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="102" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="59"/>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="100" t="s">
+      <c r="G6" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="100" t="s">
+      <c r="H6" s="102" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="102"/>
-      <c r="C7" s="102"/>
-      <c r="D7" s="101"/>
+      <c r="B7" s="101"/>
+      <c r="C7" s="101"/>
+      <c r="D7" s="103"/>
       <c r="E7" s="59"/>
-      <c r="F7" s="102"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="101"/>
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="103"/>
     </row>
     <row r="8" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="66">
@@ -3876,13 +3876,13 @@
       </c>
       <c r="D17" s="68"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="103" t="s">
+      <c r="F17" s="100" t="s">
         <v>37</v>
       </c>
-      <c r="G17" s="103" t="s">
+      <c r="G17" s="100" t="s">
         <v>38</v>
       </c>
-      <c r="H17" s="103" t="s">
+      <c r="H17" s="100" t="s">
         <v>34</v>
       </c>
     </row>
@@ -3895,9 +3895,9 @@
       </c>
       <c r="D18" s="68"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="102"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="102"/>
+      <c r="F18" s="101"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="101"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="66">
@@ -4283,13 +4283,13 @@
       <c r="H41" s="29"/>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="100" t="s">
+      <c r="B42" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="100" t="s">
+      <c r="C42" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="D42" s="100" t="s">
+      <c r="D42" s="102" t="s">
         <v>34</v>
       </c>
       <c r="E42" s="71"/>
@@ -4298,9 +4298,9 @@
       <c r="H42" s="4"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="102"/>
-      <c r="C43" s="102"/>
-      <c r="D43" s="102"/>
+      <c r="B43" s="101"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="101"/>
       <c r="E43" s="71"/>
       <c r="F43" s="69"/>
       <c r="G43" s="70"/>
@@ -4660,18 +4660,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="G6:G7"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="G17:G18"/>
     <mergeCell ref="H17:H18"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="D42:D43"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4741,48 +4741,48 @@
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="114" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="100" t="s">
+      <c r="D8" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="100" t="s">
+      <c r="E8" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="113" t="s">
+      <c r="F8" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="100" t="s">
+      <c r="I8" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="100" t="s">
+      <c r="J8" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="100" t="s">
+      <c r="K8" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="112"/>
+      <c r="L8" s="118"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="109"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="112"/>
+      <c r="C9" s="115"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="117"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="103"/>
+      <c r="K9" s="103"/>
+      <c r="L9" s="118"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
     </row>
@@ -4857,50 +4857,50 @@
       </c>
     </row>
     <row r="15" spans="3:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="100" t="s">
+      <c r="D15" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="100" t="s">
+      <c r="E15" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="F15" s="100" t="s">
+      <c r="F15" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="100" t="s">
+      <c r="G15" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="100" t="s">
+      <c r="H15" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="I15" s="104" t="s">
+      <c r="I15" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="J15" s="110" t="s">
+      <c r="J15" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="K15" s="112"/>
-      <c r="L15" s="112"/>
-      <c r="M15" s="112"/>
-      <c r="N15" s="112"/>
-      <c r="O15" s="112"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+      <c r="O15" s="118"/>
     </row>
     <row r="16" spans="3:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="109"/>
-      <c r="D16" s="101"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="111"/>
-      <c r="K16" s="112"/>
-      <c r="L16" s="112"/>
-      <c r="M16" s="112"/>
-      <c r="N16" s="112"/>
-      <c r="O16" s="112"/>
+      <c r="C16" s="115"/>
+      <c r="D16" s="103"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="103"/>
+      <c r="H16" s="103"/>
+      <c r="I16" s="106"/>
+      <c r="J16" s="120"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
+      <c r="O16" s="118"/>
     </row>
     <row r="17" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C17" s="45" t="s">
@@ -4984,76 +4984,76 @@
       </c>
     </row>
     <row r="22" spans="3:19" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="108" t="s">
+      <c r="D22" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="100" t="s">
+      <c r="E22" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="100" t="s">
+      <c r="F22" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="100" t="s">
+      <c r="G22" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="H22" s="100" t="s">
+      <c r="H22" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="100" t="s">
+      <c r="I22" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="J22" s="104" t="s">
+      <c r="J22" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="K22" s="110" t="s">
+      <c r="K22" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="L22" s="100" t="s">
+      <c r="L22" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="M22" s="100" t="s">
+      <c r="M22" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="N22" s="104" t="s">
+      <c r="N22" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="O22" s="104" t="s">
+      <c r="O22" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="P22" s="100" t="s">
+      <c r="P22" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="104" t="s">
+      <c r="Q22" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="R22" s="104" t="s">
+      <c r="R22" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="S22" s="100" t="s">
+      <c r="S22" s="102" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="101"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
-      <c r="J23" s="105"/>
-      <c r="K23" s="111"/>
-      <c r="L23" s="101"/>
-      <c r="M23" s="101"/>
-      <c r="N23" s="105"/>
-      <c r="O23" s="105"/>
-      <c r="P23" s="101"/>
-      <c r="Q23" s="105"/>
-      <c r="R23" s="105"/>
-      <c r="S23" s="101"/>
+      <c r="C23" s="103"/>
+      <c r="D23" s="115"/>
+      <c r="E23" s="103"/>
+      <c r="F23" s="103"/>
+      <c r="G23" s="103"/>
+      <c r="H23" s="103"/>
+      <c r="I23" s="103"/>
+      <c r="J23" s="106"/>
+      <c r="K23" s="120"/>
+      <c r="L23" s="103"/>
+      <c r="M23" s="103"/>
+      <c r="N23" s="106"/>
+      <c r="O23" s="106"/>
+      <c r="P23" s="103"/>
+      <c r="Q23" s="106"/>
+      <c r="R23" s="106"/>
+      <c r="S23" s="103"/>
     </row>
     <row r="24" spans="3:19" s="48" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C24" s="45" t="s">
@@ -5163,72 +5163,72 @@
       </c>
     </row>
     <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="C29" s="100" t="s">
+      <c r="C29" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="108" t="s">
+      <c r="D29" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="100" t="s">
+      <c r="E29" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="100" t="s">
+      <c r="F29" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="110" t="s">
+      <c r="G29" s="119" t="s">
         <v>16</v>
       </c>
-      <c r="H29" s="100" t="s">
+      <c r="H29" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="I29" s="100" t="s">
+      <c r="I29" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="J29" s="104" t="s">
+      <c r="J29" s="105" t="s">
         <v>22</v>
       </c>
-      <c r="K29" s="104" t="s">
+      <c r="K29" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="L29" s="100" t="s">
+      <c r="L29" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="M29" s="104" t="s">
+      <c r="M29" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="N29" s="104" t="s">
+      <c r="N29" s="105" t="s">
         <v>26</v>
       </c>
-      <c r="O29" s="100" t="s">
+      <c r="O29" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="P29" s="100" t="s">
+      <c r="P29" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="Q29" s="100" t="s">
+      <c r="Q29" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="R29" s="100" t="s">
+      <c r="R29" s="102" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="3:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="101"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="101"/>
-      <c r="G30" s="111"/>
-      <c r="H30" s="101"/>
-      <c r="I30" s="101"/>
-      <c r="J30" s="105"/>
-      <c r="K30" s="105"/>
-      <c r="L30" s="101"/>
-      <c r="M30" s="105"/>
-      <c r="N30" s="105"/>
-      <c r="O30" s="101"/>
-      <c r="P30" s="101"/>
-      <c r="Q30" s="101"/>
-      <c r="R30" s="101"/>
+      <c r="C30" s="103"/>
+      <c r="D30" s="115"/>
+      <c r="E30" s="103"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
+      <c r="J30" s="106"/>
+      <c r="K30" s="106"/>
+      <c r="L30" s="103"/>
+      <c r="M30" s="106"/>
+      <c r="N30" s="106"/>
+      <c r="O30" s="103"/>
+      <c r="P30" s="103"/>
+      <c r="Q30" s="103"/>
+      <c r="R30" s="103"/>
     </row>
     <row r="31" spans="3:19" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C31" s="45" t="s">
@@ -5331,13 +5331,13 @@
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="100" t="s">
+      <c r="C36" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="D36" s="100" t="s">
+      <c r="D36" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="E36" s="100" t="s">
+      <c r="E36" s="102" t="s">
         <v>34</v>
       </c>
       <c r="F36" s="12"/>
@@ -5348,9 +5348,9 @@
       <c r="K36" s="12"/>
     </row>
     <row r="37" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="101"/>
-      <c r="D37" s="101"/>
-      <c r="E37" s="101"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="103"/>
       <c r="F37" s="12"/>
       <c r="G37" s="12"/>
       <c r="H37" s="12"/>
@@ -5428,19 +5428,19 @@
       <c r="L43" s="4"/>
     </row>
     <row r="44" spans="3:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="100" t="s">
+      <c r="C44" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="D44" s="100" t="s">
+      <c r="D44" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="E44" s="100" t="s">
+      <c r="E44" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="104" t="s">
+      <c r="F44" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="G44" s="106" t="s">
+      <c r="G44" s="121" t="s">
         <v>7</v>
       </c>
       <c r="H44" s="4"/>
@@ -5450,11 +5450,11 @@
       <c r="L44" s="4"/>
     </row>
     <row r="45" spans="3:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="101"/>
-      <c r="D45" s="101"/>
-      <c r="E45" s="101"/>
-      <c r="F45" s="105"/>
-      <c r="G45" s="107"/>
+      <c r="C45" s="103"/>
+      <c r="D45" s="103"/>
+      <c r="E45" s="103"/>
+      <c r="F45" s="106"/>
+      <c r="G45" s="122"/>
       <c r="H45" s="4"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
@@ -5499,28 +5499,28 @@
       </c>
     </row>
     <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C52" s="100" t="s">
+      <c r="C52" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="D52" s="100" t="s">
+      <c r="D52" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="E52" s="100" t="s">
+      <c r="E52" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="F52" s="100" t="s">
+      <c r="F52" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="G52" s="100" t="s">
+      <c r="G52" s="102" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="53" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="101"/>
-      <c r="D53" s="101"/>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101"/>
-      <c r="G53" s="101"/>
+      <c r="C53" s="103"/>
+      <c r="D53" s="103"/>
+      <c r="E53" s="103"/>
+      <c r="F53" s="103"/>
+      <c r="G53" s="103"/>
     </row>
     <row r="54" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C54" s="2" t="s">
@@ -5558,30 +5558,30 @@
       </c>
     </row>
     <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="104" t="s">
+      <c r="C59" s="105" t="s">
         <v>38</v>
       </c>
-      <c r="D59" s="116"/>
-      <c r="E59" s="100" t="s">
+      <c r="D59" s="112"/>
+      <c r="E59" s="102" t="s">
         <v>69</v>
       </c>
-      <c r="F59" s="104" t="s">
+      <c r="F59" s="105" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="115"/>
+      <c r="G59" s="111"/>
     </row>
     <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C60" s="115"/>
-      <c r="D60" s="117"/>
-      <c r="E60" s="102"/>
-      <c r="F60" s="105"/>
-      <c r="G60" s="115"/>
+      <c r="C60" s="111"/>
+      <c r="D60" s="113"/>
+      <c r="E60" s="101"/>
+      <c r="F60" s="106"/>
+      <c r="G60" s="111"/>
     </row>
     <row r="61" spans="3:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="C61" s="119" t="s">
+      <c r="C61" s="107" t="s">
         <v>95</v>
       </c>
-      <c r="D61" s="120"/>
+      <c r="D61" s="108"/>
       <c r="E61" s="1" t="s">
         <v>96</v>
       </c>
@@ -5590,14 +5590,14 @@
       </c>
     </row>
     <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="121"/>
-      <c r="D62" s="122"/>
+      <c r="C62" s="109"/>
+      <c r="D62" s="110"/>
       <c r="E62" s="1"/>
       <c r="F62" s="2"/>
     </row>
     <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="118"/>
-      <c r="D63" s="118"/>
+      <c r="C63" s="104"/>
+      <c r="D63" s="104"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="4"/>
@@ -5608,82 +5608,30 @@
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C65" s="118" t="s">
+      <c r="C65" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="D65" s="118"/>
+      <c r="D65" s="104"/>
       <c r="E65" s="49">
         <v>0.2</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66" s="118" t="s">
+      <c r="C66" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="D66" s="118"/>
+      <c r="D66" s="104"/>
       <c r="E66" s="49">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="C59:D60"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="D52:D53"/>
-    <mergeCell ref="E52:E53"/>
-    <mergeCell ref="F52:F53"/>
-    <mergeCell ref="G52:G53"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="R22:R23"/>
-    <mergeCell ref="S22:S23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="N15:N16"/>
-    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G44:G45"/>
     <mergeCell ref="R29:R30"/>
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="D36:D37"/>
@@ -5700,11 +5648,63 @@
     <mergeCell ref="L29:L30"/>
     <mergeCell ref="C29:C30"/>
     <mergeCell ref="D29:D30"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="N15:N16"/>
+    <mergeCell ref="O15:O16"/>
+    <mergeCell ref="R22:R23"/>
+    <mergeCell ref="S22:S23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="G59:G60"/>
+    <mergeCell ref="C59:D60"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="D52:D53"/>
+    <mergeCell ref="E52:E53"/>
+    <mergeCell ref="F52:F53"/>
+    <mergeCell ref="G52:G53"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -5715,8 +5715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E120" sqref="E120"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5744,12 +5744,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
     </row>
     <row r="2" spans="1:10" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="72" t="s">
@@ -5914,46 +5914,46 @@
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="100" t="s">
+      <c r="A16" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="105" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="100" t="s">
+      <c r="C16" s="112"/>
+      <c r="D16" s="102" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="100" t="s">
+      <c r="E16" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="F16" s="100" t="s">
+      <c r="F16" s="102" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="100" t="s">
+      <c r="G16" s="102" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="100" t="s">
+      <c r="H16" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="125" t="s">
+      <c r="I16" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="100" t="s">
+      <c r="J16" s="102" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="101"/>
-      <c r="B17" s="105"/>
-      <c r="C17" s="124"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101"/>
-      <c r="I17" s="126"/>
-      <c r="J17" s="101"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="106"/>
+      <c r="C17" s="126"/>
+      <c r="D17" s="103"/>
+      <c r="E17" s="103"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="103"/>
+      <c r="H17" s="103"/>
+      <c r="I17" s="124"/>
+      <c r="J17" s="103"/>
     </row>
     <row r="18" spans="1:10" s="57" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A18" s="52">
@@ -5995,8 +5995,8 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="121"/>
-      <c r="C19" s="122"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="110"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -6314,40 +6314,40 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="108" t="s">
+      <c r="A51" s="114" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="100" t="s">
+      <c r="B51" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="100" t="s">
+      <c r="C51" s="102" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="100" t="s">
+      <c r="D51" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="100" t="s">
+      <c r="E51" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="F51" s="100" t="s">
+      <c r="F51" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="G51" s="104" t="s">
+      <c r="G51" s="105" t="s">
         <v>30</v>
       </c>
-      <c r="H51" s="110" t="s">
+      <c r="H51" s="119" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="109"/>
-      <c r="B52" s="101"/>
-      <c r="C52" s="101"/>
-      <c r="D52" s="101"/>
-      <c r="E52" s="101"/>
-      <c r="F52" s="101"/>
-      <c r="G52" s="105"/>
-      <c r="H52" s="111"/>
+      <c r="A52" s="115"/>
+      <c r="B52" s="103"/>
+      <c r="C52" s="103"/>
+      <c r="D52" s="103"/>
+      <c r="E52" s="103"/>
+      <c r="F52" s="103"/>
+      <c r="G52" s="106"/>
+      <c r="H52" s="120"/>
     </row>
     <row r="53" spans="1:10" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A53" s="82" t="s">
@@ -8036,17 +8036,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
     <mergeCell ref="F51:F52"/>
     <mergeCell ref="G51:G52"/>
     <mergeCell ref="H51:H52"/>
@@ -8055,6 +8044,17 @@
     <mergeCell ref="C51:C52"/>
     <mergeCell ref="D51:D52"/>
     <mergeCell ref="E51:E52"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F16:F17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -8066,7 +8066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
@@ -8084,12 +8084,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="123" t="s">
+      <c r="A1" s="125" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="123"/>
-      <c r="C1" s="123"/>
-      <c r="D1" s="123"/>
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
     </row>
     <row r="22" spans="10:18" x14ac:dyDescent="0.25">
       <c r="K22" s="5"/>

</xml_diff>